<commit_message>
Fully working excel import
</commit_message>
<xml_diff>
--- a/ExcelDataImport/ranking_data.xlsx
+++ b/ExcelDataImport/ranking_data.xlsx
@@ -3,13 +3,8 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="19001"/>
   <workbookPr defaultThemeVersion="124226"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jarno\Dropbox\Ohjelmointi\HaurRanking\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="119" yWindow="16" windowWidth="19036" windowHeight="12018" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16172" windowHeight="3655" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Production" sheetId="1" r:id="rId1"/>
@@ -18,7 +13,8 @@
     <sheet name="Classic" sheetId="10" r:id="rId4"/>
     <sheet name="Open" sheetId="12" r:id="rId5"/>
   </sheets>
-  <calcPr calcId="171027"/>
+  <calcPr calcId="0"/>
+  <oleSize ref="Q1:AE10"/>
 </workbook>
 </file>
 
@@ -326,13 +322,22 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="0.0000"/>
+  </numFmts>
+  <fonts count="2">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Arial Unicode MS"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -355,8 +360,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normaali" xfId="0" builtinId="0"/>
@@ -695,19 +702,23 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AE62"/>
+  <dimension ref="A1:BP62"/>
   <sheetViews>
     <sheetView topLeftCell="R1" workbookViewId="0">
       <selection activeCell="AF1" sqref="AF1:BP1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.65" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="14.65"/>
   <cols>
     <col min="1" max="1" width="18.28515625" customWidth="1"/>
     <col min="2" max="31" width="9.140625" customWidth="1"/>
+    <col min="33" max="33" width="18.28515625" customWidth="1"/>
+    <col min="34" max="34" width="4.42578125" customWidth="1"/>
+    <col min="35" max="35" width="3.28515625" customWidth="1"/>
+    <col min="36" max="36" width="4" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:31" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:68">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -802,7 +813,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="2" spans="1:31" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:68">
       <c r="A2" t="s">
         <v>82</v>
       </c>
@@ -896,8 +907,40 @@
       <c r="AE2">
         <v>-1</v>
       </c>
+      <c r="AF2" s="1"/>
+      <c r="AK2" s="2"/>
+      <c r="AL2" s="2"/>
+      <c r="AM2" s="2"/>
+      <c r="AN2" s="2"/>
+      <c r="AO2" s="2"/>
+      <c r="AP2" s="2"/>
+      <c r="AQ2" s="2"/>
+      <c r="AR2" s="2"/>
+      <c r="AS2" s="2"/>
+      <c r="AT2" s="2"/>
+      <c r="AU2" s="2"/>
+      <c r="AV2" s="2"/>
+      <c r="AW2" s="2"/>
+      <c r="AX2" s="2"/>
+      <c r="AY2" s="2"/>
+      <c r="AZ2" s="2"/>
+      <c r="BA2" s="2"/>
+      <c r="BB2" s="2"/>
+      <c r="BC2" s="2"/>
+      <c r="BD2" s="2"/>
+      <c r="BE2" s="2"/>
+      <c r="BF2" s="2"/>
+      <c r="BG2" s="2"/>
+      <c r="BH2" s="2"/>
+      <c r="BI2" s="2"/>
+      <c r="BJ2" s="2"/>
+      <c r="BK2" s="2"/>
+      <c r="BL2" s="2"/>
+      <c r="BM2" s="2"/>
+      <c r="BN2" s="2"/>
+      <c r="BP2" s="2"/>
     </row>
-    <row r="3" spans="1:31" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:68">
       <c r="A3" t="s">
         <v>26</v>
       </c>
@@ -991,8 +1034,40 @@
       <c r="AE3">
         <v>4.3693999999999997</v>
       </c>
+      <c r="AF3" s="1"/>
+      <c r="AK3" s="2"/>
+      <c r="AL3" s="2"/>
+      <c r="AM3" s="2"/>
+      <c r="AN3" s="2"/>
+      <c r="AO3" s="2"/>
+      <c r="AP3" s="2"/>
+      <c r="AQ3" s="2"/>
+      <c r="AR3" s="2"/>
+      <c r="AS3" s="2"/>
+      <c r="AT3" s="2"/>
+      <c r="AU3" s="2"/>
+      <c r="AV3" s="2"/>
+      <c r="AW3" s="2"/>
+      <c r="AX3" s="2"/>
+      <c r="AY3" s="2"/>
+      <c r="AZ3" s="2"/>
+      <c r="BA3" s="2"/>
+      <c r="BB3" s="2"/>
+      <c r="BC3" s="2"/>
+      <c r="BD3" s="2"/>
+      <c r="BE3" s="2"/>
+      <c r="BF3" s="2"/>
+      <c r="BG3" s="2"/>
+      <c r="BH3" s="2"/>
+      <c r="BI3" s="2"/>
+      <c r="BJ3" s="2"/>
+      <c r="BK3" s="2"/>
+      <c r="BL3" s="2"/>
+      <c r="BM3" s="2"/>
+      <c r="BN3" s="2"/>
+      <c r="BP3" s="2"/>
     </row>
-    <row r="4" spans="1:31" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:68">
       <c r="A4" t="s">
         <v>5</v>
       </c>
@@ -1086,8 +1161,40 @@
       <c r="AE4">
         <v>4.6889000000000003</v>
       </c>
+      <c r="AF4" s="1"/>
+      <c r="AK4" s="2"/>
+      <c r="AL4" s="2"/>
+      <c r="AM4" s="2"/>
+      <c r="AN4" s="2"/>
+      <c r="AO4" s="2"/>
+      <c r="AP4" s="2"/>
+      <c r="AQ4" s="2"/>
+      <c r="AR4" s="2"/>
+      <c r="AS4" s="2"/>
+      <c r="AT4" s="2"/>
+      <c r="AU4" s="2"/>
+      <c r="AV4" s="2"/>
+      <c r="AW4" s="2"/>
+      <c r="AX4" s="2"/>
+      <c r="AY4" s="2"/>
+      <c r="AZ4" s="2"/>
+      <c r="BA4" s="2"/>
+      <c r="BB4" s="2"/>
+      <c r="BC4" s="2"/>
+      <c r="BD4" s="2"/>
+      <c r="BE4" s="2"/>
+      <c r="BF4" s="2"/>
+      <c r="BG4" s="2"/>
+      <c r="BH4" s="2"/>
+      <c r="BI4" s="2"/>
+      <c r="BJ4" s="2"/>
+      <c r="BK4" s="2"/>
+      <c r="BL4" s="2"/>
+      <c r="BM4" s="2"/>
+      <c r="BN4" s="2"/>
+      <c r="BP4" s="2"/>
     </row>
-    <row r="5" spans="1:31" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:68">
       <c r="A5" t="s">
         <v>58</v>
       </c>
@@ -1181,8 +1288,40 @@
       <c r="AE5">
         <v>4.2220000000000004</v>
       </c>
+      <c r="AF5" s="1"/>
+      <c r="AK5" s="2"/>
+      <c r="AL5" s="2"/>
+      <c r="AM5" s="2"/>
+      <c r="AN5" s="2"/>
+      <c r="AO5" s="2"/>
+      <c r="AP5" s="2"/>
+      <c r="AQ5" s="2"/>
+      <c r="AR5" s="2"/>
+      <c r="AS5" s="2"/>
+      <c r="AT5" s="2"/>
+      <c r="AU5" s="2"/>
+      <c r="AV5" s="2"/>
+      <c r="AW5" s="2"/>
+      <c r="AX5" s="2"/>
+      <c r="AY5" s="2"/>
+      <c r="AZ5" s="2"/>
+      <c r="BA5" s="2"/>
+      <c r="BB5" s="2"/>
+      <c r="BC5" s="2"/>
+      <c r="BD5" s="2"/>
+      <c r="BE5" s="2"/>
+      <c r="BF5" s="2"/>
+      <c r="BG5" s="2"/>
+      <c r="BH5" s="2"/>
+      <c r="BI5" s="2"/>
+      <c r="BJ5" s="2"/>
+      <c r="BK5" s="2"/>
+      <c r="BL5" s="2"/>
+      <c r="BM5" s="2"/>
+      <c r="BN5" s="2"/>
+      <c r="BP5" s="2"/>
     </row>
-    <row r="6" spans="1:31" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:68">
       <c r="A6" t="s">
         <v>91</v>
       </c>
@@ -1276,8 +1415,40 @@
       <c r="AE6">
         <v>-1</v>
       </c>
+      <c r="AF6" s="1"/>
+      <c r="AK6" s="2"/>
+      <c r="AL6" s="2"/>
+      <c r="AM6" s="2"/>
+      <c r="AN6" s="2"/>
+      <c r="AO6" s="2"/>
+      <c r="AP6" s="2"/>
+      <c r="AQ6" s="2"/>
+      <c r="AR6" s="2"/>
+      <c r="AS6" s="2"/>
+      <c r="AT6" s="2"/>
+      <c r="AU6" s="2"/>
+      <c r="AV6" s="2"/>
+      <c r="AW6" s="2"/>
+      <c r="AX6" s="2"/>
+      <c r="AY6" s="2"/>
+      <c r="AZ6" s="2"/>
+      <c r="BA6" s="2"/>
+      <c r="BB6" s="2"/>
+      <c r="BC6" s="2"/>
+      <c r="BD6" s="2"/>
+      <c r="BE6" s="2"/>
+      <c r="BF6" s="2"/>
+      <c r="BG6" s="2"/>
+      <c r="BH6" s="2"/>
+      <c r="BI6" s="2"/>
+      <c r="BJ6" s="2"/>
+      <c r="BK6" s="2"/>
+      <c r="BL6" s="2"/>
+      <c r="BM6" s="2"/>
+      <c r="BN6" s="2"/>
+      <c r="BP6" s="2"/>
     </row>
-    <row r="7" spans="1:31" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:68">
       <c r="A7" t="s">
         <v>87</v>
       </c>
@@ -1371,8 +1542,40 @@
       <c r="AE7">
         <v>3.7410000000000001</v>
       </c>
+      <c r="AF7" s="1"/>
+      <c r="AK7" s="2"/>
+      <c r="AL7" s="2"/>
+      <c r="AM7" s="2"/>
+      <c r="AN7" s="2"/>
+      <c r="AO7" s="2"/>
+      <c r="AP7" s="2"/>
+      <c r="AQ7" s="2"/>
+      <c r="AR7" s="2"/>
+      <c r="AS7" s="2"/>
+      <c r="AT7" s="2"/>
+      <c r="AU7" s="2"/>
+      <c r="AV7" s="2"/>
+      <c r="AW7" s="2"/>
+      <c r="AX7" s="2"/>
+      <c r="AY7" s="2"/>
+      <c r="AZ7" s="2"/>
+      <c r="BA7" s="2"/>
+      <c r="BB7" s="2"/>
+      <c r="BC7" s="2"/>
+      <c r="BD7" s="2"/>
+      <c r="BE7" s="2"/>
+      <c r="BF7" s="2"/>
+      <c r="BG7" s="2"/>
+      <c r="BH7" s="2"/>
+      <c r="BI7" s="2"/>
+      <c r="BJ7" s="2"/>
+      <c r="BK7" s="2"/>
+      <c r="BL7" s="2"/>
+      <c r="BM7" s="2"/>
+      <c r="BN7" s="2"/>
+      <c r="BP7" s="2"/>
     </row>
-    <row r="8" spans="1:31" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:68">
       <c r="A8" t="s">
         <v>59</v>
       </c>
@@ -1466,8 +1669,40 @@
       <c r="AE8">
         <v>-1</v>
       </c>
+      <c r="AF8" s="1"/>
+      <c r="AK8" s="2"/>
+      <c r="AL8" s="2"/>
+      <c r="AM8" s="2"/>
+      <c r="AN8" s="2"/>
+      <c r="AO8" s="2"/>
+      <c r="AP8" s="2"/>
+      <c r="AQ8" s="2"/>
+      <c r="AR8" s="2"/>
+      <c r="AS8" s="2"/>
+      <c r="AT8" s="2"/>
+      <c r="AU8" s="2"/>
+      <c r="AV8" s="2"/>
+      <c r="AW8" s="2"/>
+      <c r="AX8" s="2"/>
+      <c r="AY8" s="2"/>
+      <c r="AZ8" s="2"/>
+      <c r="BA8" s="2"/>
+      <c r="BB8" s="2"/>
+      <c r="BC8" s="2"/>
+      <c r="BD8" s="2"/>
+      <c r="BE8" s="2"/>
+      <c r="BF8" s="2"/>
+      <c r="BG8" s="2"/>
+      <c r="BH8" s="2"/>
+      <c r="BI8" s="2"/>
+      <c r="BJ8" s="2"/>
+      <c r="BK8" s="2"/>
+      <c r="BL8" s="2"/>
+      <c r="BM8" s="2"/>
+      <c r="BN8" s="2"/>
+      <c r="BP8" s="2"/>
     </row>
-    <row r="9" spans="1:31" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:68">
       <c r="A9" t="s">
         <v>27</v>
       </c>
@@ -1561,8 +1796,40 @@
       <c r="AE9">
         <v>-1</v>
       </c>
+      <c r="AF9" s="1"/>
+      <c r="AK9" s="2"/>
+      <c r="AL9" s="2"/>
+      <c r="AM9" s="2"/>
+      <c r="AN9" s="2"/>
+      <c r="AO9" s="2"/>
+      <c r="AP9" s="2"/>
+      <c r="AQ9" s="2"/>
+      <c r="AR9" s="2"/>
+      <c r="AS9" s="2"/>
+      <c r="AT9" s="2"/>
+      <c r="AU9" s="2"/>
+      <c r="AV9" s="2"/>
+      <c r="AW9" s="2"/>
+      <c r="AX9" s="2"/>
+      <c r="AY9" s="2"/>
+      <c r="AZ9" s="2"/>
+      <c r="BA9" s="2"/>
+      <c r="BB9" s="2"/>
+      <c r="BC9" s="2"/>
+      <c r="BD9" s="2"/>
+      <c r="BE9" s="2"/>
+      <c r="BF9" s="2"/>
+      <c r="BG9" s="2"/>
+      <c r="BH9" s="2"/>
+      <c r="BI9" s="2"/>
+      <c r="BJ9" s="2"/>
+      <c r="BK9" s="2"/>
+      <c r="BL9" s="2"/>
+      <c r="BM9" s="2"/>
+      <c r="BN9" s="2"/>
+      <c r="BP9" s="2"/>
     </row>
-    <row r="10" spans="1:31" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:68">
       <c r="A10" t="s">
         <v>63</v>
       </c>
@@ -1656,8 +1923,40 @@
       <c r="AE10">
         <v>6.8044000000000002</v>
       </c>
+      <c r="AF10" s="1"/>
+      <c r="AK10" s="2"/>
+      <c r="AL10" s="2"/>
+      <c r="AM10" s="2"/>
+      <c r="AN10" s="2"/>
+      <c r="AO10" s="2"/>
+      <c r="AP10" s="2"/>
+      <c r="AQ10" s="2"/>
+      <c r="AR10" s="2"/>
+      <c r="AS10" s="2"/>
+      <c r="AT10" s="2"/>
+      <c r="AU10" s="2"/>
+      <c r="AV10" s="2"/>
+      <c r="AW10" s="2"/>
+      <c r="AX10" s="2"/>
+      <c r="AY10" s="2"/>
+      <c r="AZ10" s="2"/>
+      <c r="BA10" s="2"/>
+      <c r="BB10" s="2"/>
+      <c r="BC10" s="2"/>
+      <c r="BD10" s="2"/>
+      <c r="BE10" s="2"/>
+      <c r="BF10" s="2"/>
+      <c r="BG10" s="2"/>
+      <c r="BH10" s="2"/>
+      <c r="BI10" s="2"/>
+      <c r="BJ10" s="2"/>
+      <c r="BK10" s="2"/>
+      <c r="BL10" s="2"/>
+      <c r="BM10" s="2"/>
+      <c r="BN10" s="2"/>
+      <c r="BP10" s="2"/>
     </row>
-    <row r="11" spans="1:31" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:68">
       <c r="A11" t="s">
         <v>36</v>
       </c>
@@ -1751,8 +2050,40 @@
       <c r="AE11">
         <v>5.1546000000000003</v>
       </c>
+      <c r="AF11" s="1"/>
+      <c r="AK11" s="2"/>
+      <c r="AL11" s="2"/>
+      <c r="AM11" s="2"/>
+      <c r="AN11" s="2"/>
+      <c r="AO11" s="2"/>
+      <c r="AP11" s="2"/>
+      <c r="AQ11" s="2"/>
+      <c r="AR11" s="2"/>
+      <c r="AS11" s="2"/>
+      <c r="AT11" s="2"/>
+      <c r="AU11" s="2"/>
+      <c r="AV11" s="2"/>
+      <c r="AW11" s="2"/>
+      <c r="AX11" s="2"/>
+      <c r="AY11" s="2"/>
+      <c r="AZ11" s="2"/>
+      <c r="BA11" s="2"/>
+      <c r="BB11" s="2"/>
+      <c r="BC11" s="2"/>
+      <c r="BD11" s="2"/>
+      <c r="BE11" s="2"/>
+      <c r="BF11" s="2"/>
+      <c r="BG11" s="2"/>
+      <c r="BH11" s="2"/>
+      <c r="BI11" s="2"/>
+      <c r="BJ11" s="2"/>
+      <c r="BK11" s="2"/>
+      <c r="BL11" s="2"/>
+      <c r="BM11" s="2"/>
+      <c r="BN11" s="2"/>
+      <c r="BP11" s="2"/>
     </row>
-    <row r="12" spans="1:31" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:68">
       <c r="A12" t="s">
         <v>48</v>
       </c>
@@ -1846,8 +2177,40 @@
       <c r="AE12">
         <v>4.0728999999999997</v>
       </c>
+      <c r="AF12" s="1"/>
+      <c r="AK12" s="2"/>
+      <c r="AL12" s="2"/>
+      <c r="AM12" s="2"/>
+      <c r="AN12" s="2"/>
+      <c r="AO12" s="2"/>
+      <c r="AP12" s="2"/>
+      <c r="AQ12" s="2"/>
+      <c r="AR12" s="2"/>
+      <c r="AS12" s="2"/>
+      <c r="AT12" s="2"/>
+      <c r="AU12" s="2"/>
+      <c r="AV12" s="2"/>
+      <c r="AW12" s="2"/>
+      <c r="AX12" s="2"/>
+      <c r="AY12" s="2"/>
+      <c r="AZ12" s="2"/>
+      <c r="BA12" s="2"/>
+      <c r="BB12" s="2"/>
+      <c r="BC12" s="2"/>
+      <c r="BD12" s="2"/>
+      <c r="BE12" s="2"/>
+      <c r="BF12" s="2"/>
+      <c r="BG12" s="2"/>
+      <c r="BH12" s="2"/>
+      <c r="BI12" s="2"/>
+      <c r="BJ12" s="2"/>
+      <c r="BK12" s="2"/>
+      <c r="BL12" s="2"/>
+      <c r="BM12" s="2"/>
+      <c r="BN12" s="2"/>
+      <c r="BP12" s="2"/>
     </row>
-    <row r="13" spans="1:31" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:68">
       <c r="A13" t="s">
         <v>18</v>
       </c>
@@ -1941,8 +2304,40 @@
       <c r="AE13">
         <v>0</v>
       </c>
+      <c r="AF13" s="1"/>
+      <c r="AK13" s="2"/>
+      <c r="AL13" s="2"/>
+      <c r="AM13" s="2"/>
+      <c r="AN13" s="2"/>
+      <c r="AO13" s="2"/>
+      <c r="AP13" s="2"/>
+      <c r="AQ13" s="2"/>
+      <c r="AR13" s="2"/>
+      <c r="AS13" s="2"/>
+      <c r="AT13" s="2"/>
+      <c r="AU13" s="2"/>
+      <c r="AV13" s="2"/>
+      <c r="AW13" s="2"/>
+      <c r="AX13" s="2"/>
+      <c r="AY13" s="2"/>
+      <c r="AZ13" s="2"/>
+      <c r="BA13" s="2"/>
+      <c r="BB13" s="2"/>
+      <c r="BC13" s="2"/>
+      <c r="BD13" s="2"/>
+      <c r="BE13" s="2"/>
+      <c r="BF13" s="2"/>
+      <c r="BG13" s="2"/>
+      <c r="BH13" s="2"/>
+      <c r="BI13" s="2"/>
+      <c r="BJ13" s="2"/>
+      <c r="BK13" s="2"/>
+      <c r="BL13" s="2"/>
+      <c r="BM13" s="2"/>
+      <c r="BN13" s="2"/>
+      <c r="BP13" s="2"/>
     </row>
-    <row r="14" spans="1:31" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:68">
       <c r="A14" t="s">
         <v>3</v>
       </c>
@@ -2036,8 +2431,40 @@
       <c r="AE14">
         <v>4.5494000000000003</v>
       </c>
+      <c r="AF14" s="1"/>
+      <c r="AK14" s="2"/>
+      <c r="AL14" s="2"/>
+      <c r="AM14" s="2"/>
+      <c r="AN14" s="2"/>
+      <c r="AO14" s="2"/>
+      <c r="AP14" s="2"/>
+      <c r="AQ14" s="2"/>
+      <c r="AR14" s="2"/>
+      <c r="AS14" s="2"/>
+      <c r="AT14" s="2"/>
+      <c r="AU14" s="2"/>
+      <c r="AV14" s="2"/>
+      <c r="AW14" s="2"/>
+      <c r="AX14" s="2"/>
+      <c r="AY14" s="2"/>
+      <c r="AZ14" s="2"/>
+      <c r="BA14" s="2"/>
+      <c r="BB14" s="2"/>
+      <c r="BC14" s="2"/>
+      <c r="BD14" s="2"/>
+      <c r="BE14" s="2"/>
+      <c r="BF14" s="2"/>
+      <c r="BG14" s="2"/>
+      <c r="BH14" s="2"/>
+      <c r="BI14" s="2"/>
+      <c r="BJ14" s="2"/>
+      <c r="BK14" s="2"/>
+      <c r="BL14" s="2"/>
+      <c r="BM14" s="2"/>
+      <c r="BN14" s="2"/>
+      <c r="BP14" s="2"/>
     </row>
-    <row r="15" spans="1:31" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:68">
       <c r="A15" t="s">
         <v>14</v>
       </c>
@@ -2131,8 +2558,40 @@
       <c r="AE15">
         <v>-1</v>
       </c>
+      <c r="AF15" s="1"/>
+      <c r="AK15" s="2"/>
+      <c r="AL15" s="2"/>
+      <c r="AM15" s="2"/>
+      <c r="AN15" s="2"/>
+      <c r="AO15" s="2"/>
+      <c r="AP15" s="2"/>
+      <c r="AQ15" s="2"/>
+      <c r="AR15" s="2"/>
+      <c r="AS15" s="2"/>
+      <c r="AT15" s="2"/>
+      <c r="AU15" s="2"/>
+      <c r="AV15" s="2"/>
+      <c r="AW15" s="2"/>
+      <c r="AX15" s="2"/>
+      <c r="AY15" s="2"/>
+      <c r="AZ15" s="2"/>
+      <c r="BA15" s="2"/>
+      <c r="BB15" s="2"/>
+      <c r="BC15" s="2"/>
+      <c r="BD15" s="2"/>
+      <c r="BE15" s="2"/>
+      <c r="BF15" s="2"/>
+      <c r="BG15" s="2"/>
+      <c r="BH15" s="2"/>
+      <c r="BI15" s="2"/>
+      <c r="BJ15" s="2"/>
+      <c r="BK15" s="2"/>
+      <c r="BL15" s="2"/>
+      <c r="BM15" s="2"/>
+      <c r="BN15" s="2"/>
+      <c r="BP15" s="2"/>
     </row>
-    <row r="16" spans="1:31" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:68">
       <c r="A16" t="s">
         <v>47</v>
       </c>
@@ -2226,8 +2685,40 @@
       <c r="AE16">
         <v>-1</v>
       </c>
+      <c r="AF16" s="1"/>
+      <c r="AK16" s="2"/>
+      <c r="AL16" s="2"/>
+      <c r="AM16" s="2"/>
+      <c r="AN16" s="2"/>
+      <c r="AO16" s="2"/>
+      <c r="AP16" s="2"/>
+      <c r="AQ16" s="2"/>
+      <c r="AR16" s="2"/>
+      <c r="AS16" s="2"/>
+      <c r="AT16" s="2"/>
+      <c r="AU16" s="2"/>
+      <c r="AV16" s="2"/>
+      <c r="AW16" s="2"/>
+      <c r="AX16" s="2"/>
+      <c r="AY16" s="2"/>
+      <c r="AZ16" s="2"/>
+      <c r="BA16" s="2"/>
+      <c r="BB16" s="2"/>
+      <c r="BC16" s="2"/>
+      <c r="BD16" s="2"/>
+      <c r="BE16" s="2"/>
+      <c r="BF16" s="2"/>
+      <c r="BG16" s="2"/>
+      <c r="BH16" s="2"/>
+      <c r="BI16" s="2"/>
+      <c r="BJ16" s="2"/>
+      <c r="BK16" s="2"/>
+      <c r="BL16" s="2"/>
+      <c r="BM16" s="2"/>
+      <c r="BN16" s="2"/>
+      <c r="BP16" s="2"/>
     </row>
-    <row r="17" spans="1:31" x14ac:dyDescent="0.45">
+    <row r="17" spans="1:68">
       <c r="A17" t="s">
         <v>4</v>
       </c>
@@ -2321,8 +2812,40 @@
       <c r="AE17">
         <v>5.1177000000000001</v>
       </c>
+      <c r="AF17" s="1"/>
+      <c r="AK17" s="2"/>
+      <c r="AL17" s="2"/>
+      <c r="AM17" s="2"/>
+      <c r="AN17" s="2"/>
+      <c r="AO17" s="2"/>
+      <c r="AP17" s="2"/>
+      <c r="AQ17" s="2"/>
+      <c r="AR17" s="2"/>
+      <c r="AS17" s="2"/>
+      <c r="AT17" s="2"/>
+      <c r="AU17" s="2"/>
+      <c r="AV17" s="2"/>
+      <c r="AW17" s="2"/>
+      <c r="AX17" s="2"/>
+      <c r="AY17" s="2"/>
+      <c r="AZ17" s="2"/>
+      <c r="BA17" s="2"/>
+      <c r="BB17" s="2"/>
+      <c r="BC17" s="2"/>
+      <c r="BD17" s="2"/>
+      <c r="BE17" s="2"/>
+      <c r="BF17" s="2"/>
+      <c r="BG17" s="2"/>
+      <c r="BH17" s="2"/>
+      <c r="BI17" s="2"/>
+      <c r="BJ17" s="2"/>
+      <c r="BK17" s="2"/>
+      <c r="BL17" s="2"/>
+      <c r="BM17" s="2"/>
+      <c r="BN17" s="2"/>
+      <c r="BP17" s="2"/>
     </row>
-    <row r="18" spans="1:31" x14ac:dyDescent="0.45">
+    <row r="18" spans="1:68">
       <c r="A18" t="s">
         <v>10</v>
       </c>
@@ -2416,8 +2939,40 @@
       <c r="AE18">
         <v>2.0846</v>
       </c>
+      <c r="AF18" s="1"/>
+      <c r="AK18" s="2"/>
+      <c r="AL18" s="2"/>
+      <c r="AM18" s="2"/>
+      <c r="AN18" s="2"/>
+      <c r="AO18" s="2"/>
+      <c r="AP18" s="2"/>
+      <c r="AQ18" s="2"/>
+      <c r="AR18" s="2"/>
+      <c r="AS18" s="2"/>
+      <c r="AT18" s="2"/>
+      <c r="AU18" s="2"/>
+      <c r="AV18" s="2"/>
+      <c r="AW18" s="2"/>
+      <c r="AX18" s="2"/>
+      <c r="AY18" s="2"/>
+      <c r="AZ18" s="2"/>
+      <c r="BA18" s="2"/>
+      <c r="BB18" s="2"/>
+      <c r="BC18" s="2"/>
+      <c r="BD18" s="2"/>
+      <c r="BE18" s="2"/>
+      <c r="BF18" s="2"/>
+      <c r="BG18" s="2"/>
+      <c r="BH18" s="2"/>
+      <c r="BI18" s="2"/>
+      <c r="BJ18" s="2"/>
+      <c r="BK18" s="2"/>
+      <c r="BL18" s="2"/>
+      <c r="BM18" s="2"/>
+      <c r="BN18" s="2"/>
+      <c r="BP18" s="2"/>
     </row>
-    <row r="19" spans="1:31" x14ac:dyDescent="0.45">
+    <row r="19" spans="1:68">
       <c r="A19" t="s">
         <v>9</v>
       </c>
@@ -2511,8 +3066,40 @@
       <c r="AE19">
         <v>2.6187999999999998</v>
       </c>
+      <c r="AF19" s="1"/>
+      <c r="AK19" s="2"/>
+      <c r="AL19" s="2"/>
+      <c r="AM19" s="2"/>
+      <c r="AN19" s="2"/>
+      <c r="AO19" s="2"/>
+      <c r="AP19" s="2"/>
+      <c r="AQ19" s="2"/>
+      <c r="AR19" s="2"/>
+      <c r="AS19" s="2"/>
+      <c r="AT19" s="2"/>
+      <c r="AU19" s="2"/>
+      <c r="AV19" s="2"/>
+      <c r="AW19" s="2"/>
+      <c r="AX19" s="2"/>
+      <c r="AY19" s="2"/>
+      <c r="AZ19" s="2"/>
+      <c r="BA19" s="2"/>
+      <c r="BB19" s="2"/>
+      <c r="BC19" s="2"/>
+      <c r="BD19" s="2"/>
+      <c r="BE19" s="2"/>
+      <c r="BF19" s="2"/>
+      <c r="BG19" s="2"/>
+      <c r="BH19" s="2"/>
+      <c r="BI19" s="2"/>
+      <c r="BJ19" s="2"/>
+      <c r="BK19" s="2"/>
+      <c r="BL19" s="2"/>
+      <c r="BM19" s="2"/>
+      <c r="BN19" s="2"/>
+      <c r="BP19" s="2"/>
     </row>
-    <row r="20" spans="1:31" x14ac:dyDescent="0.45">
+    <row r="20" spans="1:68">
       <c r="A20" t="s">
         <v>16</v>
       </c>
@@ -2606,8 +3193,40 @@
       <c r="AE20">
         <v>-1</v>
       </c>
+      <c r="AF20" s="1"/>
+      <c r="AK20" s="2"/>
+      <c r="AL20" s="2"/>
+      <c r="AM20" s="2"/>
+      <c r="AN20" s="2"/>
+      <c r="AO20" s="2"/>
+      <c r="AP20" s="2"/>
+      <c r="AQ20" s="2"/>
+      <c r="AR20" s="2"/>
+      <c r="AS20" s="2"/>
+      <c r="AT20" s="2"/>
+      <c r="AU20" s="2"/>
+      <c r="AV20" s="2"/>
+      <c r="AW20" s="2"/>
+      <c r="AX20" s="2"/>
+      <c r="AY20" s="2"/>
+      <c r="AZ20" s="2"/>
+      <c r="BA20" s="2"/>
+      <c r="BB20" s="2"/>
+      <c r="BC20" s="2"/>
+      <c r="BD20" s="2"/>
+      <c r="BE20" s="2"/>
+      <c r="BF20" s="2"/>
+      <c r="BG20" s="2"/>
+      <c r="BH20" s="2"/>
+      <c r="BI20" s="2"/>
+      <c r="BJ20" s="2"/>
+      <c r="BK20" s="2"/>
+      <c r="BL20" s="2"/>
+      <c r="BM20" s="2"/>
+      <c r="BN20" s="2"/>
+      <c r="BP20" s="2"/>
     </row>
-    <row r="21" spans="1:31" x14ac:dyDescent="0.45">
+    <row r="21" spans="1:68">
       <c r="A21" t="s">
         <v>34</v>
       </c>
@@ -2701,8 +3320,40 @@
       <c r="AE21">
         <v>3.6817000000000002</v>
       </c>
+      <c r="AF21" s="1"/>
+      <c r="AK21" s="2"/>
+      <c r="AL21" s="2"/>
+      <c r="AM21" s="2"/>
+      <c r="AN21" s="2"/>
+      <c r="AO21" s="2"/>
+      <c r="AP21" s="2"/>
+      <c r="AQ21" s="2"/>
+      <c r="AR21" s="2"/>
+      <c r="AS21" s="2"/>
+      <c r="AT21" s="2"/>
+      <c r="AU21" s="2"/>
+      <c r="AV21" s="2"/>
+      <c r="AW21" s="2"/>
+      <c r="AX21" s="2"/>
+      <c r="AY21" s="2"/>
+      <c r="AZ21" s="2"/>
+      <c r="BA21" s="2"/>
+      <c r="BB21" s="2"/>
+      <c r="BC21" s="2"/>
+      <c r="BD21" s="2"/>
+      <c r="BE21" s="2"/>
+      <c r="BF21" s="2"/>
+      <c r="BG21" s="2"/>
+      <c r="BH21" s="2"/>
+      <c r="BI21" s="2"/>
+      <c r="BJ21" s="2"/>
+      <c r="BK21" s="2"/>
+      <c r="BL21" s="2"/>
+      <c r="BM21" s="2"/>
+      <c r="BN21" s="2"/>
+      <c r="BP21" s="2"/>
     </row>
-    <row r="22" spans="1:31" x14ac:dyDescent="0.45">
+    <row r="22" spans="1:68">
       <c r="A22" t="s">
         <v>44</v>
       </c>
@@ -2796,8 +3447,40 @@
       <c r="AE22">
         <v>4.5627000000000004</v>
       </c>
+      <c r="AF22" s="1"/>
+      <c r="AK22" s="2"/>
+      <c r="AL22" s="2"/>
+      <c r="AM22" s="2"/>
+      <c r="AN22" s="2"/>
+      <c r="AO22" s="2"/>
+      <c r="AP22" s="2"/>
+      <c r="AQ22" s="2"/>
+      <c r="AR22" s="2"/>
+      <c r="AS22" s="2"/>
+      <c r="AT22" s="2"/>
+      <c r="AU22" s="2"/>
+      <c r="AV22" s="2"/>
+      <c r="AW22" s="2"/>
+      <c r="AX22" s="2"/>
+      <c r="AY22" s="2"/>
+      <c r="AZ22" s="2"/>
+      <c r="BA22" s="2"/>
+      <c r="BB22" s="2"/>
+      <c r="BC22" s="2"/>
+      <c r="BD22" s="2"/>
+      <c r="BE22" s="2"/>
+      <c r="BF22" s="2"/>
+      <c r="BG22" s="2"/>
+      <c r="BH22" s="2"/>
+      <c r="BI22" s="2"/>
+      <c r="BJ22" s="2"/>
+      <c r="BK22" s="2"/>
+      <c r="BL22" s="2"/>
+      <c r="BM22" s="2"/>
+      <c r="BN22" s="2"/>
+      <c r="BP22" s="2"/>
     </row>
-    <row r="23" spans="1:31" x14ac:dyDescent="0.45">
+    <row r="23" spans="1:68">
       <c r="A23" t="s">
         <v>1</v>
       </c>
@@ -2891,8 +3574,40 @@
       <c r="AE23">
         <v>6.7668999999999997</v>
       </c>
+      <c r="AF23" s="1"/>
+      <c r="AK23" s="2"/>
+      <c r="AL23" s="2"/>
+      <c r="AM23" s="2"/>
+      <c r="AN23" s="2"/>
+      <c r="AO23" s="2"/>
+      <c r="AP23" s="2"/>
+      <c r="AQ23" s="2"/>
+      <c r="AR23" s="2"/>
+      <c r="AS23" s="2"/>
+      <c r="AT23" s="2"/>
+      <c r="AU23" s="2"/>
+      <c r="AV23" s="2"/>
+      <c r="AW23" s="2"/>
+      <c r="AX23" s="2"/>
+      <c r="AY23" s="2"/>
+      <c r="AZ23" s="2"/>
+      <c r="BA23" s="2"/>
+      <c r="BB23" s="2"/>
+      <c r="BC23" s="2"/>
+      <c r="BD23" s="2"/>
+      <c r="BE23" s="2"/>
+      <c r="BF23" s="2"/>
+      <c r="BG23" s="2"/>
+      <c r="BH23" s="2"/>
+      <c r="BI23" s="2"/>
+      <c r="BJ23" s="2"/>
+      <c r="BK23" s="2"/>
+      <c r="BL23" s="2"/>
+      <c r="BM23" s="2"/>
+      <c r="BN23" s="2"/>
+      <c r="BP23" s="2"/>
     </row>
-    <row r="24" spans="1:31" x14ac:dyDescent="0.45">
+    <row r="24" spans="1:68">
       <c r="A24" t="s">
         <v>51</v>
       </c>
@@ -2986,8 +3701,40 @@
       <c r="AE24">
         <v>4.3299000000000003</v>
       </c>
+      <c r="AF24" s="1"/>
+      <c r="AK24" s="2"/>
+      <c r="AL24" s="2"/>
+      <c r="AM24" s="2"/>
+      <c r="AN24" s="2"/>
+      <c r="AO24" s="2"/>
+      <c r="AP24" s="2"/>
+      <c r="AQ24" s="2"/>
+      <c r="AR24" s="2"/>
+      <c r="AS24" s="2"/>
+      <c r="AT24" s="2"/>
+      <c r="AU24" s="2"/>
+      <c r="AV24" s="2"/>
+      <c r="AW24" s="2"/>
+      <c r="AX24" s="2"/>
+      <c r="AY24" s="2"/>
+      <c r="AZ24" s="2"/>
+      <c r="BA24" s="2"/>
+      <c r="BB24" s="2"/>
+      <c r="BC24" s="2"/>
+      <c r="BD24" s="2"/>
+      <c r="BE24" s="2"/>
+      <c r="BF24" s="2"/>
+      <c r="BG24" s="2"/>
+      <c r="BH24" s="2"/>
+      <c r="BI24" s="2"/>
+      <c r="BJ24" s="2"/>
+      <c r="BK24" s="2"/>
+      <c r="BL24" s="2"/>
+      <c r="BM24" s="2"/>
+      <c r="BN24" s="2"/>
+      <c r="BP24" s="2"/>
     </row>
-    <row r="25" spans="1:31" x14ac:dyDescent="0.45">
+    <row r="25" spans="1:68">
       <c r="A25" t="s">
         <v>71</v>
       </c>
@@ -3081,8 +3828,40 @@
       <c r="AE25">
         <v>5.1773999999999996</v>
       </c>
+      <c r="AF25" s="1"/>
+      <c r="AK25" s="2"/>
+      <c r="AL25" s="2"/>
+      <c r="AM25" s="2"/>
+      <c r="AN25" s="2"/>
+      <c r="AO25" s="2"/>
+      <c r="AP25" s="2"/>
+      <c r="AQ25" s="2"/>
+      <c r="AR25" s="2"/>
+      <c r="AS25" s="2"/>
+      <c r="AT25" s="2"/>
+      <c r="AU25" s="2"/>
+      <c r="AV25" s="2"/>
+      <c r="AW25" s="2"/>
+      <c r="AX25" s="2"/>
+      <c r="AY25" s="2"/>
+      <c r="AZ25" s="2"/>
+      <c r="BA25" s="2"/>
+      <c r="BB25" s="2"/>
+      <c r="BC25" s="2"/>
+      <c r="BD25" s="2"/>
+      <c r="BE25" s="2"/>
+      <c r="BF25" s="2"/>
+      <c r="BG25" s="2"/>
+      <c r="BH25" s="2"/>
+      <c r="BI25" s="2"/>
+      <c r="BJ25" s="2"/>
+      <c r="BK25" s="2"/>
+      <c r="BL25" s="2"/>
+      <c r="BM25" s="2"/>
+      <c r="BN25" s="2"/>
+      <c r="BP25" s="2"/>
     </row>
-    <row r="26" spans="1:31" x14ac:dyDescent="0.45">
+    <row r="26" spans="1:68">
       <c r="A26" t="s">
         <v>29</v>
       </c>
@@ -3176,8 +3955,40 @@
       <c r="AE26">
         <v>-1</v>
       </c>
+      <c r="AF26" s="1"/>
+      <c r="AK26" s="2"/>
+      <c r="AL26" s="2"/>
+      <c r="AM26" s="2"/>
+      <c r="AN26" s="2"/>
+      <c r="AO26" s="2"/>
+      <c r="AP26" s="2"/>
+      <c r="AQ26" s="2"/>
+      <c r="AR26" s="2"/>
+      <c r="AS26" s="2"/>
+      <c r="AT26" s="2"/>
+      <c r="AU26" s="2"/>
+      <c r="AV26" s="2"/>
+      <c r="AW26" s="2"/>
+      <c r="AX26" s="2"/>
+      <c r="AY26" s="2"/>
+      <c r="AZ26" s="2"/>
+      <c r="BA26" s="2"/>
+      <c r="BB26" s="2"/>
+      <c r="BC26" s="2"/>
+      <c r="BD26" s="2"/>
+      <c r="BE26" s="2"/>
+      <c r="BF26" s="2"/>
+      <c r="BG26" s="2"/>
+      <c r="BH26" s="2"/>
+      <c r="BI26" s="2"/>
+      <c r="BJ26" s="2"/>
+      <c r="BK26" s="2"/>
+      <c r="BL26" s="2"/>
+      <c r="BM26" s="2"/>
+      <c r="BN26" s="2"/>
+      <c r="BP26" s="2"/>
     </row>
-    <row r="27" spans="1:31" x14ac:dyDescent="0.45">
+    <row r="27" spans="1:68">
       <c r="A27" t="s">
         <v>2</v>
       </c>
@@ -3271,8 +4082,40 @@
       <c r="AE27">
         <v>2.7189999999999999</v>
       </c>
+      <c r="AF27" s="1"/>
+      <c r="AK27" s="2"/>
+      <c r="AL27" s="2"/>
+      <c r="AM27" s="2"/>
+      <c r="AN27" s="2"/>
+      <c r="AO27" s="2"/>
+      <c r="AP27" s="2"/>
+      <c r="AQ27" s="2"/>
+      <c r="AR27" s="2"/>
+      <c r="AS27" s="2"/>
+      <c r="AT27" s="2"/>
+      <c r="AU27" s="2"/>
+      <c r="AV27" s="2"/>
+      <c r="AW27" s="2"/>
+      <c r="AX27" s="2"/>
+      <c r="AY27" s="2"/>
+      <c r="AZ27" s="2"/>
+      <c r="BA27" s="2"/>
+      <c r="BB27" s="2"/>
+      <c r="BC27" s="2"/>
+      <c r="BD27" s="2"/>
+      <c r="BE27" s="2"/>
+      <c r="BF27" s="2"/>
+      <c r="BG27" s="2"/>
+      <c r="BH27" s="2"/>
+      <c r="BI27" s="2"/>
+      <c r="BJ27" s="2"/>
+      <c r="BK27" s="2"/>
+      <c r="BL27" s="2"/>
+      <c r="BM27" s="2"/>
+      <c r="BN27" s="2"/>
+      <c r="BP27" s="2"/>
     </row>
-    <row r="28" spans="1:31" x14ac:dyDescent="0.45">
+    <row r="28" spans="1:68">
       <c r="A28" t="s">
         <v>25</v>
       </c>
@@ -3366,8 +4209,40 @@
       <c r="AE28">
         <v>-1</v>
       </c>
+      <c r="AF28" s="1"/>
+      <c r="AK28" s="2"/>
+      <c r="AL28" s="2"/>
+      <c r="AM28" s="2"/>
+      <c r="AN28" s="2"/>
+      <c r="AO28" s="2"/>
+      <c r="AP28" s="2"/>
+      <c r="AQ28" s="2"/>
+      <c r="AR28" s="2"/>
+      <c r="AS28" s="2"/>
+      <c r="AT28" s="2"/>
+      <c r="AU28" s="2"/>
+      <c r="AV28" s="2"/>
+      <c r="AW28" s="2"/>
+      <c r="AX28" s="2"/>
+      <c r="AY28" s="2"/>
+      <c r="AZ28" s="2"/>
+      <c r="BA28" s="2"/>
+      <c r="BB28" s="2"/>
+      <c r="BC28" s="2"/>
+      <c r="BD28" s="2"/>
+      <c r="BE28" s="2"/>
+      <c r="BF28" s="2"/>
+      <c r="BG28" s="2"/>
+      <c r="BH28" s="2"/>
+      <c r="BI28" s="2"/>
+      <c r="BJ28" s="2"/>
+      <c r="BK28" s="2"/>
+      <c r="BL28" s="2"/>
+      <c r="BM28" s="2"/>
+      <c r="BN28" s="2"/>
+      <c r="BP28" s="2"/>
     </row>
-    <row r="29" spans="1:31" x14ac:dyDescent="0.45">
+    <row r="29" spans="1:68">
       <c r="A29" t="s">
         <v>53</v>
       </c>
@@ -3461,8 +4336,40 @@
       <c r="AE29">
         <v>-1</v>
       </c>
+      <c r="AF29" s="1"/>
+      <c r="AK29" s="2"/>
+      <c r="AL29" s="2"/>
+      <c r="AM29" s="2"/>
+      <c r="AN29" s="2"/>
+      <c r="AO29" s="2"/>
+      <c r="AP29" s="2"/>
+      <c r="AQ29" s="2"/>
+      <c r="AR29" s="2"/>
+      <c r="AS29" s="2"/>
+      <c r="AT29" s="2"/>
+      <c r="AU29" s="2"/>
+      <c r="AV29" s="2"/>
+      <c r="AW29" s="2"/>
+      <c r="AX29" s="2"/>
+      <c r="AY29" s="2"/>
+      <c r="AZ29" s="2"/>
+      <c r="BA29" s="2"/>
+      <c r="BB29" s="2"/>
+      <c r="BC29" s="2"/>
+      <c r="BD29" s="2"/>
+      <c r="BE29" s="2"/>
+      <c r="BF29" s="2"/>
+      <c r="BG29" s="2"/>
+      <c r="BH29" s="2"/>
+      <c r="BI29" s="2"/>
+      <c r="BJ29" s="2"/>
+      <c r="BK29" s="2"/>
+      <c r="BL29" s="2"/>
+      <c r="BM29" s="2"/>
+      <c r="BN29" s="2"/>
+      <c r="BP29" s="2"/>
     </row>
-    <row r="30" spans="1:31" x14ac:dyDescent="0.45">
+    <row r="30" spans="1:68">
       <c r="A30" t="s">
         <v>54</v>
       </c>
@@ -3556,8 +4463,40 @@
       <c r="AE30">
         <v>-1</v>
       </c>
+      <c r="AF30" s="1"/>
+      <c r="AK30" s="2"/>
+      <c r="AL30" s="2"/>
+      <c r="AM30" s="2"/>
+      <c r="AN30" s="2"/>
+      <c r="AO30" s="2"/>
+      <c r="AP30" s="2"/>
+      <c r="AQ30" s="2"/>
+      <c r="AR30" s="2"/>
+      <c r="AS30" s="2"/>
+      <c r="AT30" s="2"/>
+      <c r="AU30" s="2"/>
+      <c r="AV30" s="2"/>
+      <c r="AW30" s="2"/>
+      <c r="AX30" s="2"/>
+      <c r="AY30" s="2"/>
+      <c r="AZ30" s="2"/>
+      <c r="BA30" s="2"/>
+      <c r="BB30" s="2"/>
+      <c r="BC30" s="2"/>
+      <c r="BD30" s="2"/>
+      <c r="BE30" s="2"/>
+      <c r="BF30" s="2"/>
+      <c r="BG30" s="2"/>
+      <c r="BH30" s="2"/>
+      <c r="BI30" s="2"/>
+      <c r="BJ30" s="2"/>
+      <c r="BK30" s="2"/>
+      <c r="BL30" s="2"/>
+      <c r="BM30" s="2"/>
+      <c r="BN30" s="2"/>
+      <c r="BP30" s="2"/>
     </row>
-    <row r="31" spans="1:31" x14ac:dyDescent="0.45">
+    <row r="31" spans="1:68">
       <c r="A31" t="s">
         <v>85</v>
       </c>
@@ -3651,8 +4590,40 @@
       <c r="AE31">
         <v>9.6600000000000005E-2</v>
       </c>
+      <c r="AF31" s="1"/>
+      <c r="AK31" s="2"/>
+      <c r="AL31" s="2"/>
+      <c r="AM31" s="2"/>
+      <c r="AN31" s="2"/>
+      <c r="AO31" s="2"/>
+      <c r="AP31" s="2"/>
+      <c r="AQ31" s="2"/>
+      <c r="AR31" s="2"/>
+      <c r="AS31" s="2"/>
+      <c r="AT31" s="2"/>
+      <c r="AU31" s="2"/>
+      <c r="AV31" s="2"/>
+      <c r="AW31" s="2"/>
+      <c r="AX31" s="2"/>
+      <c r="AY31" s="2"/>
+      <c r="AZ31" s="2"/>
+      <c r="BA31" s="2"/>
+      <c r="BB31" s="2"/>
+      <c r="BC31" s="2"/>
+      <c r="BD31" s="2"/>
+      <c r="BE31" s="2"/>
+      <c r="BF31" s="2"/>
+      <c r="BG31" s="2"/>
+      <c r="BH31" s="2"/>
+      <c r="BI31" s="2"/>
+      <c r="BJ31" s="2"/>
+      <c r="BK31" s="2"/>
+      <c r="BL31" s="2"/>
+      <c r="BM31" s="2"/>
+      <c r="BN31" s="2"/>
+      <c r="BP31" s="2"/>
     </row>
-    <row r="32" spans="1:31" x14ac:dyDescent="0.45">
+    <row r="32" spans="1:68">
       <c r="A32" t="s">
         <v>52</v>
       </c>
@@ -3746,8 +4717,40 @@
       <c r="AE32">
         <v>2.4443999999999999</v>
       </c>
+      <c r="AF32" s="1"/>
+      <c r="AK32" s="2"/>
+      <c r="AL32" s="2"/>
+      <c r="AM32" s="2"/>
+      <c r="AN32" s="2"/>
+      <c r="AO32" s="2"/>
+      <c r="AP32" s="2"/>
+      <c r="AQ32" s="2"/>
+      <c r="AR32" s="2"/>
+      <c r="AS32" s="2"/>
+      <c r="AT32" s="2"/>
+      <c r="AU32" s="2"/>
+      <c r="AV32" s="2"/>
+      <c r="AW32" s="2"/>
+      <c r="AX32" s="2"/>
+      <c r="AY32" s="2"/>
+      <c r="AZ32" s="2"/>
+      <c r="BA32" s="2"/>
+      <c r="BB32" s="2"/>
+      <c r="BC32" s="2"/>
+      <c r="BD32" s="2"/>
+      <c r="BE32" s="2"/>
+      <c r="BF32" s="2"/>
+      <c r="BG32" s="2"/>
+      <c r="BH32" s="2"/>
+      <c r="BI32" s="2"/>
+      <c r="BJ32" s="2"/>
+      <c r="BK32" s="2"/>
+      <c r="BL32" s="2"/>
+      <c r="BM32" s="2"/>
+      <c r="BN32" s="2"/>
+      <c r="BP32" s="2"/>
     </row>
-    <row r="33" spans="1:31" x14ac:dyDescent="0.45">
+    <row r="33" spans="1:68">
       <c r="A33" t="s">
         <v>95</v>
       </c>
@@ -3841,8 +4844,40 @@
       <c r="AE33">
         <v>-1</v>
       </c>
+      <c r="AF33" s="1"/>
+      <c r="AK33" s="2"/>
+      <c r="AL33" s="2"/>
+      <c r="AM33" s="2"/>
+      <c r="AN33" s="2"/>
+      <c r="AO33" s="2"/>
+      <c r="AP33" s="2"/>
+      <c r="AQ33" s="2"/>
+      <c r="AR33" s="2"/>
+      <c r="AS33" s="2"/>
+      <c r="AT33" s="2"/>
+      <c r="AU33" s="2"/>
+      <c r="AV33" s="2"/>
+      <c r="AW33" s="2"/>
+      <c r="AX33" s="2"/>
+      <c r="AY33" s="2"/>
+      <c r="AZ33" s="2"/>
+      <c r="BA33" s="2"/>
+      <c r="BB33" s="2"/>
+      <c r="BC33" s="2"/>
+      <c r="BD33" s="2"/>
+      <c r="BE33" s="2"/>
+      <c r="BF33" s="2"/>
+      <c r="BG33" s="2"/>
+      <c r="BH33" s="2"/>
+      <c r="BI33" s="2"/>
+      <c r="BJ33" s="2"/>
+      <c r="BK33" s="2"/>
+      <c r="BL33" s="2"/>
+      <c r="BM33" s="2"/>
+      <c r="BN33" s="2"/>
+      <c r="BP33" s="2"/>
     </row>
-    <row r="34" spans="1:31" x14ac:dyDescent="0.45">
+    <row r="34" spans="1:68">
       <c r="A34" t="s">
         <v>62</v>
       </c>
@@ -3936,8 +4971,40 @@
       <c r="AE34">
         <v>-1</v>
       </c>
+      <c r="AF34" s="1"/>
+      <c r="AK34" s="2"/>
+      <c r="AL34" s="2"/>
+      <c r="AM34" s="2"/>
+      <c r="AN34" s="2"/>
+      <c r="AO34" s="2"/>
+      <c r="AP34" s="2"/>
+      <c r="AQ34" s="2"/>
+      <c r="AR34" s="2"/>
+      <c r="AS34" s="2"/>
+      <c r="AT34" s="2"/>
+      <c r="AU34" s="2"/>
+      <c r="AV34" s="2"/>
+      <c r="AW34" s="2"/>
+      <c r="AX34" s="2"/>
+      <c r="AY34" s="2"/>
+      <c r="AZ34" s="2"/>
+      <c r="BA34" s="2"/>
+      <c r="BB34" s="2"/>
+      <c r="BC34" s="2"/>
+      <c r="BD34" s="2"/>
+      <c r="BE34" s="2"/>
+      <c r="BF34" s="2"/>
+      <c r="BG34" s="2"/>
+      <c r="BH34" s="2"/>
+      <c r="BI34" s="2"/>
+      <c r="BJ34" s="2"/>
+      <c r="BK34" s="2"/>
+      <c r="BL34" s="2"/>
+      <c r="BM34" s="2"/>
+      <c r="BN34" s="2"/>
+      <c r="BP34" s="2"/>
     </row>
-    <row r="35" spans="1:31" x14ac:dyDescent="0.45">
+    <row r="35" spans="1:68">
       <c r="A35" t="s">
         <v>12</v>
       </c>
@@ -4031,8 +5098,40 @@
       <c r="AE35">
         <v>4.5602999999999998</v>
       </c>
+      <c r="AF35" s="1"/>
+      <c r="AK35" s="2"/>
+      <c r="AL35" s="2"/>
+      <c r="AM35" s="2"/>
+      <c r="AN35" s="2"/>
+      <c r="AO35" s="2"/>
+      <c r="AP35" s="2"/>
+      <c r="AQ35" s="2"/>
+      <c r="AR35" s="2"/>
+      <c r="AS35" s="2"/>
+      <c r="AT35" s="2"/>
+      <c r="AU35" s="2"/>
+      <c r="AV35" s="2"/>
+      <c r="AW35" s="2"/>
+      <c r="AX35" s="2"/>
+      <c r="AY35" s="2"/>
+      <c r="AZ35" s="2"/>
+      <c r="BA35" s="2"/>
+      <c r="BB35" s="2"/>
+      <c r="BC35" s="2"/>
+      <c r="BD35" s="2"/>
+      <c r="BE35" s="2"/>
+      <c r="BF35" s="2"/>
+      <c r="BG35" s="2"/>
+      <c r="BH35" s="2"/>
+      <c r="BI35" s="2"/>
+      <c r="BJ35" s="2"/>
+      <c r="BK35" s="2"/>
+      <c r="BL35" s="2"/>
+      <c r="BM35" s="2"/>
+      <c r="BN35" s="2"/>
+      <c r="BP35" s="2"/>
     </row>
-    <row r="36" spans="1:31" x14ac:dyDescent="0.45">
+    <row r="36" spans="1:68">
       <c r="A36" t="s">
         <v>19</v>
       </c>
@@ -4126,8 +5225,40 @@
       <c r="AE36">
         <v>-1</v>
       </c>
+      <c r="AF36" s="1"/>
+      <c r="AK36" s="2"/>
+      <c r="AL36" s="2"/>
+      <c r="AM36" s="2"/>
+      <c r="AN36" s="2"/>
+      <c r="AO36" s="2"/>
+      <c r="AP36" s="2"/>
+      <c r="AQ36" s="2"/>
+      <c r="AR36" s="2"/>
+      <c r="AS36" s="2"/>
+      <c r="AT36" s="2"/>
+      <c r="AU36" s="2"/>
+      <c r="AV36" s="2"/>
+      <c r="AW36" s="2"/>
+      <c r="AX36" s="2"/>
+      <c r="AY36" s="2"/>
+      <c r="AZ36" s="2"/>
+      <c r="BA36" s="2"/>
+      <c r="BB36" s="2"/>
+      <c r="BC36" s="2"/>
+      <c r="BD36" s="2"/>
+      <c r="BE36" s="2"/>
+      <c r="BF36" s="2"/>
+      <c r="BG36" s="2"/>
+      <c r="BH36" s="2"/>
+      <c r="BI36" s="2"/>
+      <c r="BJ36" s="2"/>
+      <c r="BK36" s="2"/>
+      <c r="BL36" s="2"/>
+      <c r="BM36" s="2"/>
+      <c r="BN36" s="2"/>
+      <c r="BP36" s="2"/>
     </row>
-    <row r="37" spans="1:31" x14ac:dyDescent="0.45">
+    <row r="37" spans="1:68">
       <c r="A37" t="s">
         <v>96</v>
       </c>
@@ -4221,8 +5352,40 @@
       <c r="AE37">
         <v>4.3327999999999998</v>
       </c>
+      <c r="AF37" s="1"/>
+      <c r="AK37" s="2"/>
+      <c r="AL37" s="2"/>
+      <c r="AM37" s="2"/>
+      <c r="AN37" s="2"/>
+      <c r="AO37" s="2"/>
+      <c r="AP37" s="2"/>
+      <c r="AQ37" s="2"/>
+      <c r="AR37" s="2"/>
+      <c r="AS37" s="2"/>
+      <c r="AT37" s="2"/>
+      <c r="AU37" s="2"/>
+      <c r="AV37" s="2"/>
+      <c r="AW37" s="2"/>
+      <c r="AX37" s="2"/>
+      <c r="AY37" s="2"/>
+      <c r="AZ37" s="2"/>
+      <c r="BA37" s="2"/>
+      <c r="BB37" s="2"/>
+      <c r="BC37" s="2"/>
+      <c r="BD37" s="2"/>
+      <c r="BE37" s="2"/>
+      <c r="BF37" s="2"/>
+      <c r="BG37" s="2"/>
+      <c r="BH37" s="2"/>
+      <c r="BI37" s="2"/>
+      <c r="BJ37" s="2"/>
+      <c r="BK37" s="2"/>
+      <c r="BL37" s="2"/>
+      <c r="BM37" s="2"/>
+      <c r="BN37" s="2"/>
+      <c r="BP37" s="2"/>
     </row>
-    <row r="38" spans="1:31" x14ac:dyDescent="0.45">
+    <row r="38" spans="1:68">
       <c r="A38" t="s">
         <v>88</v>
       </c>
@@ -4316,8 +5479,40 @@
       <c r="AE38">
         <v>4.1749999999999998</v>
       </c>
+      <c r="AF38" s="1"/>
+      <c r="AK38" s="2"/>
+      <c r="AL38" s="2"/>
+      <c r="AM38" s="2"/>
+      <c r="AN38" s="2"/>
+      <c r="AO38" s="2"/>
+      <c r="AP38" s="2"/>
+      <c r="AQ38" s="2"/>
+      <c r="AR38" s="2"/>
+      <c r="AS38" s="2"/>
+      <c r="AT38" s="2"/>
+      <c r="AU38" s="2"/>
+      <c r="AV38" s="2"/>
+      <c r="AW38" s="2"/>
+      <c r="AX38" s="2"/>
+      <c r="AY38" s="2"/>
+      <c r="AZ38" s="2"/>
+      <c r="BA38" s="2"/>
+      <c r="BB38" s="2"/>
+      <c r="BC38" s="2"/>
+      <c r="BD38" s="2"/>
+      <c r="BE38" s="2"/>
+      <c r="BF38" s="2"/>
+      <c r="BG38" s="2"/>
+      <c r="BH38" s="2"/>
+      <c r="BI38" s="2"/>
+      <c r="BJ38" s="2"/>
+      <c r="BK38" s="2"/>
+      <c r="BL38" s="2"/>
+      <c r="BM38" s="2"/>
+      <c r="BN38" s="2"/>
+      <c r="BP38" s="2"/>
     </row>
-    <row r="39" spans="1:31" x14ac:dyDescent="0.45">
+    <row r="39" spans="1:68">
       <c r="A39" t="s">
         <v>84</v>
       </c>
@@ -4411,8 +5606,40 @@
       <c r="AE39">
         <v>-1</v>
       </c>
+      <c r="AF39" s="1"/>
+      <c r="AK39" s="2"/>
+      <c r="AL39" s="2"/>
+      <c r="AM39" s="2"/>
+      <c r="AN39" s="2"/>
+      <c r="AO39" s="2"/>
+      <c r="AP39" s="2"/>
+      <c r="AQ39" s="2"/>
+      <c r="AR39" s="2"/>
+      <c r="AS39" s="2"/>
+      <c r="AT39" s="2"/>
+      <c r="AU39" s="2"/>
+      <c r="AV39" s="2"/>
+      <c r="AW39" s="2"/>
+      <c r="AX39" s="2"/>
+      <c r="AY39" s="2"/>
+      <c r="AZ39" s="2"/>
+      <c r="BA39" s="2"/>
+      <c r="BB39" s="2"/>
+      <c r="BC39" s="2"/>
+      <c r="BD39" s="2"/>
+      <c r="BE39" s="2"/>
+      <c r="BF39" s="2"/>
+      <c r="BG39" s="2"/>
+      <c r="BH39" s="2"/>
+      <c r="BI39" s="2"/>
+      <c r="BJ39" s="2"/>
+      <c r="BK39" s="2"/>
+      <c r="BL39" s="2"/>
+      <c r="BM39" s="2"/>
+      <c r="BN39" s="2"/>
+      <c r="BP39" s="2"/>
     </row>
-    <row r="40" spans="1:31" x14ac:dyDescent="0.45">
+    <row r="40" spans="1:68">
       <c r="A40" t="s">
         <v>33</v>
       </c>
@@ -4506,8 +5733,40 @@
       <c r="AE40">
         <v>2.1863999999999999</v>
       </c>
+      <c r="AF40" s="1"/>
+      <c r="AK40" s="2"/>
+      <c r="AL40" s="2"/>
+      <c r="AM40" s="2"/>
+      <c r="AN40" s="2"/>
+      <c r="AO40" s="2"/>
+      <c r="AP40" s="2"/>
+      <c r="AQ40" s="2"/>
+      <c r="AR40" s="2"/>
+      <c r="AS40" s="2"/>
+      <c r="AT40" s="2"/>
+      <c r="AU40" s="2"/>
+      <c r="AV40" s="2"/>
+      <c r="AW40" s="2"/>
+      <c r="AX40" s="2"/>
+      <c r="AY40" s="2"/>
+      <c r="AZ40" s="2"/>
+      <c r="BA40" s="2"/>
+      <c r="BB40" s="2"/>
+      <c r="BC40" s="2"/>
+      <c r="BD40" s="2"/>
+      <c r="BE40" s="2"/>
+      <c r="BF40" s="2"/>
+      <c r="BG40" s="2"/>
+      <c r="BH40" s="2"/>
+      <c r="BI40" s="2"/>
+      <c r="BJ40" s="2"/>
+      <c r="BK40" s="2"/>
+      <c r="BL40" s="2"/>
+      <c r="BM40" s="2"/>
+      <c r="BN40" s="2"/>
+      <c r="BP40" s="2"/>
     </row>
-    <row r="41" spans="1:31" x14ac:dyDescent="0.45">
+    <row r="41" spans="1:68">
       <c r="A41" t="s">
         <v>74</v>
       </c>
@@ -4601,8 +5860,40 @@
       <c r="AE41">
         <v>-1</v>
       </c>
+      <c r="AF41" s="1"/>
+      <c r="AK41" s="2"/>
+      <c r="AL41" s="2"/>
+      <c r="AM41" s="2"/>
+      <c r="AN41" s="2"/>
+      <c r="AO41" s="2"/>
+      <c r="AP41" s="2"/>
+      <c r="AQ41" s="2"/>
+      <c r="AR41" s="2"/>
+      <c r="AS41" s="2"/>
+      <c r="AT41" s="2"/>
+      <c r="AU41" s="2"/>
+      <c r="AV41" s="2"/>
+      <c r="AW41" s="2"/>
+      <c r="AX41" s="2"/>
+      <c r="AY41" s="2"/>
+      <c r="AZ41" s="2"/>
+      <c r="BA41" s="2"/>
+      <c r="BB41" s="2"/>
+      <c r="BC41" s="2"/>
+      <c r="BD41" s="2"/>
+      <c r="BE41" s="2"/>
+      <c r="BF41" s="2"/>
+      <c r="BG41" s="2"/>
+      <c r="BH41" s="2"/>
+      <c r="BI41" s="2"/>
+      <c r="BJ41" s="2"/>
+      <c r="BK41" s="2"/>
+      <c r="BL41" s="2"/>
+      <c r="BM41" s="2"/>
+      <c r="BN41" s="2"/>
+      <c r="BP41" s="2"/>
     </row>
-    <row r="42" spans="1:31" x14ac:dyDescent="0.45">
+    <row r="42" spans="1:68">
       <c r="A42" t="s">
         <v>70</v>
       </c>
@@ -4696,8 +5987,40 @@
       <c r="AE42">
         <v>3.6600999999999999</v>
       </c>
+      <c r="AF42" s="1"/>
+      <c r="AK42" s="2"/>
+      <c r="AL42" s="2"/>
+      <c r="AM42" s="2"/>
+      <c r="AN42" s="2"/>
+      <c r="AO42" s="2"/>
+      <c r="AP42" s="2"/>
+      <c r="AQ42" s="2"/>
+      <c r="AR42" s="2"/>
+      <c r="AS42" s="2"/>
+      <c r="AT42" s="2"/>
+      <c r="AU42" s="2"/>
+      <c r="AV42" s="2"/>
+      <c r="AW42" s="2"/>
+      <c r="AX42" s="2"/>
+      <c r="AY42" s="2"/>
+      <c r="AZ42" s="2"/>
+      <c r="BA42" s="2"/>
+      <c r="BB42" s="2"/>
+      <c r="BC42" s="2"/>
+      <c r="BD42" s="2"/>
+      <c r="BE42" s="2"/>
+      <c r="BF42" s="2"/>
+      <c r="BG42" s="2"/>
+      <c r="BH42" s="2"/>
+      <c r="BI42" s="2"/>
+      <c r="BJ42" s="2"/>
+      <c r="BK42" s="2"/>
+      <c r="BL42" s="2"/>
+      <c r="BM42" s="2"/>
+      <c r="BN42" s="2"/>
+      <c r="BP42" s="2"/>
     </row>
-    <row r="43" spans="1:31" x14ac:dyDescent="0.45">
+    <row r="43" spans="1:68">
       <c r="A43" t="s">
         <v>6</v>
       </c>
@@ -4791,8 +6114,40 @@
       <c r="AE43">
         <v>3.6074999999999999</v>
       </c>
+      <c r="AF43" s="1"/>
+      <c r="AK43" s="2"/>
+      <c r="AL43" s="2"/>
+      <c r="AM43" s="2"/>
+      <c r="AN43" s="2"/>
+      <c r="AO43" s="2"/>
+      <c r="AP43" s="2"/>
+      <c r="AQ43" s="2"/>
+      <c r="AR43" s="2"/>
+      <c r="AS43" s="2"/>
+      <c r="AT43" s="2"/>
+      <c r="AU43" s="2"/>
+      <c r="AV43" s="2"/>
+      <c r="AW43" s="2"/>
+      <c r="AX43" s="2"/>
+      <c r="AY43" s="2"/>
+      <c r="AZ43" s="2"/>
+      <c r="BA43" s="2"/>
+      <c r="BB43" s="2"/>
+      <c r="BC43" s="2"/>
+      <c r="BD43" s="2"/>
+      <c r="BE43" s="2"/>
+      <c r="BF43" s="2"/>
+      <c r="BG43" s="2"/>
+      <c r="BH43" s="2"/>
+      <c r="BI43" s="2"/>
+      <c r="BJ43" s="2"/>
+      <c r="BK43" s="2"/>
+      <c r="BL43" s="2"/>
+      <c r="BM43" s="2"/>
+      <c r="BN43" s="2"/>
+      <c r="BP43" s="2"/>
     </row>
-    <row r="44" spans="1:31" x14ac:dyDescent="0.45">
+    <row r="44" spans="1:68">
       <c r="A44" t="s">
         <v>8</v>
       </c>
@@ -4886,8 +6241,40 @@
       <c r="AE44">
         <v>-1</v>
       </c>
+      <c r="AF44" s="1"/>
+      <c r="AK44" s="2"/>
+      <c r="AL44" s="2"/>
+      <c r="AM44" s="2"/>
+      <c r="AN44" s="2"/>
+      <c r="AO44" s="2"/>
+      <c r="AP44" s="2"/>
+      <c r="AQ44" s="2"/>
+      <c r="AR44" s="2"/>
+      <c r="AS44" s="2"/>
+      <c r="AT44" s="2"/>
+      <c r="AU44" s="2"/>
+      <c r="AV44" s="2"/>
+      <c r="AW44" s="2"/>
+      <c r="AX44" s="2"/>
+      <c r="AY44" s="2"/>
+      <c r="AZ44" s="2"/>
+      <c r="BA44" s="2"/>
+      <c r="BB44" s="2"/>
+      <c r="BC44" s="2"/>
+      <c r="BD44" s="2"/>
+      <c r="BE44" s="2"/>
+      <c r="BF44" s="2"/>
+      <c r="BG44" s="2"/>
+      <c r="BH44" s="2"/>
+      <c r="BI44" s="2"/>
+      <c r="BJ44" s="2"/>
+      <c r="BK44" s="2"/>
+      <c r="BL44" s="2"/>
+      <c r="BM44" s="2"/>
+      <c r="BN44" s="2"/>
+      <c r="BP44" s="2"/>
     </row>
-    <row r="45" spans="1:31" x14ac:dyDescent="0.45">
+    <row r="45" spans="1:68">
       <c r="A45" t="s">
         <v>81</v>
       </c>
@@ -4981,8 +6368,40 @@
       <c r="AE45">
         <v>0</v>
       </c>
+      <c r="AF45" s="1"/>
+      <c r="AK45" s="2"/>
+      <c r="AL45" s="2"/>
+      <c r="AM45" s="2"/>
+      <c r="AN45" s="2"/>
+      <c r="AO45" s="2"/>
+      <c r="AP45" s="2"/>
+      <c r="AQ45" s="2"/>
+      <c r="AR45" s="2"/>
+      <c r="AS45" s="2"/>
+      <c r="AT45" s="2"/>
+      <c r="AU45" s="2"/>
+      <c r="AV45" s="2"/>
+      <c r="AW45" s="2"/>
+      <c r="AX45" s="2"/>
+      <c r="AY45" s="2"/>
+      <c r="AZ45" s="2"/>
+      <c r="BA45" s="2"/>
+      <c r="BB45" s="2"/>
+      <c r="BC45" s="2"/>
+      <c r="BD45" s="2"/>
+      <c r="BE45" s="2"/>
+      <c r="BF45" s="2"/>
+      <c r="BG45" s="2"/>
+      <c r="BH45" s="2"/>
+      <c r="BI45" s="2"/>
+      <c r="BJ45" s="2"/>
+      <c r="BK45" s="2"/>
+      <c r="BL45" s="2"/>
+      <c r="BM45" s="2"/>
+      <c r="BN45" s="2"/>
+      <c r="BP45" s="2"/>
     </row>
-    <row r="46" spans="1:31" x14ac:dyDescent="0.45">
+    <row r="46" spans="1:68">
       <c r="A46" t="s">
         <v>23</v>
       </c>
@@ -5076,8 +6495,40 @@
       <c r="AE46">
         <v>-1</v>
       </c>
+      <c r="AF46" s="1"/>
+      <c r="AK46" s="2"/>
+      <c r="AL46" s="2"/>
+      <c r="AM46" s="2"/>
+      <c r="AN46" s="2"/>
+      <c r="AO46" s="2"/>
+      <c r="AP46" s="2"/>
+      <c r="AQ46" s="2"/>
+      <c r="AR46" s="2"/>
+      <c r="AS46" s="2"/>
+      <c r="AT46" s="2"/>
+      <c r="AU46" s="2"/>
+      <c r="AV46" s="2"/>
+      <c r="AW46" s="2"/>
+      <c r="AX46" s="2"/>
+      <c r="AY46" s="2"/>
+      <c r="AZ46" s="2"/>
+      <c r="BA46" s="2"/>
+      <c r="BB46" s="2"/>
+      <c r="BC46" s="2"/>
+      <c r="BD46" s="2"/>
+      <c r="BE46" s="2"/>
+      <c r="BF46" s="2"/>
+      <c r="BG46" s="2"/>
+      <c r="BH46" s="2"/>
+      <c r="BI46" s="2"/>
+      <c r="BJ46" s="2"/>
+      <c r="BK46" s="2"/>
+      <c r="BL46" s="2"/>
+      <c r="BM46" s="2"/>
+      <c r="BN46" s="2"/>
+      <c r="BP46" s="2"/>
     </row>
-    <row r="47" spans="1:31" x14ac:dyDescent="0.45">
+    <row r="47" spans="1:68">
       <c r="A47" t="s">
         <v>83</v>
       </c>
@@ -5171,8 +6622,40 @@
       <c r="AE47">
         <v>-1</v>
       </c>
+      <c r="AF47" s="1"/>
+      <c r="AK47" s="2"/>
+      <c r="AL47" s="2"/>
+      <c r="AM47" s="2"/>
+      <c r="AN47" s="2"/>
+      <c r="AO47" s="2"/>
+      <c r="AP47" s="2"/>
+      <c r="AQ47" s="2"/>
+      <c r="AR47" s="2"/>
+      <c r="AS47" s="2"/>
+      <c r="AT47" s="2"/>
+      <c r="AU47" s="2"/>
+      <c r="AV47" s="2"/>
+      <c r="AW47" s="2"/>
+      <c r="AX47" s="2"/>
+      <c r="AY47" s="2"/>
+      <c r="AZ47" s="2"/>
+      <c r="BA47" s="2"/>
+      <c r="BB47" s="2"/>
+      <c r="BC47" s="2"/>
+      <c r="BD47" s="2"/>
+      <c r="BE47" s="2"/>
+      <c r="BF47" s="2"/>
+      <c r="BG47" s="2"/>
+      <c r="BH47" s="2"/>
+      <c r="BI47" s="2"/>
+      <c r="BJ47" s="2"/>
+      <c r="BK47" s="2"/>
+      <c r="BL47" s="2"/>
+      <c r="BM47" s="2"/>
+      <c r="BN47" s="2"/>
+      <c r="BP47" s="2"/>
     </row>
-    <row r="48" spans="1:31" x14ac:dyDescent="0.45">
+    <row r="48" spans="1:68">
       <c r="A48" t="s">
         <v>31</v>
       </c>
@@ -5266,8 +6749,40 @@
       <c r="AE48">
         <v>-1</v>
       </c>
+      <c r="AF48" s="1"/>
+      <c r="AK48" s="2"/>
+      <c r="AL48" s="2"/>
+      <c r="AM48" s="2"/>
+      <c r="AN48" s="2"/>
+      <c r="AO48" s="2"/>
+      <c r="AP48" s="2"/>
+      <c r="AQ48" s="2"/>
+      <c r="AR48" s="2"/>
+      <c r="AS48" s="2"/>
+      <c r="AT48" s="2"/>
+      <c r="AU48" s="2"/>
+      <c r="AV48" s="2"/>
+      <c r="AW48" s="2"/>
+      <c r="AX48" s="2"/>
+      <c r="AY48" s="2"/>
+      <c r="AZ48" s="2"/>
+      <c r="BA48" s="2"/>
+      <c r="BB48" s="2"/>
+      <c r="BC48" s="2"/>
+      <c r="BD48" s="2"/>
+      <c r="BE48" s="2"/>
+      <c r="BF48" s="2"/>
+      <c r="BG48" s="2"/>
+      <c r="BH48" s="2"/>
+      <c r="BI48" s="2"/>
+      <c r="BJ48" s="2"/>
+      <c r="BK48" s="2"/>
+      <c r="BL48" s="2"/>
+      <c r="BM48" s="2"/>
+      <c r="BN48" s="2"/>
+      <c r="BP48" s="2"/>
     </row>
-    <row r="49" spans="1:31" x14ac:dyDescent="0.45">
+    <row r="49" spans="1:68">
       <c r="A49" t="s">
         <v>68</v>
       </c>
@@ -5361,8 +6876,40 @@
       <c r="AE49">
         <v>-1</v>
       </c>
+      <c r="AF49" s="1"/>
+      <c r="AK49" s="2"/>
+      <c r="AL49" s="2"/>
+      <c r="AM49" s="2"/>
+      <c r="AN49" s="2"/>
+      <c r="AO49" s="2"/>
+      <c r="AP49" s="2"/>
+      <c r="AQ49" s="2"/>
+      <c r="AR49" s="2"/>
+      <c r="AS49" s="2"/>
+      <c r="AT49" s="2"/>
+      <c r="AU49" s="2"/>
+      <c r="AV49" s="2"/>
+      <c r="AW49" s="2"/>
+      <c r="AX49" s="2"/>
+      <c r="AY49" s="2"/>
+      <c r="AZ49" s="2"/>
+      <c r="BA49" s="2"/>
+      <c r="BB49" s="2"/>
+      <c r="BC49" s="2"/>
+      <c r="BD49" s="2"/>
+      <c r="BE49" s="2"/>
+      <c r="BF49" s="2"/>
+      <c r="BG49" s="2"/>
+      <c r="BH49" s="2"/>
+      <c r="BI49" s="2"/>
+      <c r="BJ49" s="2"/>
+      <c r="BK49" s="2"/>
+      <c r="BL49" s="2"/>
+      <c r="BM49" s="2"/>
+      <c r="BN49" s="2"/>
+      <c r="BP49" s="2"/>
     </row>
-    <row r="50" spans="1:31" x14ac:dyDescent="0.45">
+    <row r="50" spans="1:68">
       <c r="A50" t="s">
         <v>39</v>
       </c>
@@ -5456,8 +7003,40 @@
       <c r="AE50">
         <v>-1</v>
       </c>
+      <c r="AF50" s="1"/>
+      <c r="AK50" s="2"/>
+      <c r="AL50" s="2"/>
+      <c r="AM50" s="2"/>
+      <c r="AN50" s="2"/>
+      <c r="AO50" s="2"/>
+      <c r="AP50" s="2"/>
+      <c r="AQ50" s="2"/>
+      <c r="AR50" s="2"/>
+      <c r="AS50" s="2"/>
+      <c r="AT50" s="2"/>
+      <c r="AU50" s="2"/>
+      <c r="AV50" s="2"/>
+      <c r="AW50" s="2"/>
+      <c r="AX50" s="2"/>
+      <c r="AY50" s="2"/>
+      <c r="AZ50" s="2"/>
+      <c r="BA50" s="2"/>
+      <c r="BB50" s="2"/>
+      <c r="BC50" s="2"/>
+      <c r="BD50" s="2"/>
+      <c r="BE50" s="2"/>
+      <c r="BF50" s="2"/>
+      <c r="BG50" s="2"/>
+      <c r="BH50" s="2"/>
+      <c r="BI50" s="2"/>
+      <c r="BJ50" s="2"/>
+      <c r="BK50" s="2"/>
+      <c r="BL50" s="2"/>
+      <c r="BM50" s="2"/>
+      <c r="BN50" s="2"/>
+      <c r="BP50" s="2"/>
     </row>
-    <row r="51" spans="1:31" x14ac:dyDescent="0.45">
+    <row r="51" spans="1:68">
       <c r="A51" t="s">
         <v>65</v>
       </c>
@@ -5551,8 +7130,40 @@
       <c r="AE51">
         <v>-1</v>
       </c>
+      <c r="AF51" s="1"/>
+      <c r="AK51" s="2"/>
+      <c r="AL51" s="2"/>
+      <c r="AM51" s="2"/>
+      <c r="AN51" s="2"/>
+      <c r="AO51" s="2"/>
+      <c r="AP51" s="2"/>
+      <c r="AQ51" s="2"/>
+      <c r="AR51" s="2"/>
+      <c r="AS51" s="2"/>
+      <c r="AT51" s="2"/>
+      <c r="AU51" s="2"/>
+      <c r="AV51" s="2"/>
+      <c r="AW51" s="2"/>
+      <c r="AX51" s="2"/>
+      <c r="AY51" s="2"/>
+      <c r="AZ51" s="2"/>
+      <c r="BA51" s="2"/>
+      <c r="BB51" s="2"/>
+      <c r="BC51" s="2"/>
+      <c r="BD51" s="2"/>
+      <c r="BE51" s="2"/>
+      <c r="BF51" s="2"/>
+      <c r="BG51" s="2"/>
+      <c r="BH51" s="2"/>
+      <c r="BI51" s="2"/>
+      <c r="BJ51" s="2"/>
+      <c r="BK51" s="2"/>
+      <c r="BL51" s="2"/>
+      <c r="BM51" s="2"/>
+      <c r="BN51" s="2"/>
+      <c r="BP51" s="2"/>
     </row>
-    <row r="52" spans="1:31" x14ac:dyDescent="0.45">
+    <row r="52" spans="1:68">
       <c r="A52" t="s">
         <v>79</v>
       </c>
@@ -5646,8 +7257,40 @@
       <c r="AE52">
         <v>-1</v>
       </c>
+      <c r="AF52" s="1"/>
+      <c r="AK52" s="2"/>
+      <c r="AL52" s="2"/>
+      <c r="AM52" s="2"/>
+      <c r="AN52" s="2"/>
+      <c r="AO52" s="2"/>
+      <c r="AP52" s="2"/>
+      <c r="AQ52" s="2"/>
+      <c r="AR52" s="2"/>
+      <c r="AS52" s="2"/>
+      <c r="AT52" s="2"/>
+      <c r="AU52" s="2"/>
+      <c r="AV52" s="2"/>
+      <c r="AW52" s="2"/>
+      <c r="AX52" s="2"/>
+      <c r="AY52" s="2"/>
+      <c r="AZ52" s="2"/>
+      <c r="BA52" s="2"/>
+      <c r="BB52" s="2"/>
+      <c r="BC52" s="2"/>
+      <c r="BD52" s="2"/>
+      <c r="BE52" s="2"/>
+      <c r="BF52" s="2"/>
+      <c r="BG52" s="2"/>
+      <c r="BH52" s="2"/>
+      <c r="BI52" s="2"/>
+      <c r="BJ52" s="2"/>
+      <c r="BK52" s="2"/>
+      <c r="BL52" s="2"/>
+      <c r="BM52" s="2"/>
+      <c r="BN52" s="2"/>
+      <c r="BP52" s="2"/>
     </row>
-    <row r="53" spans="1:31" x14ac:dyDescent="0.45">
+    <row r="53" spans="1:68">
       <c r="A53" t="s">
         <v>7</v>
       </c>
@@ -5741,8 +7384,40 @@
       <c r="AE53">
         <v>4.6512000000000002</v>
       </c>
+      <c r="AF53" s="1"/>
+      <c r="AK53" s="2"/>
+      <c r="AL53" s="2"/>
+      <c r="AM53" s="2"/>
+      <c r="AN53" s="2"/>
+      <c r="AO53" s="2"/>
+      <c r="AP53" s="2"/>
+      <c r="AQ53" s="2"/>
+      <c r="AR53" s="2"/>
+      <c r="AS53" s="2"/>
+      <c r="AT53" s="2"/>
+      <c r="AU53" s="2"/>
+      <c r="AV53" s="2"/>
+      <c r="AW53" s="2"/>
+      <c r="AX53" s="2"/>
+      <c r="AY53" s="2"/>
+      <c r="AZ53" s="2"/>
+      <c r="BA53" s="2"/>
+      <c r="BB53" s="2"/>
+      <c r="BC53" s="2"/>
+      <c r="BD53" s="2"/>
+      <c r="BE53" s="2"/>
+      <c r="BF53" s="2"/>
+      <c r="BG53" s="2"/>
+      <c r="BH53" s="2"/>
+      <c r="BI53" s="2"/>
+      <c r="BJ53" s="2"/>
+      <c r="BK53" s="2"/>
+      <c r="BL53" s="2"/>
+      <c r="BM53" s="2"/>
+      <c r="BN53" s="2"/>
+      <c r="BP53" s="2"/>
     </row>
-    <row r="54" spans="1:31" x14ac:dyDescent="0.45">
+    <row r="54" spans="1:68">
       <c r="A54" t="s">
         <v>56</v>
       </c>
@@ -5836,8 +7511,40 @@
       <c r="AE54">
         <v>-1</v>
       </c>
+      <c r="AF54" s="1"/>
+      <c r="AK54" s="2"/>
+      <c r="AL54" s="2"/>
+      <c r="AM54" s="2"/>
+      <c r="AN54" s="2"/>
+      <c r="AO54" s="2"/>
+      <c r="AP54" s="2"/>
+      <c r="AQ54" s="2"/>
+      <c r="AR54" s="2"/>
+      <c r="AS54" s="2"/>
+      <c r="AT54" s="2"/>
+      <c r="AU54" s="2"/>
+      <c r="AV54" s="2"/>
+      <c r="AW54" s="2"/>
+      <c r="AX54" s="2"/>
+      <c r="AY54" s="2"/>
+      <c r="AZ54" s="2"/>
+      <c r="BA54" s="2"/>
+      <c r="BB54" s="2"/>
+      <c r="BC54" s="2"/>
+      <c r="BD54" s="2"/>
+      <c r="BE54" s="2"/>
+      <c r="BF54" s="2"/>
+      <c r="BG54" s="2"/>
+      <c r="BH54" s="2"/>
+      <c r="BI54" s="2"/>
+      <c r="BJ54" s="2"/>
+      <c r="BK54" s="2"/>
+      <c r="BL54" s="2"/>
+      <c r="BM54" s="2"/>
+      <c r="BN54" s="2"/>
+      <c r="BP54" s="2"/>
     </row>
-    <row r="55" spans="1:31" x14ac:dyDescent="0.45">
+    <row r="55" spans="1:68">
       <c r="A55" t="s">
         <v>40</v>
       </c>
@@ -5931,8 +7638,40 @@
       <c r="AE55">
         <v>2.6444999999999999</v>
       </c>
+      <c r="AF55" s="1"/>
+      <c r="AK55" s="2"/>
+      <c r="AL55" s="2"/>
+      <c r="AM55" s="2"/>
+      <c r="AN55" s="2"/>
+      <c r="AO55" s="2"/>
+      <c r="AP55" s="2"/>
+      <c r="AQ55" s="2"/>
+      <c r="AR55" s="2"/>
+      <c r="AS55" s="2"/>
+      <c r="AT55" s="2"/>
+      <c r="AU55" s="2"/>
+      <c r="AV55" s="2"/>
+      <c r="AW55" s="2"/>
+      <c r="AX55" s="2"/>
+      <c r="AY55" s="2"/>
+      <c r="AZ55" s="2"/>
+      <c r="BA55" s="2"/>
+      <c r="BB55" s="2"/>
+      <c r="BC55" s="2"/>
+      <c r="BD55" s="2"/>
+      <c r="BE55" s="2"/>
+      <c r="BF55" s="2"/>
+      <c r="BG55" s="2"/>
+      <c r="BH55" s="2"/>
+      <c r="BI55" s="2"/>
+      <c r="BJ55" s="2"/>
+      <c r="BK55" s="2"/>
+      <c r="BL55" s="2"/>
+      <c r="BM55" s="2"/>
+      <c r="BN55" s="2"/>
+      <c r="BP55" s="2"/>
     </row>
-    <row r="56" spans="1:31" x14ac:dyDescent="0.45">
+    <row r="56" spans="1:68">
       <c r="A56" t="s">
         <v>75</v>
       </c>
@@ -6026,8 +7765,40 @@
       <c r="AE56">
         <v>-1</v>
       </c>
+      <c r="AF56" s="1"/>
+      <c r="AK56" s="2"/>
+      <c r="AL56" s="2"/>
+      <c r="AM56" s="2"/>
+      <c r="AN56" s="2"/>
+      <c r="AO56" s="2"/>
+      <c r="AP56" s="2"/>
+      <c r="AQ56" s="2"/>
+      <c r="AR56" s="2"/>
+      <c r="AS56" s="2"/>
+      <c r="AT56" s="2"/>
+      <c r="AU56" s="2"/>
+      <c r="AV56" s="2"/>
+      <c r="AW56" s="2"/>
+      <c r="AX56" s="2"/>
+      <c r="AY56" s="2"/>
+      <c r="AZ56" s="2"/>
+      <c r="BA56" s="2"/>
+      <c r="BB56" s="2"/>
+      <c r="BC56" s="2"/>
+      <c r="BD56" s="2"/>
+      <c r="BE56" s="2"/>
+      <c r="BF56" s="2"/>
+      <c r="BG56" s="2"/>
+      <c r="BH56" s="2"/>
+      <c r="BI56" s="2"/>
+      <c r="BJ56" s="2"/>
+      <c r="BK56" s="2"/>
+      <c r="BL56" s="2"/>
+      <c r="BM56" s="2"/>
+      <c r="BN56" s="2"/>
+      <c r="BP56" s="2"/>
     </row>
-    <row r="57" spans="1:31" x14ac:dyDescent="0.45">
+    <row r="57" spans="1:68">
       <c r="A57" t="s">
         <v>93</v>
       </c>
@@ -6121,8 +7892,40 @@
       <c r="AE57">
         <v>1.8826000000000001</v>
       </c>
+      <c r="AF57" s="1"/>
+      <c r="AK57" s="2"/>
+      <c r="AL57" s="2"/>
+      <c r="AM57" s="2"/>
+      <c r="AN57" s="2"/>
+      <c r="AO57" s="2"/>
+      <c r="AP57" s="2"/>
+      <c r="AQ57" s="2"/>
+      <c r="AR57" s="2"/>
+      <c r="AS57" s="2"/>
+      <c r="AT57" s="2"/>
+      <c r="AU57" s="2"/>
+      <c r="AV57" s="2"/>
+      <c r="AW57" s="2"/>
+      <c r="AX57" s="2"/>
+      <c r="AY57" s="2"/>
+      <c r="AZ57" s="2"/>
+      <c r="BA57" s="2"/>
+      <c r="BB57" s="2"/>
+      <c r="BC57" s="2"/>
+      <c r="BD57" s="2"/>
+      <c r="BE57" s="2"/>
+      <c r="BF57" s="2"/>
+      <c r="BG57" s="2"/>
+      <c r="BH57" s="2"/>
+      <c r="BI57" s="2"/>
+      <c r="BJ57" s="2"/>
+      <c r="BK57" s="2"/>
+      <c r="BL57" s="2"/>
+      <c r="BM57" s="2"/>
+      <c r="BN57" s="2"/>
+      <c r="BP57" s="2"/>
     </row>
-    <row r="58" spans="1:31" x14ac:dyDescent="0.45">
+    <row r="58" spans="1:68">
       <c r="A58" t="s">
         <v>45</v>
       </c>
@@ -6216,8 +8019,40 @@
       <c r="AE58">
         <v>0</v>
       </c>
+      <c r="AF58" s="1"/>
+      <c r="AK58" s="2"/>
+      <c r="AL58" s="2"/>
+      <c r="AM58" s="2"/>
+      <c r="AN58" s="2"/>
+      <c r="AO58" s="2"/>
+      <c r="AP58" s="2"/>
+      <c r="AQ58" s="2"/>
+      <c r="AR58" s="2"/>
+      <c r="AS58" s="2"/>
+      <c r="AT58" s="2"/>
+      <c r="AU58" s="2"/>
+      <c r="AV58" s="2"/>
+      <c r="AW58" s="2"/>
+      <c r="AX58" s="2"/>
+      <c r="AY58" s="2"/>
+      <c r="AZ58" s="2"/>
+      <c r="BA58" s="2"/>
+      <c r="BB58" s="2"/>
+      <c r="BC58" s="2"/>
+      <c r="BD58" s="2"/>
+      <c r="BE58" s="2"/>
+      <c r="BF58" s="2"/>
+      <c r="BG58" s="2"/>
+      <c r="BH58" s="2"/>
+      <c r="BI58" s="2"/>
+      <c r="BJ58" s="2"/>
+      <c r="BK58" s="2"/>
+      <c r="BL58" s="2"/>
+      <c r="BM58" s="2"/>
+      <c r="BN58" s="2"/>
+      <c r="BP58" s="2"/>
     </row>
-    <row r="59" spans="1:31" x14ac:dyDescent="0.45">
+    <row r="59" spans="1:68">
       <c r="A59" t="s">
         <v>50</v>
       </c>
@@ -6311,8 +8146,40 @@
       <c r="AE59">
         <v>1.2613000000000001</v>
       </c>
+      <c r="AF59" s="1"/>
+      <c r="AK59" s="2"/>
+      <c r="AL59" s="2"/>
+      <c r="AM59" s="2"/>
+      <c r="AN59" s="2"/>
+      <c r="AO59" s="2"/>
+      <c r="AP59" s="2"/>
+      <c r="AQ59" s="2"/>
+      <c r="AR59" s="2"/>
+      <c r="AS59" s="2"/>
+      <c r="AT59" s="2"/>
+      <c r="AU59" s="2"/>
+      <c r="AV59" s="2"/>
+      <c r="AW59" s="2"/>
+      <c r="AX59" s="2"/>
+      <c r="AY59" s="2"/>
+      <c r="AZ59" s="2"/>
+      <c r="BA59" s="2"/>
+      <c r="BB59" s="2"/>
+      <c r="BC59" s="2"/>
+      <c r="BD59" s="2"/>
+      <c r="BE59" s="2"/>
+      <c r="BF59" s="2"/>
+      <c r="BG59" s="2"/>
+      <c r="BH59" s="2"/>
+      <c r="BI59" s="2"/>
+      <c r="BJ59" s="2"/>
+      <c r="BK59" s="2"/>
+      <c r="BL59" s="2"/>
+      <c r="BM59" s="2"/>
+      <c r="BN59" s="2"/>
+      <c r="BP59" s="2"/>
     </row>
-    <row r="60" spans="1:31" x14ac:dyDescent="0.45">
+    <row r="60" spans="1:68">
       <c r="A60" t="s">
         <v>46</v>
       </c>
@@ -6406,8 +8273,40 @@
       <c r="AE60">
         <v>3.7797999999999998</v>
       </c>
+      <c r="AF60" s="1"/>
+      <c r="AK60" s="2"/>
+      <c r="AL60" s="2"/>
+      <c r="AM60" s="2"/>
+      <c r="AN60" s="2"/>
+      <c r="AO60" s="2"/>
+      <c r="AP60" s="2"/>
+      <c r="AQ60" s="2"/>
+      <c r="AR60" s="2"/>
+      <c r="AS60" s="2"/>
+      <c r="AT60" s="2"/>
+      <c r="AU60" s="2"/>
+      <c r="AV60" s="2"/>
+      <c r="AW60" s="2"/>
+      <c r="AX60" s="2"/>
+      <c r="AY60" s="2"/>
+      <c r="AZ60" s="2"/>
+      <c r="BA60" s="2"/>
+      <c r="BB60" s="2"/>
+      <c r="BC60" s="2"/>
+      <c r="BD60" s="2"/>
+      <c r="BE60" s="2"/>
+      <c r="BF60" s="2"/>
+      <c r="BG60" s="2"/>
+      <c r="BH60" s="2"/>
+      <c r="BI60" s="2"/>
+      <c r="BJ60" s="2"/>
+      <c r="BK60" s="2"/>
+      <c r="BL60" s="2"/>
+      <c r="BM60" s="2"/>
+      <c r="BN60" s="2"/>
+      <c r="BP60" s="2"/>
     </row>
-    <row r="61" spans="1:31" x14ac:dyDescent="0.45">
+    <row r="61" spans="1:68">
       <c r="A61" t="s">
         <v>64</v>
       </c>
@@ -6501,8 +8400,40 @@
       <c r="AE61">
         <v>-1</v>
       </c>
+      <c r="AF61" s="1"/>
+      <c r="AK61" s="2"/>
+      <c r="AL61" s="2"/>
+      <c r="AM61" s="2"/>
+      <c r="AN61" s="2"/>
+      <c r="AO61" s="2"/>
+      <c r="AP61" s="2"/>
+      <c r="AQ61" s="2"/>
+      <c r="AR61" s="2"/>
+      <c r="AS61" s="2"/>
+      <c r="AT61" s="2"/>
+      <c r="AU61" s="2"/>
+      <c r="AV61" s="2"/>
+      <c r="AW61" s="2"/>
+      <c r="AX61" s="2"/>
+      <c r="AY61" s="2"/>
+      <c r="AZ61" s="2"/>
+      <c r="BA61" s="2"/>
+      <c r="BB61" s="2"/>
+      <c r="BC61" s="2"/>
+      <c r="BD61" s="2"/>
+      <c r="BE61" s="2"/>
+      <c r="BF61" s="2"/>
+      <c r="BG61" s="2"/>
+      <c r="BH61" s="2"/>
+      <c r="BI61" s="2"/>
+      <c r="BJ61" s="2"/>
+      <c r="BK61" s="2"/>
+      <c r="BL61" s="2"/>
+      <c r="BM61" s="2"/>
+      <c r="BN61" s="2"/>
+      <c r="BP61" s="2"/>
     </row>
-    <row r="62" spans="1:31" x14ac:dyDescent="0.45">
+    <row r="62" spans="1:68">
       <c r="A62" t="s">
         <v>76</v>
       </c>
@@ -6596,9 +8527,41 @@
       <c r="AE62">
         <v>5.2779999999999996</v>
       </c>
+      <c r="AF62" s="1"/>
+      <c r="AK62" s="2"/>
+      <c r="AL62" s="2"/>
+      <c r="AM62" s="2"/>
+      <c r="AN62" s="2"/>
+      <c r="AO62" s="2"/>
+      <c r="AP62" s="2"/>
+      <c r="AQ62" s="2"/>
+      <c r="AR62" s="2"/>
+      <c r="AS62" s="2"/>
+      <c r="AT62" s="2"/>
+      <c r="AU62" s="2"/>
+      <c r="AV62" s="2"/>
+      <c r="AW62" s="2"/>
+      <c r="AX62" s="2"/>
+      <c r="AY62" s="2"/>
+      <c r="AZ62" s="2"/>
+      <c r="BA62" s="2"/>
+      <c r="BB62" s="2"/>
+      <c r="BC62" s="2"/>
+      <c r="BD62" s="2"/>
+      <c r="BE62" s="2"/>
+      <c r="BF62" s="2"/>
+      <c r="BG62" s="2"/>
+      <c r="BH62" s="2"/>
+      <c r="BI62" s="2"/>
+      <c r="BJ62" s="2"/>
+      <c r="BK62" s="2"/>
+      <c r="BL62" s="2"/>
+      <c r="BM62" s="2"/>
+      <c r="BN62" s="2"/>
+      <c r="BP62" s="2"/>
     </row>
   </sheetData>
-  <sortState ref="A2:AE32">
+  <sortState ref="A2:BH32">
     <sortCondition ref="A2"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -6608,19 +8571,20 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:AD79"/>
+  <dimension ref="A1:AF79"/>
   <sheetViews>
-    <sheetView topLeftCell="Q46" workbookViewId="0">
-      <selection activeCell="AE46" sqref="AE1:BP1048576"/>
+    <sheetView topLeftCell="R46" workbookViewId="0">
+      <selection activeCell="AF46" sqref="AF1:BP1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.65" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="14.65"/>
   <cols>
     <col min="1" max="1" width="18.28515625" customWidth="1"/>
-    <col min="2" max="30" width="9.140625" customWidth="1"/>
+    <col min="2" max="31" width="9.140625" customWidth="1"/>
+    <col min="33" max="36" width="18.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:30" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:32">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -6711,8 +8675,11 @@
       <c r="AD1">
         <v>59</v>
       </c>
+      <c r="AE1">
+        <v>13</v>
+      </c>
     </row>
-    <row r="2" spans="1:30" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:32">
       <c r="A2" t="s">
         <v>26</v>
       </c>
@@ -6803,8 +8770,12 @@
       <c r="AD2">
         <v>2.0651999999999999</v>
       </c>
+      <c r="AE2">
+        <v>4.6242999999999999</v>
+      </c>
+      <c r="AF2" s="1"/>
     </row>
-    <row r="3" spans="1:30" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:32">
       <c r="A3" t="s">
         <v>5</v>
       </c>
@@ -6895,8 +8866,12 @@
       <c r="AD3">
         <v>4.5636999999999999</v>
       </c>
+      <c r="AE3">
+        <v>3.8835000000000002</v>
+      </c>
+      <c r="AF3" s="1"/>
     </row>
-    <row r="4" spans="1:30" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:32">
       <c r="A4" t="s">
         <v>66</v>
       </c>
@@ -6987,8 +8962,12 @@
       <c r="AD4">
         <v>-1</v>
       </c>
+      <c r="AE4">
+        <v>-1</v>
+      </c>
+      <c r="AF4" s="1"/>
     </row>
-    <row r="5" spans="1:30" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:32">
       <c r="A5" t="s">
         <v>58</v>
       </c>
@@ -7079,8 +9058,12 @@
       <c r="AD5">
         <v>-1</v>
       </c>
+      <c r="AE5">
+        <v>-1</v>
+      </c>
+      <c r="AF5" s="1"/>
     </row>
-    <row r="6" spans="1:30" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:32">
       <c r="A6" t="s">
         <v>72</v>
       </c>
@@ -7171,8 +9154,12 @@
       <c r="AD6">
         <v>-1</v>
       </c>
+      <c r="AE6">
+        <v>2.3386999999999998</v>
+      </c>
+      <c r="AF6" s="1"/>
     </row>
-    <row r="7" spans="1:30" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:32">
       <c r="A7" t="s">
         <v>35</v>
       </c>
@@ -7263,8 +9250,12 @@
       <c r="AD7">
         <v>3.7528999999999999</v>
       </c>
+      <c r="AE7">
+        <v>-1</v>
+      </c>
+      <c r="AF7" s="1"/>
     </row>
-    <row r="8" spans="1:30" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:32">
       <c r="A8" t="s">
         <v>63</v>
       </c>
@@ -7355,8 +9346,12 @@
       <c r="AD8">
         <v>4.7347999999999999</v>
       </c>
+      <c r="AE8">
+        <v>0</v>
+      </c>
+      <c r="AF8" s="1"/>
     </row>
-    <row r="9" spans="1:30" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:32">
       <c r="A9" t="s">
         <v>27</v>
       </c>
@@ -7447,8 +9442,12 @@
       <c r="AD9">
         <v>-1</v>
       </c>
+      <c r="AE9">
+        <v>-1</v>
+      </c>
+      <c r="AF9" s="1"/>
     </row>
-    <row r="10" spans="1:30" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:32">
       <c r="A10" t="s">
         <v>89</v>
       </c>
@@ -7539,8 +9538,12 @@
       <c r="AD10">
         <v>-1</v>
       </c>
+      <c r="AE10">
+        <v>-1</v>
+      </c>
+      <c r="AF10" s="1"/>
     </row>
-    <row r="11" spans="1:30" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:32">
       <c r="A11" t="s">
         <v>87</v>
       </c>
@@ -7631,8 +9634,12 @@
       <c r="AD11">
         <v>-1</v>
       </c>
+      <c r="AE11">
+        <v>-1</v>
+      </c>
+      <c r="AF11" s="1"/>
     </row>
-    <row r="12" spans="1:30" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:32">
       <c r="A12" t="s">
         <v>42</v>
       </c>
@@ -7723,8 +9730,12 @@
       <c r="AD12">
         <v>-1</v>
       </c>
+      <c r="AE12">
+        <v>3.6568999999999998</v>
+      </c>
+      <c r="AF12" s="1"/>
     </row>
-    <row r="13" spans="1:30" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:32">
       <c r="A13" t="s">
         <v>59</v>
       </c>
@@ -7815,8 +9826,12 @@
       <c r="AD13">
         <v>-1</v>
       </c>
+      <c r="AE13">
+        <v>-1</v>
+      </c>
+      <c r="AF13" s="1"/>
     </row>
-    <row r="14" spans="1:30" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:32">
       <c r="A14" t="s">
         <v>18</v>
       </c>
@@ -7907,8 +9922,12 @@
       <c r="AD14">
         <v>-1</v>
       </c>
+      <c r="AE14">
+        <v>3.2282000000000002</v>
+      </c>
+      <c r="AF14" s="1"/>
     </row>
-    <row r="15" spans="1:30" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:32">
       <c r="A15" t="s">
         <v>3</v>
       </c>
@@ -7999,8 +10018,12 @@
       <c r="AD15">
         <v>4.0034999999999998</v>
       </c>
+      <c r="AE15">
+        <v>5.4383999999999997</v>
+      </c>
+      <c r="AF15" s="1"/>
     </row>
-    <row r="16" spans="1:30" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:32">
       <c r="A16" t="s">
         <v>14</v>
       </c>
@@ -8091,8 +10114,12 @@
       <c r="AD16">
         <v>2.7921</v>
       </c>
+      <c r="AE16">
+        <v>4.5929000000000002</v>
+      </c>
+      <c r="AF16" s="1"/>
     </row>
-    <row r="17" spans="1:30" x14ac:dyDescent="0.45">
+    <row r="17" spans="1:32">
       <c r="A17" t="s">
         <v>32</v>
       </c>
@@ -8183,8 +10210,12 @@
       <c r="AD17">
         <v>5.2583000000000002</v>
       </c>
+      <c r="AE17">
+        <v>-1</v>
+      </c>
+      <c r="AF17" s="1"/>
     </row>
-    <row r="18" spans="1:30" x14ac:dyDescent="0.45">
+    <row r="18" spans="1:32">
       <c r="A18" t="s">
         <v>4</v>
       </c>
@@ -8275,8 +10306,12 @@
       <c r="AD18">
         <v>1.9968999999999999</v>
       </c>
+      <c r="AE18">
+        <v>6.5919999999999996</v>
+      </c>
+      <c r="AF18" s="1"/>
     </row>
-    <row r="19" spans="1:30" x14ac:dyDescent="0.45">
+    <row r="19" spans="1:32">
       <c r="A19" t="s">
         <v>73</v>
       </c>
@@ -8367,8 +10402,12 @@
       <c r="AD19">
         <v>-1</v>
       </c>
+      <c r="AE19">
+        <v>-1</v>
+      </c>
+      <c r="AF19" s="1"/>
     </row>
-    <row r="20" spans="1:30" x14ac:dyDescent="0.45">
+    <row r="20" spans="1:32">
       <c r="A20" t="s">
         <v>28</v>
       </c>
@@ -8459,8 +10498,12 @@
       <c r="AD20">
         <v>-1</v>
       </c>
+      <c r="AE20">
+        <v>-1</v>
+      </c>
+      <c r="AF20" s="1"/>
     </row>
-    <row r="21" spans="1:30" x14ac:dyDescent="0.45">
+    <row r="21" spans="1:32">
       <c r="A21" t="s">
         <v>20</v>
       </c>
@@ -8551,8 +10594,12 @@
       <c r="AD21">
         <v>-1</v>
       </c>
+      <c r="AE21">
+        <v>-1</v>
+      </c>
+      <c r="AF21" s="1"/>
     </row>
-    <row r="22" spans="1:30" x14ac:dyDescent="0.45">
+    <row r="22" spans="1:32">
       <c r="A22" t="s">
         <v>41</v>
       </c>
@@ -8643,8 +10690,12 @@
       <c r="AD22">
         <v>2.0424000000000002</v>
       </c>
+      <c r="AE22">
+        <v>-1</v>
+      </c>
+      <c r="AF22" s="1"/>
     </row>
-    <row r="23" spans="1:30" x14ac:dyDescent="0.45">
+    <row r="23" spans="1:32">
       <c r="A23" t="s">
         <v>9</v>
       </c>
@@ -8735,8 +10786,12 @@
       <c r="AD23">
         <v>6.0126999999999997</v>
       </c>
+      <c r="AE23">
+        <v>2.7372000000000001</v>
+      </c>
+      <c r="AF23" s="1"/>
     </row>
-    <row r="24" spans="1:30" x14ac:dyDescent="0.45">
+    <row r="24" spans="1:32">
       <c r="A24" t="s">
         <v>94</v>
       </c>
@@ -8827,8 +10882,12 @@
       <c r="AD24">
         <v>-1</v>
       </c>
+      <c r="AE24">
+        <v>-1</v>
+      </c>
+      <c r="AF24" s="1"/>
     </row>
-    <row r="25" spans="1:30" x14ac:dyDescent="0.45">
+    <row r="25" spans="1:32">
       <c r="A25" t="s">
         <v>24</v>
       </c>
@@ -8919,8 +10978,12 @@
       <c r="AD25">
         <v>-1</v>
       </c>
+      <c r="AE25">
+        <v>-1</v>
+      </c>
+      <c r="AF25" s="1"/>
     </row>
-    <row r="26" spans="1:30" x14ac:dyDescent="0.45">
+    <row r="26" spans="1:32">
       <c r="A26" t="s">
         <v>1</v>
       </c>
@@ -9011,8 +11074,12 @@
       <c r="AD26">
         <v>3.1153</v>
       </c>
+      <c r="AE26">
+        <v>7.9062999999999999</v>
+      </c>
+      <c r="AF26" s="1"/>
     </row>
-    <row r="27" spans="1:30" x14ac:dyDescent="0.45">
+    <row r="27" spans="1:32">
       <c r="A27" t="s">
         <v>51</v>
       </c>
@@ -9103,8 +11170,12 @@
       <c r="AD27">
         <v>-1</v>
       </c>
+      <c r="AE27">
+        <v>2.2115</v>
+      </c>
+      <c r="AF27" s="1"/>
     </row>
-    <row r="28" spans="1:30" x14ac:dyDescent="0.45">
+    <row r="28" spans="1:32">
       <c r="A28" t="s">
         <v>71</v>
       </c>
@@ -9195,8 +11266,12 @@
       <c r="AD28">
         <v>-1</v>
       </c>
+      <c r="AE28">
+        <v>5.6009000000000002</v>
+      </c>
+      <c r="AF28" s="1"/>
     </row>
-    <row r="29" spans="1:30" x14ac:dyDescent="0.45">
+    <row r="29" spans="1:32">
       <c r="A29" t="s">
         <v>57</v>
       </c>
@@ -9287,8 +11362,12 @@
       <c r="AD29">
         <v>-1</v>
       </c>
+      <c r="AE29">
+        <v>-1</v>
+      </c>
+      <c r="AF29" s="1"/>
     </row>
-    <row r="30" spans="1:30" x14ac:dyDescent="0.45">
+    <row r="30" spans="1:32">
       <c r="A30" t="s">
         <v>29</v>
       </c>
@@ -9379,8 +11458,12 @@
       <c r="AD30">
         <v>-1</v>
       </c>
+      <c r="AE30">
+        <v>6.6501999999999999</v>
+      </c>
+      <c r="AF30" s="1"/>
     </row>
-    <row r="31" spans="1:30" x14ac:dyDescent="0.45">
+    <row r="31" spans="1:32">
       <c r="A31" t="s">
         <v>25</v>
       </c>
@@ -9471,8 +11554,12 @@
       <c r="AD31">
         <v>0</v>
       </c>
+      <c r="AE31">
+        <v>3.3965000000000001</v>
+      </c>
+      <c r="AF31" s="1"/>
     </row>
-    <row r="32" spans="1:30" x14ac:dyDescent="0.45">
+    <row r="32" spans="1:32">
       <c r="A32" t="s">
         <v>54</v>
       </c>
@@ -9563,8 +11650,12 @@
       <c r="AD32">
         <v>-1</v>
       </c>
+      <c r="AE32">
+        <v>-1</v>
+      </c>
+      <c r="AF32" s="1"/>
     </row>
-    <row r="33" spans="1:30" x14ac:dyDescent="0.45">
+    <row r="33" spans="1:32">
       <c r="A33" t="s">
         <v>53</v>
       </c>
@@ -9655,8 +11746,12 @@
       <c r="AD33">
         <v>-1</v>
       </c>
+      <c r="AE33">
+        <v>-1</v>
+      </c>
+      <c r="AF33" s="1"/>
     </row>
-    <row r="34" spans="1:30" x14ac:dyDescent="0.45">
+    <row r="34" spans="1:32">
       <c r="A34" t="s">
         <v>11</v>
       </c>
@@ -9747,8 +11842,12 @@
       <c r="AD34">
         <v>-1</v>
       </c>
+      <c r="AE34">
+        <v>4.2419000000000002</v>
+      </c>
+      <c r="AF34" s="1"/>
     </row>
-    <row r="35" spans="1:30" x14ac:dyDescent="0.45">
+    <row r="35" spans="1:32">
       <c r="A35" t="s">
         <v>43</v>
       </c>
@@ -9839,8 +11938,12 @@
       <c r="AD35">
         <v>-1</v>
       </c>
+      <c r="AE35">
+        <v>0</v>
+      </c>
+      <c r="AF35" s="1"/>
     </row>
-    <row r="36" spans="1:30" x14ac:dyDescent="0.45">
+    <row r="36" spans="1:32">
       <c r="A36" t="s">
         <v>69</v>
       </c>
@@ -9931,8 +12034,12 @@
       <c r="AD36">
         <v>-1</v>
       </c>
+      <c r="AE36">
+        <v>-1</v>
+      </c>
+      <c r="AF36" s="1"/>
     </row>
-    <row r="37" spans="1:30" x14ac:dyDescent="0.45">
+    <row r="37" spans="1:32">
       <c r="A37" t="s">
         <v>85</v>
       </c>
@@ -10023,8 +12130,12 @@
       <c r="AD37">
         <v>-1</v>
       </c>
+      <c r="AE37">
+        <v>0</v>
+      </c>
+      <c r="AF37" s="1"/>
     </row>
-    <row r="38" spans="1:30" x14ac:dyDescent="0.45">
+    <row r="38" spans="1:32">
       <c r="A38" t="s">
         <v>38</v>
       </c>
@@ -10115,8 +12226,12 @@
       <c r="AD38">
         <v>-1</v>
       </c>
+      <c r="AE38">
+        <v>-1</v>
+      </c>
+      <c r="AF38" s="1"/>
     </row>
-    <row r="39" spans="1:30" x14ac:dyDescent="0.45">
+    <row r="39" spans="1:32">
       <c r="A39" t="s">
         <v>52</v>
       </c>
@@ -10207,8 +12322,12 @@
       <c r="AD39">
         <v>-1</v>
       </c>
+      <c r="AE39">
+        <v>-1</v>
+      </c>
+      <c r="AF39" s="1"/>
     </row>
-    <row r="40" spans="1:30" x14ac:dyDescent="0.45">
+    <row r="40" spans="1:32">
       <c r="A40" t="s">
         <v>37</v>
       </c>
@@ -10299,8 +12418,12 @@
       <c r="AD40">
         <v>-1</v>
       </c>
+      <c r="AE40">
+        <v>2.573</v>
+      </c>
+      <c r="AF40" s="1"/>
     </row>
-    <row r="41" spans="1:30" x14ac:dyDescent="0.45">
+    <row r="41" spans="1:32">
       <c r="A41" t="s">
         <v>95</v>
       </c>
@@ -10391,8 +12514,12 @@
       <c r="AD41">
         <v>-1</v>
       </c>
+      <c r="AE41">
+        <v>-1</v>
+      </c>
+      <c r="AF41" s="1"/>
     </row>
-    <row r="42" spans="1:30" x14ac:dyDescent="0.45">
+    <row r="42" spans="1:32">
       <c r="A42" t="s">
         <v>62</v>
       </c>
@@ -10483,8 +12610,12 @@
       <c r="AD42">
         <v>4.7275999999999998</v>
       </c>
+      <c r="AE42">
+        <v>5.2355999999999998</v>
+      </c>
+      <c r="AF42" s="1"/>
     </row>
-    <row r="43" spans="1:30" x14ac:dyDescent="0.45">
+    <row r="43" spans="1:32">
       <c r="A43" t="s">
         <v>12</v>
       </c>
@@ -10575,8 +12706,12 @@
       <c r="AD43">
         <v>-1</v>
       </c>
+      <c r="AE43">
+        <v>4.931</v>
+      </c>
+      <c r="AF43" s="1"/>
     </row>
-    <row r="44" spans="1:30" x14ac:dyDescent="0.45">
+    <row r="44" spans="1:32">
       <c r="A44" t="s">
         <v>19</v>
       </c>
@@ -10667,8 +12802,12 @@
       <c r="AD44">
         <v>-1</v>
       </c>
+      <c r="AE44">
+        <v>-1</v>
+      </c>
+      <c r="AF44" s="1"/>
     </row>
-    <row r="45" spans="1:30" x14ac:dyDescent="0.45">
+    <row r="45" spans="1:32">
       <c r="A45" t="s">
         <v>96</v>
       </c>
@@ -10759,8 +12898,12 @@
       <c r="AD45">
         <v>4.8109999999999999</v>
       </c>
+      <c r="AE45">
+        <v>4.7664</v>
+      </c>
+      <c r="AF45" s="1"/>
     </row>
-    <row r="46" spans="1:30" x14ac:dyDescent="0.45">
+    <row r="46" spans="1:32">
       <c r="A46" t="s">
         <v>8</v>
       </c>
@@ -10851,8 +12994,12 @@
       <c r="AD46">
         <v>-1</v>
       </c>
+      <c r="AE46">
+        <v>2.1355</v>
+      </c>
+      <c r="AF46" s="1"/>
     </row>
-    <row r="47" spans="1:30" x14ac:dyDescent="0.45">
+    <row r="47" spans="1:32">
       <c r="A47" t="s">
         <v>81</v>
       </c>
@@ -10943,8 +13090,12 @@
       <c r="AD47">
         <v>-1</v>
       </c>
+      <c r="AE47">
+        <v>4.6154000000000002</v>
+      </c>
+      <c r="AF47" s="1"/>
     </row>
-    <row r="48" spans="1:30" x14ac:dyDescent="0.45">
+    <row r="48" spans="1:32">
       <c r="A48" t="s">
         <v>88</v>
       </c>
@@ -11035,8 +13186,12 @@
       <c r="AD48">
         <v>-1</v>
       </c>
+      <c r="AE48">
+        <v>-1</v>
+      </c>
+      <c r="AF48" s="1"/>
     </row>
-    <row r="49" spans="1:30" x14ac:dyDescent="0.45">
+    <row r="49" spans="1:32">
       <c r="A49" t="s">
         <v>84</v>
       </c>
@@ -11127,8 +13282,12 @@
       <c r="AD49">
         <v>3.2967</v>
       </c>
+      <c r="AE49">
+        <v>5.3747999999999996</v>
+      </c>
+      <c r="AF49" s="1"/>
     </row>
-    <row r="50" spans="1:30" x14ac:dyDescent="0.45">
+    <row r="50" spans="1:32">
       <c r="A50" t="s">
         <v>74</v>
       </c>
@@ -11219,8 +13378,12 @@
       <c r="AD50">
         <v>-1</v>
       </c>
+      <c r="AE50">
+        <v>-1</v>
+      </c>
+      <c r="AF50" s="1"/>
     </row>
-    <row r="51" spans="1:30" x14ac:dyDescent="0.45">
+    <row r="51" spans="1:32">
       <c r="A51" t="s">
         <v>92</v>
       </c>
@@ -11311,8 +13474,12 @@
       <c r="AD51">
         <v>-1</v>
       </c>
+      <c r="AE51">
+        <v>5.7458999999999998</v>
+      </c>
+      <c r="AF51" s="1"/>
     </row>
-    <row r="52" spans="1:30" x14ac:dyDescent="0.45">
+    <row r="52" spans="1:32">
       <c r="A52" t="s">
         <v>22</v>
       </c>
@@ -11403,8 +13570,12 @@
       <c r="AD52">
         <v>-1</v>
       </c>
+      <c r="AE52">
+        <v>3.7831999999999999</v>
+      </c>
+      <c r="AF52" s="1"/>
     </row>
-    <row r="53" spans="1:30" x14ac:dyDescent="0.45">
+    <row r="53" spans="1:32">
       <c r="A53" t="s">
         <v>23</v>
       </c>
@@ -11495,8 +13666,12 @@
       <c r="AD53">
         <v>6.5434000000000001</v>
       </c>
+      <c r="AE53">
+        <v>7.5472000000000001</v>
+      </c>
+      <c r="AF53" s="1"/>
     </row>
-    <row r="54" spans="1:30" x14ac:dyDescent="0.45">
+    <row r="54" spans="1:32">
       <c r="A54" t="s">
         <v>49</v>
       </c>
@@ -11587,8 +13762,12 @@
       <c r="AD54">
         <v>-1</v>
       </c>
+      <c r="AE54">
+        <v>-1</v>
+      </c>
+      <c r="AF54" s="1"/>
     </row>
-    <row r="55" spans="1:30" x14ac:dyDescent="0.45">
+    <row r="55" spans="1:32">
       <c r="A55" t="s">
         <v>21</v>
       </c>
@@ -11679,8 +13858,12 @@
       <c r="AD55">
         <v>-1</v>
       </c>
+      <c r="AE55">
+        <v>-1</v>
+      </c>
+      <c r="AF55" s="1"/>
     </row>
-    <row r="56" spans="1:30" x14ac:dyDescent="0.45">
+    <row r="56" spans="1:32">
       <c r="A56" t="s">
         <v>67</v>
       </c>
@@ -11771,8 +13954,12 @@
       <c r="AD56">
         <v>-1</v>
       </c>
+      <c r="AE56">
+        <v>-1</v>
+      </c>
+      <c r="AF56" s="1"/>
     </row>
-    <row r="57" spans="1:30" x14ac:dyDescent="0.45">
+    <row r="57" spans="1:32">
       <c r="A57" t="s">
         <v>55</v>
       </c>
@@ -11863,8 +14050,12 @@
       <c r="AD57">
         <v>-1</v>
       </c>
+      <c r="AE57">
+        <v>0.3755</v>
+      </c>
+      <c r="AF57" s="1"/>
     </row>
-    <row r="58" spans="1:30" x14ac:dyDescent="0.45">
+    <row r="58" spans="1:32">
       <c r="A58" t="s">
         <v>30</v>
       </c>
@@ -11955,8 +14146,12 @@
       <c r="AD58">
         <v>-1</v>
       </c>
+      <c r="AE58">
+        <v>-1</v>
+      </c>
+      <c r="AF58" s="1"/>
     </row>
-    <row r="59" spans="1:30" x14ac:dyDescent="0.45">
+    <row r="59" spans="1:32">
       <c r="A59" t="s">
         <v>80</v>
       </c>
@@ -12047,8 +14242,12 @@
       <c r="AD59">
         <v>-1</v>
       </c>
+      <c r="AE59">
+        <v>-1</v>
+      </c>
+      <c r="AF59" s="1"/>
     </row>
-    <row r="60" spans="1:30" x14ac:dyDescent="0.45">
+    <row r="60" spans="1:32">
       <c r="A60" t="s">
         <v>31</v>
       </c>
@@ -12139,8 +14338,12 @@
       <c r="AD60">
         <v>-1</v>
       </c>
+      <c r="AE60">
+        <v>4.9069000000000003</v>
+      </c>
+      <c r="AF60" s="1"/>
     </row>
-    <row r="61" spans="1:30" x14ac:dyDescent="0.45">
+    <row r="61" spans="1:32">
       <c r="A61" t="s">
         <v>15</v>
       </c>
@@ -12231,8 +14434,12 @@
       <c r="AD61">
         <v>-1</v>
       </c>
+      <c r="AE61">
+        <v>-1</v>
+      </c>
+      <c r="AF61" s="1"/>
     </row>
-    <row r="62" spans="1:30" x14ac:dyDescent="0.45">
+    <row r="62" spans="1:32">
       <c r="A62" t="s">
         <v>39</v>
       </c>
@@ -12323,8 +14530,12 @@
       <c r="AD62">
         <v>2.3797000000000001</v>
       </c>
+      <c r="AE62">
+        <v>-1</v>
+      </c>
+      <c r="AF62" s="1"/>
     </row>
-    <row r="63" spans="1:30" x14ac:dyDescent="0.45">
+    <row r="63" spans="1:32">
       <c r="A63" t="s">
         <v>86</v>
       </c>
@@ -12415,8 +14626,12 @@
       <c r="AD63">
         <v>-1</v>
       </c>
+      <c r="AE63">
+        <v>-1</v>
+      </c>
+      <c r="AF63" s="1"/>
     </row>
-    <row r="64" spans="1:30" x14ac:dyDescent="0.45">
+    <row r="64" spans="1:32">
       <c r="A64" t="s">
         <v>97</v>
       </c>
@@ -12507,8 +14722,12 @@
       <c r="AD64">
         <v>-1</v>
       </c>
+      <c r="AE64">
+        <v>-1</v>
+      </c>
+      <c r="AF64" s="1"/>
     </row>
-    <row r="65" spans="1:30" x14ac:dyDescent="0.45">
+    <row r="65" spans="1:32">
       <c r="A65" t="s">
         <v>65</v>
       </c>
@@ -12599,8 +14818,12 @@
       <c r="AD65">
         <v>-1</v>
       </c>
+      <c r="AE65">
+        <v>-1</v>
+      </c>
+      <c r="AF65" s="1"/>
     </row>
-    <row r="66" spans="1:30" x14ac:dyDescent="0.45">
+    <row r="66" spans="1:32">
       <c r="A66" t="s">
         <v>98</v>
       </c>
@@ -12691,8 +14914,12 @@
       <c r="AD66">
         <v>-1</v>
       </c>
+      <c r="AE66">
+        <v>-1</v>
+      </c>
+      <c r="AF66" s="1"/>
     </row>
-    <row r="67" spans="1:30" x14ac:dyDescent="0.45">
+    <row r="67" spans="1:32">
       <c r="A67" t="s">
         <v>60</v>
       </c>
@@ -12783,8 +15010,12 @@
       <c r="AD67">
         <v>-1</v>
       </c>
+      <c r="AE67">
+        <v>-1</v>
+      </c>
+      <c r="AF67" s="1"/>
     </row>
-    <row r="68" spans="1:30" x14ac:dyDescent="0.45">
+    <row r="68" spans="1:32">
       <c r="A68" t="s">
         <v>77</v>
       </c>
@@ -12875,8 +15106,12 @@
       <c r="AD68">
         <v>-1</v>
       </c>
+      <c r="AE68">
+        <v>-1</v>
+      </c>
+      <c r="AF68" s="1"/>
     </row>
-    <row r="69" spans="1:30" x14ac:dyDescent="0.45">
+    <row r="69" spans="1:32">
       <c r="A69" t="s">
         <v>7</v>
       </c>
@@ -12967,8 +15202,12 @@
       <c r="AD69">
         <v>4.4603000000000002</v>
       </c>
+      <c r="AE69">
+        <v>5.2880000000000003</v>
+      </c>
+      <c r="AF69" s="1"/>
     </row>
-    <row r="70" spans="1:30" x14ac:dyDescent="0.45">
+    <row r="70" spans="1:32">
       <c r="A70" t="s">
         <v>56</v>
       </c>
@@ -13059,8 +15298,12 @@
       <c r="AD70">
         <v>3.9188000000000001</v>
       </c>
+      <c r="AE70">
+        <v>3.5908000000000002</v>
+      </c>
+      <c r="AF70" s="1"/>
     </row>
-    <row r="71" spans="1:30" x14ac:dyDescent="0.45">
+    <row r="71" spans="1:32">
       <c r="A71" t="s">
         <v>75</v>
       </c>
@@ -13151,8 +15394,12 @@
       <c r="AD71">
         <v>-1</v>
       </c>
+      <c r="AE71">
+        <v>-1</v>
+      </c>
+      <c r="AF71" s="1"/>
     </row>
-    <row r="72" spans="1:30" x14ac:dyDescent="0.45">
+    <row r="72" spans="1:32">
       <c r="A72" t="s">
         <v>90</v>
       </c>
@@ -13243,8 +15490,12 @@
       <c r="AD72">
         <v>-1</v>
       </c>
+      <c r="AE72">
+        <v>-1</v>
+      </c>
+      <c r="AF72" s="1"/>
     </row>
-    <row r="73" spans="1:30" x14ac:dyDescent="0.45">
+    <row r="73" spans="1:32">
       <c r="A73" t="s">
         <v>93</v>
       </c>
@@ -13335,8 +15586,12 @@
       <c r="AD73">
         <v>-1</v>
       </c>
+      <c r="AE73">
+        <v>-1</v>
+      </c>
+      <c r="AF73" s="1"/>
     </row>
-    <row r="74" spans="1:30" x14ac:dyDescent="0.45">
+    <row r="74" spans="1:32">
       <c r="A74" t="s">
         <v>78</v>
       </c>
@@ -13427,8 +15682,12 @@
       <c r="AD74">
         <v>-1</v>
       </c>
+      <c r="AE74">
+        <v>-1</v>
+      </c>
+      <c r="AF74" s="1"/>
     </row>
-    <row r="75" spans="1:30" x14ac:dyDescent="0.45">
+    <row r="75" spans="1:32">
       <c r="A75" t="s">
         <v>50</v>
       </c>
@@ -13519,8 +15778,12 @@
       <c r="AD75">
         <v>3.5287000000000002</v>
       </c>
+      <c r="AE75">
+        <v>2.8197999999999999</v>
+      </c>
+      <c r="AF75" s="1"/>
     </row>
-    <row r="76" spans="1:30" x14ac:dyDescent="0.45">
+    <row r="76" spans="1:32">
       <c r="A76" t="s">
         <v>13</v>
       </c>
@@ -13611,8 +15874,12 @@
       <c r="AD76">
         <v>-1</v>
       </c>
+      <c r="AE76">
+        <v>3.2</v>
+      </c>
+      <c r="AF76" s="1"/>
     </row>
-    <row r="77" spans="1:30" x14ac:dyDescent="0.45">
+    <row r="77" spans="1:32">
       <c r="A77" t="s">
         <v>17</v>
       </c>
@@ -13703,8 +15970,12 @@
       <c r="AD77">
         <v>-1</v>
       </c>
+      <c r="AE77">
+        <v>0.33439999999999998</v>
+      </c>
+      <c r="AF77" s="1"/>
     </row>
-    <row r="78" spans="1:30" x14ac:dyDescent="0.45">
+    <row r="78" spans="1:32">
       <c r="A78" t="s">
         <v>46</v>
       </c>
@@ -13795,8 +16066,12 @@
       <c r="AD78">
         <v>-1</v>
       </c>
+      <c r="AE78">
+        <v>3.2894999999999999</v>
+      </c>
+      <c r="AF78" s="1"/>
     </row>
-    <row r="79" spans="1:30" x14ac:dyDescent="0.45">
+    <row r="79" spans="1:32">
       <c r="A79" t="s">
         <v>64</v>
       </c>
@@ -13887,9 +16162,13 @@
       <c r="AD79">
         <v>-1</v>
       </c>
+      <c r="AE79">
+        <v>-1</v>
+      </c>
+      <c r="AF79" s="1"/>
     </row>
   </sheetData>
-  <sortState ref="A2:AD36">
+  <sortState ref="A2:BJ36">
     <sortCondition ref="A2"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -13901,16 +16180,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:U6"/>
   <sheetViews>
-    <sheetView topLeftCell="H1" workbookViewId="0">
-      <selection activeCell="V1" sqref="V1:AV1048576"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="T2" sqref="T2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.65" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="14.65"/>
   <cols>
     <col min="1" max="1" width="18.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:21" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:21">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -13975,7 +16254,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="2" spans="1:21" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:21">
       <c r="A2" t="s">
         <v>5</v>
       </c>
@@ -14040,7 +16319,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="3" spans="1:21" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:21">
       <c r="A3" t="s">
         <v>75</v>
       </c>
@@ -14105,7 +16384,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="4" spans="1:21" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:21">
       <c r="A4" t="s">
         <v>17</v>
       </c>
@@ -14170,7 +16449,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="5" spans="1:21" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:21">
       <c r="A5" t="s">
         <v>88</v>
       </c>
@@ -14235,7 +16514,7 @@
         <v>1.1646000000000001</v>
       </c>
     </row>
-    <row r="6" spans="1:21" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:21">
       <c r="A6" t="s">
         <v>8</v>
       </c>
@@ -14301,7 +16580,7 @@
       </c>
     </row>
   </sheetData>
-  <sortState ref="A2:U3">
+  <sortState ref="A2:Y3">
     <sortCondition ref="A2"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -14313,17 +16592,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:AC17"/>
   <sheetViews>
-    <sheetView topLeftCell="P1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="AE5" sqref="AE5"/>
+    <sheetView topLeftCell="T1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="AE14" sqref="AE14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.65" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="14.65"/>
   <cols>
     <col min="1" max="1" width="18.28515625" customWidth="1"/>
     <col min="20" max="20" width="9.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:29" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:29">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -14412,7 +16691,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="2" spans="1:29" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:29">
       <c r="A2" t="s">
         <v>26</v>
       </c>
@@ -14501,7 +16780,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="3" spans="1:29" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:29">
       <c r="A3" t="s">
         <v>3</v>
       </c>
@@ -14590,7 +16869,7 @@
         <v>4.4462999999999999</v>
       </c>
     </row>
-    <row r="4" spans="1:29" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:29">
       <c r="A4" t="s">
         <v>14</v>
       </c>
@@ -14679,7 +16958,7 @@
         <v>7.1429</v>
       </c>
     </row>
-    <row r="5" spans="1:29" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:29">
       <c r="A5" t="s">
         <v>4</v>
       </c>
@@ -14768,7 +17047,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="6" spans="1:29" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:29">
       <c r="A6" t="s">
         <v>9</v>
       </c>
@@ -14857,7 +17136,7 @@
         <v>5.2477999999999998</v>
       </c>
     </row>
-    <row r="7" spans="1:29" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:29">
       <c r="A7" t="s">
         <v>1</v>
       </c>
@@ -14946,7 +17225,7 @@
         <v>6.5517000000000003</v>
       </c>
     </row>
-    <row r="8" spans="1:29" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:29">
       <c r="A8" t="s">
         <v>71</v>
       </c>
@@ -15035,7 +17314,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="9" spans="1:29" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:29">
       <c r="A9" t="s">
         <v>29</v>
       </c>
@@ -15124,7 +17403,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="10" spans="1:29" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:29">
       <c r="A10" t="s">
         <v>54</v>
       </c>
@@ -15213,7 +17492,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="11" spans="1:29" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:29">
       <c r="A11" t="s">
         <v>52</v>
       </c>
@@ -15302,7 +17581,7 @@
         <v>1.7722</v>
       </c>
     </row>
-    <row r="12" spans="1:29" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:29">
       <c r="A12" t="s">
         <v>62</v>
       </c>
@@ -15391,7 +17670,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="13" spans="1:29" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:29">
       <c r="A13" t="s">
         <v>12</v>
       </c>
@@ -15480,7 +17759,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="14" spans="1:29" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:29">
       <c r="A14" t="s">
         <v>84</v>
       </c>
@@ -15569,7 +17848,7 @@
         <v>2.4965000000000002</v>
       </c>
     </row>
-    <row r="15" spans="1:29" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:29">
       <c r="A15" t="s">
         <v>8</v>
       </c>
@@ -15658,7 +17937,7 @@
         <v>4.3724999999999996</v>
       </c>
     </row>
-    <row r="16" spans="1:29" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:29">
       <c r="A16" t="s">
         <v>86</v>
       </c>
@@ -15747,7 +18026,7 @@
         <v>5.4526000000000003</v>
       </c>
     </row>
-    <row r="17" spans="1:29" x14ac:dyDescent="0.45">
+    <row r="17" spans="1:29">
       <c r="A17" t="s">
         <v>7</v>
       </c>
@@ -15849,16 +18128,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:AD8"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="Q1" workbookViewId="0">
-      <selection activeCell="AE1" sqref="AE1:BN1048576"/>
+    <sheetView tabSelected="1" topLeftCell="P1" workbookViewId="0">
+      <selection activeCell="AA2" sqref="AA2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.65" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="14.65"/>
   <cols>
     <col min="1" max="1" width="18.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:30" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:30">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -15950,7 +18229,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="2" spans="1:30" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:30">
       <c r="A2" t="s">
         <v>5</v>
       </c>
@@ -16042,7 +18321,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="3" spans="1:30" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:30">
       <c r="A3" t="s">
         <v>9</v>
       </c>
@@ -16134,7 +18413,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="4" spans="1:30" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:30">
       <c r="A4" t="s">
         <v>1</v>
       </c>
@@ -16226,7 +18505,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="5" spans="1:30" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:30">
       <c r="A5" t="s">
         <v>29</v>
       </c>
@@ -16318,7 +18597,7 @@
         <v>4.2878999999999996</v>
       </c>
     </row>
-    <row r="6" spans="1:30" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:30">
       <c r="A6" t="s">
         <v>15</v>
       </c>
@@ -16410,7 +18689,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:30" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:30">
       <c r="A7" t="s">
         <v>61</v>
       </c>
@@ -16502,7 +18781,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="8" spans="1:30" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:30">
       <c r="A8" t="s">
         <v>62</v>
       </c>

</xml_diff>

<commit_message>
Last fixed. Application done!
</commit_message>
<xml_diff>
--- a/ExcelDataImport/ranking_data.xlsx
+++ b/ExcelDataImport/ranking_data.xlsx
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="172" uniqueCount="99">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="172" uniqueCount="98">
   <si>
     <t>Nimi</t>
   </si>
@@ -107,9 +107,6 @@
   </si>
   <si>
     <t>Antti Otsamo</t>
-  </si>
-  <si>
-    <t>Hans Sandval</t>
   </si>
   <si>
     <t>Juha Hokkanen</t>
@@ -326,13 +323,22 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="0.0000"/>
+  </numFmts>
+  <fonts count="2">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Arial Unicode MS"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -355,8 +361,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normaali" xfId="0" builtinId="0"/>
@@ -695,19 +703,23 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AE62"/>
+  <dimension ref="A1:BP62"/>
   <sheetViews>
-    <sheetView topLeftCell="R1" workbookViewId="0">
-      <selection activeCell="AF1" sqref="AF1:BP1048576"/>
+    <sheetView topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="A18" sqref="A18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.65" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="14.65"/>
   <cols>
     <col min="1" max="1" width="18.28515625" customWidth="1"/>
     <col min="2" max="31" width="9.140625" customWidth="1"/>
+    <col min="33" max="33" width="18.28515625" customWidth="1"/>
+    <col min="34" max="34" width="4.42578125" customWidth="1"/>
+    <col min="35" max="35" width="3.28515625" customWidth="1"/>
+    <col min="36" max="36" width="4" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:31" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:68">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -802,9 +814,9 @@
         <v>13</v>
       </c>
     </row>
-    <row r="2" spans="1:31" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:68">
       <c r="A2" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B2">
         <v>-1</v>
@@ -896,8 +908,40 @@
       <c r="AE2">
         <v>-1</v>
       </c>
+      <c r="AF2" s="1"/>
+      <c r="AK2" s="2"/>
+      <c r="AL2" s="2"/>
+      <c r="AM2" s="2"/>
+      <c r="AN2" s="2"/>
+      <c r="AO2" s="2"/>
+      <c r="AP2" s="2"/>
+      <c r="AQ2" s="2"/>
+      <c r="AR2" s="2"/>
+      <c r="AS2" s="2"/>
+      <c r="AT2" s="2"/>
+      <c r="AU2" s="2"/>
+      <c r="AV2" s="2"/>
+      <c r="AW2" s="2"/>
+      <c r="AX2" s="2"/>
+      <c r="AY2" s="2"/>
+      <c r="AZ2" s="2"/>
+      <c r="BA2" s="2"/>
+      <c r="BB2" s="2"/>
+      <c r="BC2" s="2"/>
+      <c r="BD2" s="2"/>
+      <c r="BE2" s="2"/>
+      <c r="BF2" s="2"/>
+      <c r="BG2" s="2"/>
+      <c r="BH2" s="2"/>
+      <c r="BI2" s="2"/>
+      <c r="BJ2" s="2"/>
+      <c r="BK2" s="2"/>
+      <c r="BL2" s="2"/>
+      <c r="BM2" s="2"/>
+      <c r="BN2" s="2"/>
+      <c r="BP2" s="2"/>
     </row>
-    <row r="3" spans="1:31" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:68">
       <c r="A3" t="s">
         <v>26</v>
       </c>
@@ -991,8 +1035,40 @@
       <c r="AE3">
         <v>4.3693999999999997</v>
       </c>
+      <c r="AF3" s="1"/>
+      <c r="AK3" s="2"/>
+      <c r="AL3" s="2"/>
+      <c r="AM3" s="2"/>
+      <c r="AN3" s="2"/>
+      <c r="AO3" s="2"/>
+      <c r="AP3" s="2"/>
+      <c r="AQ3" s="2"/>
+      <c r="AR3" s="2"/>
+      <c r="AS3" s="2"/>
+      <c r="AT3" s="2"/>
+      <c r="AU3" s="2"/>
+      <c r="AV3" s="2"/>
+      <c r="AW3" s="2"/>
+      <c r="AX3" s="2"/>
+      <c r="AY3" s="2"/>
+      <c r="AZ3" s="2"/>
+      <c r="BA3" s="2"/>
+      <c r="BB3" s="2"/>
+      <c r="BC3" s="2"/>
+      <c r="BD3" s="2"/>
+      <c r="BE3" s="2"/>
+      <c r="BF3" s="2"/>
+      <c r="BG3" s="2"/>
+      <c r="BH3" s="2"/>
+      <c r="BI3" s="2"/>
+      <c r="BJ3" s="2"/>
+      <c r="BK3" s="2"/>
+      <c r="BL3" s="2"/>
+      <c r="BM3" s="2"/>
+      <c r="BN3" s="2"/>
+      <c r="BP3" s="2"/>
     </row>
-    <row r="4" spans="1:31" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:68">
       <c r="A4" t="s">
         <v>5</v>
       </c>
@@ -1086,10 +1162,42 @@
       <c r="AE4">
         <v>4.6889000000000003</v>
       </c>
+      <c r="AF4" s="1"/>
+      <c r="AK4" s="2"/>
+      <c r="AL4" s="2"/>
+      <c r="AM4" s="2"/>
+      <c r="AN4" s="2"/>
+      <c r="AO4" s="2"/>
+      <c r="AP4" s="2"/>
+      <c r="AQ4" s="2"/>
+      <c r="AR4" s="2"/>
+      <c r="AS4" s="2"/>
+      <c r="AT4" s="2"/>
+      <c r="AU4" s="2"/>
+      <c r="AV4" s="2"/>
+      <c r="AW4" s="2"/>
+      <c r="AX4" s="2"/>
+      <c r="AY4" s="2"/>
+      <c r="AZ4" s="2"/>
+      <c r="BA4" s="2"/>
+      <c r="BB4" s="2"/>
+      <c r="BC4" s="2"/>
+      <c r="BD4" s="2"/>
+      <c r="BE4" s="2"/>
+      <c r="BF4" s="2"/>
+      <c r="BG4" s="2"/>
+      <c r="BH4" s="2"/>
+      <c r="BI4" s="2"/>
+      <c r="BJ4" s="2"/>
+      <c r="BK4" s="2"/>
+      <c r="BL4" s="2"/>
+      <c r="BM4" s="2"/>
+      <c r="BN4" s="2"/>
+      <c r="BP4" s="2"/>
     </row>
-    <row r="5" spans="1:31" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:68">
       <c r="A5" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B5">
         <v>1.1813</v>
@@ -1181,10 +1289,42 @@
       <c r="AE5">
         <v>4.2220000000000004</v>
       </c>
+      <c r="AF5" s="1"/>
+      <c r="AK5" s="2"/>
+      <c r="AL5" s="2"/>
+      <c r="AM5" s="2"/>
+      <c r="AN5" s="2"/>
+      <c r="AO5" s="2"/>
+      <c r="AP5" s="2"/>
+      <c r="AQ5" s="2"/>
+      <c r="AR5" s="2"/>
+      <c r="AS5" s="2"/>
+      <c r="AT5" s="2"/>
+      <c r="AU5" s="2"/>
+      <c r="AV5" s="2"/>
+      <c r="AW5" s="2"/>
+      <c r="AX5" s="2"/>
+      <c r="AY5" s="2"/>
+      <c r="AZ5" s="2"/>
+      <c r="BA5" s="2"/>
+      <c r="BB5" s="2"/>
+      <c r="BC5" s="2"/>
+      <c r="BD5" s="2"/>
+      <c r="BE5" s="2"/>
+      <c r="BF5" s="2"/>
+      <c r="BG5" s="2"/>
+      <c r="BH5" s="2"/>
+      <c r="BI5" s="2"/>
+      <c r="BJ5" s="2"/>
+      <c r="BK5" s="2"/>
+      <c r="BL5" s="2"/>
+      <c r="BM5" s="2"/>
+      <c r="BN5" s="2"/>
+      <c r="BP5" s="2"/>
     </row>
-    <row r="6" spans="1:31" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:68">
       <c r="A6" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B6">
         <v>-1</v>
@@ -1276,10 +1416,42 @@
       <c r="AE6">
         <v>-1</v>
       </c>
+      <c r="AF6" s="1"/>
+      <c r="AK6" s="2"/>
+      <c r="AL6" s="2"/>
+      <c r="AM6" s="2"/>
+      <c r="AN6" s="2"/>
+      <c r="AO6" s="2"/>
+      <c r="AP6" s="2"/>
+      <c r="AQ6" s="2"/>
+      <c r="AR6" s="2"/>
+      <c r="AS6" s="2"/>
+      <c r="AT6" s="2"/>
+      <c r="AU6" s="2"/>
+      <c r="AV6" s="2"/>
+      <c r="AW6" s="2"/>
+      <c r="AX6" s="2"/>
+      <c r="AY6" s="2"/>
+      <c r="AZ6" s="2"/>
+      <c r="BA6" s="2"/>
+      <c r="BB6" s="2"/>
+      <c r="BC6" s="2"/>
+      <c r="BD6" s="2"/>
+      <c r="BE6" s="2"/>
+      <c r="BF6" s="2"/>
+      <c r="BG6" s="2"/>
+      <c r="BH6" s="2"/>
+      <c r="BI6" s="2"/>
+      <c r="BJ6" s="2"/>
+      <c r="BK6" s="2"/>
+      <c r="BL6" s="2"/>
+      <c r="BM6" s="2"/>
+      <c r="BN6" s="2"/>
+      <c r="BP6" s="2"/>
     </row>
-    <row r="7" spans="1:31" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:68">
       <c r="A7" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B7">
         <v>-1</v>
@@ -1371,10 +1543,42 @@
       <c r="AE7">
         <v>3.7410000000000001</v>
       </c>
+      <c r="AF7" s="1"/>
+      <c r="AK7" s="2"/>
+      <c r="AL7" s="2"/>
+      <c r="AM7" s="2"/>
+      <c r="AN7" s="2"/>
+      <c r="AO7" s="2"/>
+      <c r="AP7" s="2"/>
+      <c r="AQ7" s="2"/>
+      <c r="AR7" s="2"/>
+      <c r="AS7" s="2"/>
+      <c r="AT7" s="2"/>
+      <c r="AU7" s="2"/>
+      <c r="AV7" s="2"/>
+      <c r="AW7" s="2"/>
+      <c r="AX7" s="2"/>
+      <c r="AY7" s="2"/>
+      <c r="AZ7" s="2"/>
+      <c r="BA7" s="2"/>
+      <c r="BB7" s="2"/>
+      <c r="BC7" s="2"/>
+      <c r="BD7" s="2"/>
+      <c r="BE7" s="2"/>
+      <c r="BF7" s="2"/>
+      <c r="BG7" s="2"/>
+      <c r="BH7" s="2"/>
+      <c r="BI7" s="2"/>
+      <c r="BJ7" s="2"/>
+      <c r="BK7" s="2"/>
+      <c r="BL7" s="2"/>
+      <c r="BM7" s="2"/>
+      <c r="BN7" s="2"/>
+      <c r="BP7" s="2"/>
     </row>
-    <row r="8" spans="1:31" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:68">
       <c r="A8" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B8">
         <v>0.78669999999999995</v>
@@ -1466,8 +1670,40 @@
       <c r="AE8">
         <v>-1</v>
       </c>
+      <c r="AF8" s="1"/>
+      <c r="AK8" s="2"/>
+      <c r="AL8" s="2"/>
+      <c r="AM8" s="2"/>
+      <c r="AN8" s="2"/>
+      <c r="AO8" s="2"/>
+      <c r="AP8" s="2"/>
+      <c r="AQ8" s="2"/>
+      <c r="AR8" s="2"/>
+      <c r="AS8" s="2"/>
+      <c r="AT8" s="2"/>
+      <c r="AU8" s="2"/>
+      <c r="AV8" s="2"/>
+      <c r="AW8" s="2"/>
+      <c r="AX8" s="2"/>
+      <c r="AY8" s="2"/>
+      <c r="AZ8" s="2"/>
+      <c r="BA8" s="2"/>
+      <c r="BB8" s="2"/>
+      <c r="BC8" s="2"/>
+      <c r="BD8" s="2"/>
+      <c r="BE8" s="2"/>
+      <c r="BF8" s="2"/>
+      <c r="BG8" s="2"/>
+      <c r="BH8" s="2"/>
+      <c r="BI8" s="2"/>
+      <c r="BJ8" s="2"/>
+      <c r="BK8" s="2"/>
+      <c r="BL8" s="2"/>
+      <c r="BM8" s="2"/>
+      <c r="BN8" s="2"/>
+      <c r="BP8" s="2"/>
     </row>
-    <row r="9" spans="1:31" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:68">
       <c r="A9" t="s">
         <v>27</v>
       </c>
@@ -1561,10 +1797,42 @@
       <c r="AE9">
         <v>-1</v>
       </c>
+      <c r="AF9" s="1"/>
+      <c r="AK9" s="2"/>
+      <c r="AL9" s="2"/>
+      <c r="AM9" s="2"/>
+      <c r="AN9" s="2"/>
+      <c r="AO9" s="2"/>
+      <c r="AP9" s="2"/>
+      <c r="AQ9" s="2"/>
+      <c r="AR9" s="2"/>
+      <c r="AS9" s="2"/>
+      <c r="AT9" s="2"/>
+      <c r="AU9" s="2"/>
+      <c r="AV9" s="2"/>
+      <c r="AW9" s="2"/>
+      <c r="AX9" s="2"/>
+      <c r="AY9" s="2"/>
+      <c r="AZ9" s="2"/>
+      <c r="BA9" s="2"/>
+      <c r="BB9" s="2"/>
+      <c r="BC9" s="2"/>
+      <c r="BD9" s="2"/>
+      <c r="BE9" s="2"/>
+      <c r="BF9" s="2"/>
+      <c r="BG9" s="2"/>
+      <c r="BH9" s="2"/>
+      <c r="BI9" s="2"/>
+      <c r="BJ9" s="2"/>
+      <c r="BK9" s="2"/>
+      <c r="BL9" s="2"/>
+      <c r="BM9" s="2"/>
+      <c r="BN9" s="2"/>
+      <c r="BP9" s="2"/>
     </row>
-    <row r="10" spans="1:31" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:68">
       <c r="A10" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B10">
         <v>-1</v>
@@ -1656,10 +1924,42 @@
       <c r="AE10">
         <v>6.8044000000000002</v>
       </c>
+      <c r="AF10" s="1"/>
+      <c r="AK10" s="2"/>
+      <c r="AL10" s="2"/>
+      <c r="AM10" s="2"/>
+      <c r="AN10" s="2"/>
+      <c r="AO10" s="2"/>
+      <c r="AP10" s="2"/>
+      <c r="AQ10" s="2"/>
+      <c r="AR10" s="2"/>
+      <c r="AS10" s="2"/>
+      <c r="AT10" s="2"/>
+      <c r="AU10" s="2"/>
+      <c r="AV10" s="2"/>
+      <c r="AW10" s="2"/>
+      <c r="AX10" s="2"/>
+      <c r="AY10" s="2"/>
+      <c r="AZ10" s="2"/>
+      <c r="BA10" s="2"/>
+      <c r="BB10" s="2"/>
+      <c r="BC10" s="2"/>
+      <c r="BD10" s="2"/>
+      <c r="BE10" s="2"/>
+      <c r="BF10" s="2"/>
+      <c r="BG10" s="2"/>
+      <c r="BH10" s="2"/>
+      <c r="BI10" s="2"/>
+      <c r="BJ10" s="2"/>
+      <c r="BK10" s="2"/>
+      <c r="BL10" s="2"/>
+      <c r="BM10" s="2"/>
+      <c r="BN10" s="2"/>
+      <c r="BP10" s="2"/>
     </row>
-    <row r="11" spans="1:31" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:68">
       <c r="A11" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B11">
         <v>-1</v>
@@ -1751,10 +2051,42 @@
       <c r="AE11">
         <v>5.1546000000000003</v>
       </c>
+      <c r="AF11" s="1"/>
+      <c r="AK11" s="2"/>
+      <c r="AL11" s="2"/>
+      <c r="AM11" s="2"/>
+      <c r="AN11" s="2"/>
+      <c r="AO11" s="2"/>
+      <c r="AP11" s="2"/>
+      <c r="AQ11" s="2"/>
+      <c r="AR11" s="2"/>
+      <c r="AS11" s="2"/>
+      <c r="AT11" s="2"/>
+      <c r="AU11" s="2"/>
+      <c r="AV11" s="2"/>
+      <c r="AW11" s="2"/>
+      <c r="AX11" s="2"/>
+      <c r="AY11" s="2"/>
+      <c r="AZ11" s="2"/>
+      <c r="BA11" s="2"/>
+      <c r="BB11" s="2"/>
+      <c r="BC11" s="2"/>
+      <c r="BD11" s="2"/>
+      <c r="BE11" s="2"/>
+      <c r="BF11" s="2"/>
+      <c r="BG11" s="2"/>
+      <c r="BH11" s="2"/>
+      <c r="BI11" s="2"/>
+      <c r="BJ11" s="2"/>
+      <c r="BK11" s="2"/>
+      <c r="BL11" s="2"/>
+      <c r="BM11" s="2"/>
+      <c r="BN11" s="2"/>
+      <c r="BP11" s="2"/>
     </row>
-    <row r="12" spans="1:31" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:68">
       <c r="A12" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B12">
         <v>-1</v>
@@ -1846,8 +2178,40 @@
       <c r="AE12">
         <v>4.0728999999999997</v>
       </c>
+      <c r="AF12" s="1"/>
+      <c r="AK12" s="2"/>
+      <c r="AL12" s="2"/>
+      <c r="AM12" s="2"/>
+      <c r="AN12" s="2"/>
+      <c r="AO12" s="2"/>
+      <c r="AP12" s="2"/>
+      <c r="AQ12" s="2"/>
+      <c r="AR12" s="2"/>
+      <c r="AS12" s="2"/>
+      <c r="AT12" s="2"/>
+      <c r="AU12" s="2"/>
+      <c r="AV12" s="2"/>
+      <c r="AW12" s="2"/>
+      <c r="AX12" s="2"/>
+      <c r="AY12" s="2"/>
+      <c r="AZ12" s="2"/>
+      <c r="BA12" s="2"/>
+      <c r="BB12" s="2"/>
+      <c r="BC12" s="2"/>
+      <c r="BD12" s="2"/>
+      <c r="BE12" s="2"/>
+      <c r="BF12" s="2"/>
+      <c r="BG12" s="2"/>
+      <c r="BH12" s="2"/>
+      <c r="BI12" s="2"/>
+      <c r="BJ12" s="2"/>
+      <c r="BK12" s="2"/>
+      <c r="BL12" s="2"/>
+      <c r="BM12" s="2"/>
+      <c r="BN12" s="2"/>
+      <c r="BP12" s="2"/>
     </row>
-    <row r="13" spans="1:31" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:68">
       <c r="A13" t="s">
         <v>18</v>
       </c>
@@ -1941,8 +2305,40 @@
       <c r="AE13">
         <v>0</v>
       </c>
+      <c r="AF13" s="1"/>
+      <c r="AK13" s="2"/>
+      <c r="AL13" s="2"/>
+      <c r="AM13" s="2"/>
+      <c r="AN13" s="2"/>
+      <c r="AO13" s="2"/>
+      <c r="AP13" s="2"/>
+      <c r="AQ13" s="2"/>
+      <c r="AR13" s="2"/>
+      <c r="AS13" s="2"/>
+      <c r="AT13" s="2"/>
+      <c r="AU13" s="2"/>
+      <c r="AV13" s="2"/>
+      <c r="AW13" s="2"/>
+      <c r="AX13" s="2"/>
+      <c r="AY13" s="2"/>
+      <c r="AZ13" s="2"/>
+      <c r="BA13" s="2"/>
+      <c r="BB13" s="2"/>
+      <c r="BC13" s="2"/>
+      <c r="BD13" s="2"/>
+      <c r="BE13" s="2"/>
+      <c r="BF13" s="2"/>
+      <c r="BG13" s="2"/>
+      <c r="BH13" s="2"/>
+      <c r="BI13" s="2"/>
+      <c r="BJ13" s="2"/>
+      <c r="BK13" s="2"/>
+      <c r="BL13" s="2"/>
+      <c r="BM13" s="2"/>
+      <c r="BN13" s="2"/>
+      <c r="BP13" s="2"/>
     </row>
-    <row r="14" spans="1:31" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:68">
       <c r="A14" t="s">
         <v>3</v>
       </c>
@@ -2036,8 +2432,40 @@
       <c r="AE14">
         <v>4.5494000000000003</v>
       </c>
+      <c r="AF14" s="1"/>
+      <c r="AK14" s="2"/>
+      <c r="AL14" s="2"/>
+      <c r="AM14" s="2"/>
+      <c r="AN14" s="2"/>
+      <c r="AO14" s="2"/>
+      <c r="AP14" s="2"/>
+      <c r="AQ14" s="2"/>
+      <c r="AR14" s="2"/>
+      <c r="AS14" s="2"/>
+      <c r="AT14" s="2"/>
+      <c r="AU14" s="2"/>
+      <c r="AV14" s="2"/>
+      <c r="AW14" s="2"/>
+      <c r="AX14" s="2"/>
+      <c r="AY14" s="2"/>
+      <c r="AZ14" s="2"/>
+      <c r="BA14" s="2"/>
+      <c r="BB14" s="2"/>
+      <c r="BC14" s="2"/>
+      <c r="BD14" s="2"/>
+      <c r="BE14" s="2"/>
+      <c r="BF14" s="2"/>
+      <c r="BG14" s="2"/>
+      <c r="BH14" s="2"/>
+      <c r="BI14" s="2"/>
+      <c r="BJ14" s="2"/>
+      <c r="BK14" s="2"/>
+      <c r="BL14" s="2"/>
+      <c r="BM14" s="2"/>
+      <c r="BN14" s="2"/>
+      <c r="BP14" s="2"/>
     </row>
-    <row r="15" spans="1:31" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:68">
       <c r="A15" t="s">
         <v>14</v>
       </c>
@@ -2131,10 +2559,42 @@
       <c r="AE15">
         <v>-1</v>
       </c>
+      <c r="AF15" s="1"/>
+      <c r="AK15" s="2"/>
+      <c r="AL15" s="2"/>
+      <c r="AM15" s="2"/>
+      <c r="AN15" s="2"/>
+      <c r="AO15" s="2"/>
+      <c r="AP15" s="2"/>
+      <c r="AQ15" s="2"/>
+      <c r="AR15" s="2"/>
+      <c r="AS15" s="2"/>
+      <c r="AT15" s="2"/>
+      <c r="AU15" s="2"/>
+      <c r="AV15" s="2"/>
+      <c r="AW15" s="2"/>
+      <c r="AX15" s="2"/>
+      <c r="AY15" s="2"/>
+      <c r="AZ15" s="2"/>
+      <c r="BA15" s="2"/>
+      <c r="BB15" s="2"/>
+      <c r="BC15" s="2"/>
+      <c r="BD15" s="2"/>
+      <c r="BE15" s="2"/>
+      <c r="BF15" s="2"/>
+      <c r="BG15" s="2"/>
+      <c r="BH15" s="2"/>
+      <c r="BI15" s="2"/>
+      <c r="BJ15" s="2"/>
+      <c r="BK15" s="2"/>
+      <c r="BL15" s="2"/>
+      <c r="BM15" s="2"/>
+      <c r="BN15" s="2"/>
+      <c r="BP15" s="2"/>
     </row>
-    <row r="16" spans="1:31" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:68">
       <c r="A16" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B16">
         <v>-1</v>
@@ -2226,8 +2686,40 @@
       <c r="AE16">
         <v>-1</v>
       </c>
+      <c r="AF16" s="1"/>
+      <c r="AK16" s="2"/>
+      <c r="AL16" s="2"/>
+      <c r="AM16" s="2"/>
+      <c r="AN16" s="2"/>
+      <c r="AO16" s="2"/>
+      <c r="AP16" s="2"/>
+      <c r="AQ16" s="2"/>
+      <c r="AR16" s="2"/>
+      <c r="AS16" s="2"/>
+      <c r="AT16" s="2"/>
+      <c r="AU16" s="2"/>
+      <c r="AV16" s="2"/>
+      <c r="AW16" s="2"/>
+      <c r="AX16" s="2"/>
+      <c r="AY16" s="2"/>
+      <c r="AZ16" s="2"/>
+      <c r="BA16" s="2"/>
+      <c r="BB16" s="2"/>
+      <c r="BC16" s="2"/>
+      <c r="BD16" s="2"/>
+      <c r="BE16" s="2"/>
+      <c r="BF16" s="2"/>
+      <c r="BG16" s="2"/>
+      <c r="BH16" s="2"/>
+      <c r="BI16" s="2"/>
+      <c r="BJ16" s="2"/>
+      <c r="BK16" s="2"/>
+      <c r="BL16" s="2"/>
+      <c r="BM16" s="2"/>
+      <c r="BN16" s="2"/>
+      <c r="BP16" s="2"/>
     </row>
-    <row r="17" spans="1:31" x14ac:dyDescent="0.45">
+    <row r="17" spans="1:68">
       <c r="A17" t="s">
         <v>4</v>
       </c>
@@ -2321,8 +2813,40 @@
       <c r="AE17">
         <v>5.1177000000000001</v>
       </c>
+      <c r="AF17" s="1"/>
+      <c r="AK17" s="2"/>
+      <c r="AL17" s="2"/>
+      <c r="AM17" s="2"/>
+      <c r="AN17" s="2"/>
+      <c r="AO17" s="2"/>
+      <c r="AP17" s="2"/>
+      <c r="AQ17" s="2"/>
+      <c r="AR17" s="2"/>
+      <c r="AS17" s="2"/>
+      <c r="AT17" s="2"/>
+      <c r="AU17" s="2"/>
+      <c r="AV17" s="2"/>
+      <c r="AW17" s="2"/>
+      <c r="AX17" s="2"/>
+      <c r="AY17" s="2"/>
+      <c r="AZ17" s="2"/>
+      <c r="BA17" s="2"/>
+      <c r="BB17" s="2"/>
+      <c r="BC17" s="2"/>
+      <c r="BD17" s="2"/>
+      <c r="BE17" s="2"/>
+      <c r="BF17" s="2"/>
+      <c r="BG17" s="2"/>
+      <c r="BH17" s="2"/>
+      <c r="BI17" s="2"/>
+      <c r="BJ17" s="2"/>
+      <c r="BK17" s="2"/>
+      <c r="BL17" s="2"/>
+      <c r="BM17" s="2"/>
+      <c r="BN17" s="2"/>
+      <c r="BP17" s="2"/>
     </row>
-    <row r="18" spans="1:31" x14ac:dyDescent="0.45">
+    <row r="18" spans="1:68">
       <c r="A18" t="s">
         <v>10</v>
       </c>
@@ -2416,8 +2940,40 @@
       <c r="AE18">
         <v>2.0846</v>
       </c>
+      <c r="AF18" s="1"/>
+      <c r="AK18" s="2"/>
+      <c r="AL18" s="2"/>
+      <c r="AM18" s="2"/>
+      <c r="AN18" s="2"/>
+      <c r="AO18" s="2"/>
+      <c r="AP18" s="2"/>
+      <c r="AQ18" s="2"/>
+      <c r="AR18" s="2"/>
+      <c r="AS18" s="2"/>
+      <c r="AT18" s="2"/>
+      <c r="AU18" s="2"/>
+      <c r="AV18" s="2"/>
+      <c r="AW18" s="2"/>
+      <c r="AX18" s="2"/>
+      <c r="AY18" s="2"/>
+      <c r="AZ18" s="2"/>
+      <c r="BA18" s="2"/>
+      <c r="BB18" s="2"/>
+      <c r="BC18" s="2"/>
+      <c r="BD18" s="2"/>
+      <c r="BE18" s="2"/>
+      <c r="BF18" s="2"/>
+      <c r="BG18" s="2"/>
+      <c r="BH18" s="2"/>
+      <c r="BI18" s="2"/>
+      <c r="BJ18" s="2"/>
+      <c r="BK18" s="2"/>
+      <c r="BL18" s="2"/>
+      <c r="BM18" s="2"/>
+      <c r="BN18" s="2"/>
+      <c r="BP18" s="2"/>
     </row>
-    <row r="19" spans="1:31" x14ac:dyDescent="0.45">
+    <row r="19" spans="1:68">
       <c r="A19" t="s">
         <v>9</v>
       </c>
@@ -2511,8 +3067,40 @@
       <c r="AE19">
         <v>2.6187999999999998</v>
       </c>
+      <c r="AF19" s="1"/>
+      <c r="AK19" s="2"/>
+      <c r="AL19" s="2"/>
+      <c r="AM19" s="2"/>
+      <c r="AN19" s="2"/>
+      <c r="AO19" s="2"/>
+      <c r="AP19" s="2"/>
+      <c r="AQ19" s="2"/>
+      <c r="AR19" s="2"/>
+      <c r="AS19" s="2"/>
+      <c r="AT19" s="2"/>
+      <c r="AU19" s="2"/>
+      <c r="AV19" s="2"/>
+      <c r="AW19" s="2"/>
+      <c r="AX19" s="2"/>
+      <c r="AY19" s="2"/>
+      <c r="AZ19" s="2"/>
+      <c r="BA19" s="2"/>
+      <c r="BB19" s="2"/>
+      <c r="BC19" s="2"/>
+      <c r="BD19" s="2"/>
+      <c r="BE19" s="2"/>
+      <c r="BF19" s="2"/>
+      <c r="BG19" s="2"/>
+      <c r="BH19" s="2"/>
+      <c r="BI19" s="2"/>
+      <c r="BJ19" s="2"/>
+      <c r="BK19" s="2"/>
+      <c r="BL19" s="2"/>
+      <c r="BM19" s="2"/>
+      <c r="BN19" s="2"/>
+      <c r="BP19" s="2"/>
     </row>
-    <row r="20" spans="1:31" x14ac:dyDescent="0.45">
+    <row r="20" spans="1:68">
       <c r="A20" t="s">
         <v>16</v>
       </c>
@@ -2606,10 +3194,42 @@
       <c r="AE20">
         <v>-1</v>
       </c>
+      <c r="AF20" s="1"/>
+      <c r="AK20" s="2"/>
+      <c r="AL20" s="2"/>
+      <c r="AM20" s="2"/>
+      <c r="AN20" s="2"/>
+      <c r="AO20" s="2"/>
+      <c r="AP20" s="2"/>
+      <c r="AQ20" s="2"/>
+      <c r="AR20" s="2"/>
+      <c r="AS20" s="2"/>
+      <c r="AT20" s="2"/>
+      <c r="AU20" s="2"/>
+      <c r="AV20" s="2"/>
+      <c r="AW20" s="2"/>
+      <c r="AX20" s="2"/>
+      <c r="AY20" s="2"/>
+      <c r="AZ20" s="2"/>
+      <c r="BA20" s="2"/>
+      <c r="BB20" s="2"/>
+      <c r="BC20" s="2"/>
+      <c r="BD20" s="2"/>
+      <c r="BE20" s="2"/>
+      <c r="BF20" s="2"/>
+      <c r="BG20" s="2"/>
+      <c r="BH20" s="2"/>
+      <c r="BI20" s="2"/>
+      <c r="BJ20" s="2"/>
+      <c r="BK20" s="2"/>
+      <c r="BL20" s="2"/>
+      <c r="BM20" s="2"/>
+      <c r="BN20" s="2"/>
+      <c r="BP20" s="2"/>
     </row>
-    <row r="21" spans="1:31" x14ac:dyDescent="0.45">
+    <row r="21" spans="1:68">
       <c r="A21" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B21">
         <v>-1</v>
@@ -2701,10 +3321,42 @@
       <c r="AE21">
         <v>3.6817000000000002</v>
       </c>
+      <c r="AF21" s="1"/>
+      <c r="AK21" s="2"/>
+      <c r="AL21" s="2"/>
+      <c r="AM21" s="2"/>
+      <c r="AN21" s="2"/>
+      <c r="AO21" s="2"/>
+      <c r="AP21" s="2"/>
+      <c r="AQ21" s="2"/>
+      <c r="AR21" s="2"/>
+      <c r="AS21" s="2"/>
+      <c r="AT21" s="2"/>
+      <c r="AU21" s="2"/>
+      <c r="AV21" s="2"/>
+      <c r="AW21" s="2"/>
+      <c r="AX21" s="2"/>
+      <c r="AY21" s="2"/>
+      <c r="AZ21" s="2"/>
+      <c r="BA21" s="2"/>
+      <c r="BB21" s="2"/>
+      <c r="BC21" s="2"/>
+      <c r="BD21" s="2"/>
+      <c r="BE21" s="2"/>
+      <c r="BF21" s="2"/>
+      <c r="BG21" s="2"/>
+      <c r="BH21" s="2"/>
+      <c r="BI21" s="2"/>
+      <c r="BJ21" s="2"/>
+      <c r="BK21" s="2"/>
+      <c r="BL21" s="2"/>
+      <c r="BM21" s="2"/>
+      <c r="BN21" s="2"/>
+      <c r="BP21" s="2"/>
     </row>
-    <row r="22" spans="1:31" x14ac:dyDescent="0.45">
+    <row r="22" spans="1:68">
       <c r="A22" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B22">
         <v>-1</v>
@@ -2796,8 +3448,40 @@
       <c r="AE22">
         <v>4.5627000000000004</v>
       </c>
+      <c r="AF22" s="1"/>
+      <c r="AK22" s="2"/>
+      <c r="AL22" s="2"/>
+      <c r="AM22" s="2"/>
+      <c r="AN22" s="2"/>
+      <c r="AO22" s="2"/>
+      <c r="AP22" s="2"/>
+      <c r="AQ22" s="2"/>
+      <c r="AR22" s="2"/>
+      <c r="AS22" s="2"/>
+      <c r="AT22" s="2"/>
+      <c r="AU22" s="2"/>
+      <c r="AV22" s="2"/>
+      <c r="AW22" s="2"/>
+      <c r="AX22" s="2"/>
+      <c r="AY22" s="2"/>
+      <c r="AZ22" s="2"/>
+      <c r="BA22" s="2"/>
+      <c r="BB22" s="2"/>
+      <c r="BC22" s="2"/>
+      <c r="BD22" s="2"/>
+      <c r="BE22" s="2"/>
+      <c r="BF22" s="2"/>
+      <c r="BG22" s="2"/>
+      <c r="BH22" s="2"/>
+      <c r="BI22" s="2"/>
+      <c r="BJ22" s="2"/>
+      <c r="BK22" s="2"/>
+      <c r="BL22" s="2"/>
+      <c r="BM22" s="2"/>
+      <c r="BN22" s="2"/>
+      <c r="BP22" s="2"/>
     </row>
-    <row r="23" spans="1:31" x14ac:dyDescent="0.45">
+    <row r="23" spans="1:68">
       <c r="A23" t="s">
         <v>1</v>
       </c>
@@ -2891,10 +3575,42 @@
       <c r="AE23">
         <v>6.7668999999999997</v>
       </c>
+      <c r="AF23" s="1"/>
+      <c r="AK23" s="2"/>
+      <c r="AL23" s="2"/>
+      <c r="AM23" s="2"/>
+      <c r="AN23" s="2"/>
+      <c r="AO23" s="2"/>
+      <c r="AP23" s="2"/>
+      <c r="AQ23" s="2"/>
+      <c r="AR23" s="2"/>
+      <c r="AS23" s="2"/>
+      <c r="AT23" s="2"/>
+      <c r="AU23" s="2"/>
+      <c r="AV23" s="2"/>
+      <c r="AW23" s="2"/>
+      <c r="AX23" s="2"/>
+      <c r="AY23" s="2"/>
+      <c r="AZ23" s="2"/>
+      <c r="BA23" s="2"/>
+      <c r="BB23" s="2"/>
+      <c r="BC23" s="2"/>
+      <c r="BD23" s="2"/>
+      <c r="BE23" s="2"/>
+      <c r="BF23" s="2"/>
+      <c r="BG23" s="2"/>
+      <c r="BH23" s="2"/>
+      <c r="BI23" s="2"/>
+      <c r="BJ23" s="2"/>
+      <c r="BK23" s="2"/>
+      <c r="BL23" s="2"/>
+      <c r="BM23" s="2"/>
+      <c r="BN23" s="2"/>
+      <c r="BP23" s="2"/>
     </row>
-    <row r="24" spans="1:31" x14ac:dyDescent="0.45">
+    <row r="24" spans="1:68">
       <c r="A24" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B24">
         <v>-1</v>
@@ -2986,10 +3702,42 @@
       <c r="AE24">
         <v>4.3299000000000003</v>
       </c>
+      <c r="AF24" s="1"/>
+      <c r="AK24" s="2"/>
+      <c r="AL24" s="2"/>
+      <c r="AM24" s="2"/>
+      <c r="AN24" s="2"/>
+      <c r="AO24" s="2"/>
+      <c r="AP24" s="2"/>
+      <c r="AQ24" s="2"/>
+      <c r="AR24" s="2"/>
+      <c r="AS24" s="2"/>
+      <c r="AT24" s="2"/>
+      <c r="AU24" s="2"/>
+      <c r="AV24" s="2"/>
+      <c r="AW24" s="2"/>
+      <c r="AX24" s="2"/>
+      <c r="AY24" s="2"/>
+      <c r="AZ24" s="2"/>
+      <c r="BA24" s="2"/>
+      <c r="BB24" s="2"/>
+      <c r="BC24" s="2"/>
+      <c r="BD24" s="2"/>
+      <c r="BE24" s="2"/>
+      <c r="BF24" s="2"/>
+      <c r="BG24" s="2"/>
+      <c r="BH24" s="2"/>
+      <c r="BI24" s="2"/>
+      <c r="BJ24" s="2"/>
+      <c r="BK24" s="2"/>
+      <c r="BL24" s="2"/>
+      <c r="BM24" s="2"/>
+      <c r="BN24" s="2"/>
+      <c r="BP24" s="2"/>
     </row>
-    <row r="25" spans="1:31" x14ac:dyDescent="0.45">
+    <row r="25" spans="1:68">
       <c r="A25" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B25">
         <v>-1</v>
@@ -3081,10 +3829,42 @@
       <c r="AE25">
         <v>5.1773999999999996</v>
       </c>
+      <c r="AF25" s="1"/>
+      <c r="AK25" s="2"/>
+      <c r="AL25" s="2"/>
+      <c r="AM25" s="2"/>
+      <c r="AN25" s="2"/>
+      <c r="AO25" s="2"/>
+      <c r="AP25" s="2"/>
+      <c r="AQ25" s="2"/>
+      <c r="AR25" s="2"/>
+      <c r="AS25" s="2"/>
+      <c r="AT25" s="2"/>
+      <c r="AU25" s="2"/>
+      <c r="AV25" s="2"/>
+      <c r="AW25" s="2"/>
+      <c r="AX25" s="2"/>
+      <c r="AY25" s="2"/>
+      <c r="AZ25" s="2"/>
+      <c r="BA25" s="2"/>
+      <c r="BB25" s="2"/>
+      <c r="BC25" s="2"/>
+      <c r="BD25" s="2"/>
+      <c r="BE25" s="2"/>
+      <c r="BF25" s="2"/>
+      <c r="BG25" s="2"/>
+      <c r="BH25" s="2"/>
+      <c r="BI25" s="2"/>
+      <c r="BJ25" s="2"/>
+      <c r="BK25" s="2"/>
+      <c r="BL25" s="2"/>
+      <c r="BM25" s="2"/>
+      <c r="BN25" s="2"/>
+      <c r="BP25" s="2"/>
     </row>
-    <row r="26" spans="1:31" x14ac:dyDescent="0.45">
+    <row r="26" spans="1:68">
       <c r="A26" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B26">
         <v>-1</v>
@@ -3176,8 +3956,40 @@
       <c r="AE26">
         <v>-1</v>
       </c>
+      <c r="AF26" s="1"/>
+      <c r="AK26" s="2"/>
+      <c r="AL26" s="2"/>
+      <c r="AM26" s="2"/>
+      <c r="AN26" s="2"/>
+      <c r="AO26" s="2"/>
+      <c r="AP26" s="2"/>
+      <c r="AQ26" s="2"/>
+      <c r="AR26" s="2"/>
+      <c r="AS26" s="2"/>
+      <c r="AT26" s="2"/>
+      <c r="AU26" s="2"/>
+      <c r="AV26" s="2"/>
+      <c r="AW26" s="2"/>
+      <c r="AX26" s="2"/>
+      <c r="AY26" s="2"/>
+      <c r="AZ26" s="2"/>
+      <c r="BA26" s="2"/>
+      <c r="BB26" s="2"/>
+      <c r="BC26" s="2"/>
+      <c r="BD26" s="2"/>
+      <c r="BE26" s="2"/>
+      <c r="BF26" s="2"/>
+      <c r="BG26" s="2"/>
+      <c r="BH26" s="2"/>
+      <c r="BI26" s="2"/>
+      <c r="BJ26" s="2"/>
+      <c r="BK26" s="2"/>
+      <c r="BL26" s="2"/>
+      <c r="BM26" s="2"/>
+      <c r="BN26" s="2"/>
+      <c r="BP26" s="2"/>
     </row>
-    <row r="27" spans="1:31" x14ac:dyDescent="0.45">
+    <row r="27" spans="1:68">
       <c r="A27" t="s">
         <v>2</v>
       </c>
@@ -3271,8 +4083,40 @@
       <c r="AE27">
         <v>2.7189999999999999</v>
       </c>
+      <c r="AF27" s="1"/>
+      <c r="AK27" s="2"/>
+      <c r="AL27" s="2"/>
+      <c r="AM27" s="2"/>
+      <c r="AN27" s="2"/>
+      <c r="AO27" s="2"/>
+      <c r="AP27" s="2"/>
+      <c r="AQ27" s="2"/>
+      <c r="AR27" s="2"/>
+      <c r="AS27" s="2"/>
+      <c r="AT27" s="2"/>
+      <c r="AU27" s="2"/>
+      <c r="AV27" s="2"/>
+      <c r="AW27" s="2"/>
+      <c r="AX27" s="2"/>
+      <c r="AY27" s="2"/>
+      <c r="AZ27" s="2"/>
+      <c r="BA27" s="2"/>
+      <c r="BB27" s="2"/>
+      <c r="BC27" s="2"/>
+      <c r="BD27" s="2"/>
+      <c r="BE27" s="2"/>
+      <c r="BF27" s="2"/>
+      <c r="BG27" s="2"/>
+      <c r="BH27" s="2"/>
+      <c r="BI27" s="2"/>
+      <c r="BJ27" s="2"/>
+      <c r="BK27" s="2"/>
+      <c r="BL27" s="2"/>
+      <c r="BM27" s="2"/>
+      <c r="BN27" s="2"/>
+      <c r="BP27" s="2"/>
     </row>
-    <row r="28" spans="1:31" x14ac:dyDescent="0.45">
+    <row r="28" spans="1:68">
       <c r="A28" t="s">
         <v>25</v>
       </c>
@@ -3366,10 +4210,42 @@
       <c r="AE28">
         <v>-1</v>
       </c>
+      <c r="AF28" s="1"/>
+      <c r="AK28" s="2"/>
+      <c r="AL28" s="2"/>
+      <c r="AM28" s="2"/>
+      <c r="AN28" s="2"/>
+      <c r="AO28" s="2"/>
+      <c r="AP28" s="2"/>
+      <c r="AQ28" s="2"/>
+      <c r="AR28" s="2"/>
+      <c r="AS28" s="2"/>
+      <c r="AT28" s="2"/>
+      <c r="AU28" s="2"/>
+      <c r="AV28" s="2"/>
+      <c r="AW28" s="2"/>
+      <c r="AX28" s="2"/>
+      <c r="AY28" s="2"/>
+      <c r="AZ28" s="2"/>
+      <c r="BA28" s="2"/>
+      <c r="BB28" s="2"/>
+      <c r="BC28" s="2"/>
+      <c r="BD28" s="2"/>
+      <c r="BE28" s="2"/>
+      <c r="BF28" s="2"/>
+      <c r="BG28" s="2"/>
+      <c r="BH28" s="2"/>
+      <c r="BI28" s="2"/>
+      <c r="BJ28" s="2"/>
+      <c r="BK28" s="2"/>
+      <c r="BL28" s="2"/>
+      <c r="BM28" s="2"/>
+      <c r="BN28" s="2"/>
+      <c r="BP28" s="2"/>
     </row>
-    <row r="29" spans="1:31" x14ac:dyDescent="0.45">
+    <row r="29" spans="1:68">
       <c r="A29" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B29">
         <v>-1</v>
@@ -3461,10 +4337,42 @@
       <c r="AE29">
         <v>-1</v>
       </c>
+      <c r="AF29" s="1"/>
+      <c r="AK29" s="2"/>
+      <c r="AL29" s="2"/>
+      <c r="AM29" s="2"/>
+      <c r="AN29" s="2"/>
+      <c r="AO29" s="2"/>
+      <c r="AP29" s="2"/>
+      <c r="AQ29" s="2"/>
+      <c r="AR29" s="2"/>
+      <c r="AS29" s="2"/>
+      <c r="AT29" s="2"/>
+      <c r="AU29" s="2"/>
+      <c r="AV29" s="2"/>
+      <c r="AW29" s="2"/>
+      <c r="AX29" s="2"/>
+      <c r="AY29" s="2"/>
+      <c r="AZ29" s="2"/>
+      <c r="BA29" s="2"/>
+      <c r="BB29" s="2"/>
+      <c r="BC29" s="2"/>
+      <c r="BD29" s="2"/>
+      <c r="BE29" s="2"/>
+      <c r="BF29" s="2"/>
+      <c r="BG29" s="2"/>
+      <c r="BH29" s="2"/>
+      <c r="BI29" s="2"/>
+      <c r="BJ29" s="2"/>
+      <c r="BK29" s="2"/>
+      <c r="BL29" s="2"/>
+      <c r="BM29" s="2"/>
+      <c r="BN29" s="2"/>
+      <c r="BP29" s="2"/>
     </row>
-    <row r="30" spans="1:31" x14ac:dyDescent="0.45">
+    <row r="30" spans="1:68">
       <c r="A30" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B30">
         <v>-1</v>
@@ -3556,10 +4464,42 @@
       <c r="AE30">
         <v>-1</v>
       </c>
+      <c r="AF30" s="1"/>
+      <c r="AK30" s="2"/>
+      <c r="AL30" s="2"/>
+      <c r="AM30" s="2"/>
+      <c r="AN30" s="2"/>
+      <c r="AO30" s="2"/>
+      <c r="AP30" s="2"/>
+      <c r="AQ30" s="2"/>
+      <c r="AR30" s="2"/>
+      <c r="AS30" s="2"/>
+      <c r="AT30" s="2"/>
+      <c r="AU30" s="2"/>
+      <c r="AV30" s="2"/>
+      <c r="AW30" s="2"/>
+      <c r="AX30" s="2"/>
+      <c r="AY30" s="2"/>
+      <c r="AZ30" s="2"/>
+      <c r="BA30" s="2"/>
+      <c r="BB30" s="2"/>
+      <c r="BC30" s="2"/>
+      <c r="BD30" s="2"/>
+      <c r="BE30" s="2"/>
+      <c r="BF30" s="2"/>
+      <c r="BG30" s="2"/>
+      <c r="BH30" s="2"/>
+      <c r="BI30" s="2"/>
+      <c r="BJ30" s="2"/>
+      <c r="BK30" s="2"/>
+      <c r="BL30" s="2"/>
+      <c r="BM30" s="2"/>
+      <c r="BN30" s="2"/>
+      <c r="BP30" s="2"/>
     </row>
-    <row r="31" spans="1:31" x14ac:dyDescent="0.45">
+    <row r="31" spans="1:68">
       <c r="A31" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B31">
         <v>-1</v>
@@ -3651,10 +4591,42 @@
       <c r="AE31">
         <v>9.6600000000000005E-2</v>
       </c>
+      <c r="AF31" s="1"/>
+      <c r="AK31" s="2"/>
+      <c r="AL31" s="2"/>
+      <c r="AM31" s="2"/>
+      <c r="AN31" s="2"/>
+      <c r="AO31" s="2"/>
+      <c r="AP31" s="2"/>
+      <c r="AQ31" s="2"/>
+      <c r="AR31" s="2"/>
+      <c r="AS31" s="2"/>
+      <c r="AT31" s="2"/>
+      <c r="AU31" s="2"/>
+      <c r="AV31" s="2"/>
+      <c r="AW31" s="2"/>
+      <c r="AX31" s="2"/>
+      <c r="AY31" s="2"/>
+      <c r="AZ31" s="2"/>
+      <c r="BA31" s="2"/>
+      <c r="BB31" s="2"/>
+      <c r="BC31" s="2"/>
+      <c r="BD31" s="2"/>
+      <c r="BE31" s="2"/>
+      <c r="BF31" s="2"/>
+      <c r="BG31" s="2"/>
+      <c r="BH31" s="2"/>
+      <c r="BI31" s="2"/>
+      <c r="BJ31" s="2"/>
+      <c r="BK31" s="2"/>
+      <c r="BL31" s="2"/>
+      <c r="BM31" s="2"/>
+      <c r="BN31" s="2"/>
+      <c r="BP31" s="2"/>
     </row>
-    <row r="32" spans="1:31" x14ac:dyDescent="0.45">
+    <row r="32" spans="1:68">
       <c r="A32" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B32">
         <v>-1</v>
@@ -3746,10 +4718,42 @@
       <c r="AE32">
         <v>2.4443999999999999</v>
       </c>
+      <c r="AF32" s="1"/>
+      <c r="AK32" s="2"/>
+      <c r="AL32" s="2"/>
+      <c r="AM32" s="2"/>
+      <c r="AN32" s="2"/>
+      <c r="AO32" s="2"/>
+      <c r="AP32" s="2"/>
+      <c r="AQ32" s="2"/>
+      <c r="AR32" s="2"/>
+      <c r="AS32" s="2"/>
+      <c r="AT32" s="2"/>
+      <c r="AU32" s="2"/>
+      <c r="AV32" s="2"/>
+      <c r="AW32" s="2"/>
+      <c r="AX32" s="2"/>
+      <c r="AY32" s="2"/>
+      <c r="AZ32" s="2"/>
+      <c r="BA32" s="2"/>
+      <c r="BB32" s="2"/>
+      <c r="BC32" s="2"/>
+      <c r="BD32" s="2"/>
+      <c r="BE32" s="2"/>
+      <c r="BF32" s="2"/>
+      <c r="BG32" s="2"/>
+      <c r="BH32" s="2"/>
+      <c r="BI32" s="2"/>
+      <c r="BJ32" s="2"/>
+      <c r="BK32" s="2"/>
+      <c r="BL32" s="2"/>
+      <c r="BM32" s="2"/>
+      <c r="BN32" s="2"/>
+      <c r="BP32" s="2"/>
     </row>
-    <row r="33" spans="1:31" x14ac:dyDescent="0.45">
+    <row r="33" spans="1:68">
       <c r="A33" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B33">
         <v>-1</v>
@@ -3841,10 +4845,42 @@
       <c r="AE33">
         <v>-1</v>
       </c>
+      <c r="AF33" s="1"/>
+      <c r="AK33" s="2"/>
+      <c r="AL33" s="2"/>
+      <c r="AM33" s="2"/>
+      <c r="AN33" s="2"/>
+      <c r="AO33" s="2"/>
+      <c r="AP33" s="2"/>
+      <c r="AQ33" s="2"/>
+      <c r="AR33" s="2"/>
+      <c r="AS33" s="2"/>
+      <c r="AT33" s="2"/>
+      <c r="AU33" s="2"/>
+      <c r="AV33" s="2"/>
+      <c r="AW33" s="2"/>
+      <c r="AX33" s="2"/>
+      <c r="AY33" s="2"/>
+      <c r="AZ33" s="2"/>
+      <c r="BA33" s="2"/>
+      <c r="BB33" s="2"/>
+      <c r="BC33" s="2"/>
+      <c r="BD33" s="2"/>
+      <c r="BE33" s="2"/>
+      <c r="BF33" s="2"/>
+      <c r="BG33" s="2"/>
+      <c r="BH33" s="2"/>
+      <c r="BI33" s="2"/>
+      <c r="BJ33" s="2"/>
+      <c r="BK33" s="2"/>
+      <c r="BL33" s="2"/>
+      <c r="BM33" s="2"/>
+      <c r="BN33" s="2"/>
+      <c r="BP33" s="2"/>
     </row>
-    <row r="34" spans="1:31" x14ac:dyDescent="0.45">
+    <row r="34" spans="1:68">
       <c r="A34" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B34">
         <v>-1</v>
@@ -3936,8 +4972,40 @@
       <c r="AE34">
         <v>-1</v>
       </c>
+      <c r="AF34" s="1"/>
+      <c r="AK34" s="2"/>
+      <c r="AL34" s="2"/>
+      <c r="AM34" s="2"/>
+      <c r="AN34" s="2"/>
+      <c r="AO34" s="2"/>
+      <c r="AP34" s="2"/>
+      <c r="AQ34" s="2"/>
+      <c r="AR34" s="2"/>
+      <c r="AS34" s="2"/>
+      <c r="AT34" s="2"/>
+      <c r="AU34" s="2"/>
+      <c r="AV34" s="2"/>
+      <c r="AW34" s="2"/>
+      <c r="AX34" s="2"/>
+      <c r="AY34" s="2"/>
+      <c r="AZ34" s="2"/>
+      <c r="BA34" s="2"/>
+      <c r="BB34" s="2"/>
+      <c r="BC34" s="2"/>
+      <c r="BD34" s="2"/>
+      <c r="BE34" s="2"/>
+      <c r="BF34" s="2"/>
+      <c r="BG34" s="2"/>
+      <c r="BH34" s="2"/>
+      <c r="BI34" s="2"/>
+      <c r="BJ34" s="2"/>
+      <c r="BK34" s="2"/>
+      <c r="BL34" s="2"/>
+      <c r="BM34" s="2"/>
+      <c r="BN34" s="2"/>
+      <c r="BP34" s="2"/>
     </row>
-    <row r="35" spans="1:31" x14ac:dyDescent="0.45">
+    <row r="35" spans="1:68">
       <c r="A35" t="s">
         <v>12</v>
       </c>
@@ -4031,8 +5099,40 @@
       <c r="AE35">
         <v>4.5602999999999998</v>
       </c>
+      <c r="AF35" s="1"/>
+      <c r="AK35" s="2"/>
+      <c r="AL35" s="2"/>
+      <c r="AM35" s="2"/>
+      <c r="AN35" s="2"/>
+      <c r="AO35" s="2"/>
+      <c r="AP35" s="2"/>
+      <c r="AQ35" s="2"/>
+      <c r="AR35" s="2"/>
+      <c r="AS35" s="2"/>
+      <c r="AT35" s="2"/>
+      <c r="AU35" s="2"/>
+      <c r="AV35" s="2"/>
+      <c r="AW35" s="2"/>
+      <c r="AX35" s="2"/>
+      <c r="AY35" s="2"/>
+      <c r="AZ35" s="2"/>
+      <c r="BA35" s="2"/>
+      <c r="BB35" s="2"/>
+      <c r="BC35" s="2"/>
+      <c r="BD35" s="2"/>
+      <c r="BE35" s="2"/>
+      <c r="BF35" s="2"/>
+      <c r="BG35" s="2"/>
+      <c r="BH35" s="2"/>
+      <c r="BI35" s="2"/>
+      <c r="BJ35" s="2"/>
+      <c r="BK35" s="2"/>
+      <c r="BL35" s="2"/>
+      <c r="BM35" s="2"/>
+      <c r="BN35" s="2"/>
+      <c r="BP35" s="2"/>
     </row>
-    <row r="36" spans="1:31" x14ac:dyDescent="0.45">
+    <row r="36" spans="1:68">
       <c r="A36" t="s">
         <v>19</v>
       </c>
@@ -4126,10 +5226,42 @@
       <c r="AE36">
         <v>-1</v>
       </c>
+      <c r="AF36" s="1"/>
+      <c r="AK36" s="2"/>
+      <c r="AL36" s="2"/>
+      <c r="AM36" s="2"/>
+      <c r="AN36" s="2"/>
+      <c r="AO36" s="2"/>
+      <c r="AP36" s="2"/>
+      <c r="AQ36" s="2"/>
+      <c r="AR36" s="2"/>
+      <c r="AS36" s="2"/>
+      <c r="AT36" s="2"/>
+      <c r="AU36" s="2"/>
+      <c r="AV36" s="2"/>
+      <c r="AW36" s="2"/>
+      <c r="AX36" s="2"/>
+      <c r="AY36" s="2"/>
+      <c r="AZ36" s="2"/>
+      <c r="BA36" s="2"/>
+      <c r="BB36" s="2"/>
+      <c r="BC36" s="2"/>
+      <c r="BD36" s="2"/>
+      <c r="BE36" s="2"/>
+      <c r="BF36" s="2"/>
+      <c r="BG36" s="2"/>
+      <c r="BH36" s="2"/>
+      <c r="BI36" s="2"/>
+      <c r="BJ36" s="2"/>
+      <c r="BK36" s="2"/>
+      <c r="BL36" s="2"/>
+      <c r="BM36" s="2"/>
+      <c r="BN36" s="2"/>
+      <c r="BP36" s="2"/>
     </row>
-    <row r="37" spans="1:31" x14ac:dyDescent="0.45">
+    <row r="37" spans="1:68">
       <c r="A37" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B37">
         <v>-1</v>
@@ -4221,10 +5353,42 @@
       <c r="AE37">
         <v>4.3327999999999998</v>
       </c>
+      <c r="AF37" s="1"/>
+      <c r="AK37" s="2"/>
+      <c r="AL37" s="2"/>
+      <c r="AM37" s="2"/>
+      <c r="AN37" s="2"/>
+      <c r="AO37" s="2"/>
+      <c r="AP37" s="2"/>
+      <c r="AQ37" s="2"/>
+      <c r="AR37" s="2"/>
+      <c r="AS37" s="2"/>
+      <c r="AT37" s="2"/>
+      <c r="AU37" s="2"/>
+      <c r="AV37" s="2"/>
+      <c r="AW37" s="2"/>
+      <c r="AX37" s="2"/>
+      <c r="AY37" s="2"/>
+      <c r="AZ37" s="2"/>
+      <c r="BA37" s="2"/>
+      <c r="BB37" s="2"/>
+      <c r="BC37" s="2"/>
+      <c r="BD37" s="2"/>
+      <c r="BE37" s="2"/>
+      <c r="BF37" s="2"/>
+      <c r="BG37" s="2"/>
+      <c r="BH37" s="2"/>
+      <c r="BI37" s="2"/>
+      <c r="BJ37" s="2"/>
+      <c r="BK37" s="2"/>
+      <c r="BL37" s="2"/>
+      <c r="BM37" s="2"/>
+      <c r="BN37" s="2"/>
+      <c r="BP37" s="2"/>
     </row>
-    <row r="38" spans="1:31" x14ac:dyDescent="0.45">
+    <row r="38" spans="1:68">
       <c r="A38" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B38">
         <v>-1</v>
@@ -4316,10 +5480,42 @@
       <c r="AE38">
         <v>4.1749999999999998</v>
       </c>
+      <c r="AF38" s="1"/>
+      <c r="AK38" s="2"/>
+      <c r="AL38" s="2"/>
+      <c r="AM38" s="2"/>
+      <c r="AN38" s="2"/>
+      <c r="AO38" s="2"/>
+      <c r="AP38" s="2"/>
+      <c r="AQ38" s="2"/>
+      <c r="AR38" s="2"/>
+      <c r="AS38" s="2"/>
+      <c r="AT38" s="2"/>
+      <c r="AU38" s="2"/>
+      <c r="AV38" s="2"/>
+      <c r="AW38" s="2"/>
+      <c r="AX38" s="2"/>
+      <c r="AY38" s="2"/>
+      <c r="AZ38" s="2"/>
+      <c r="BA38" s="2"/>
+      <c r="BB38" s="2"/>
+      <c r="BC38" s="2"/>
+      <c r="BD38" s="2"/>
+      <c r="BE38" s="2"/>
+      <c r="BF38" s="2"/>
+      <c r="BG38" s="2"/>
+      <c r="BH38" s="2"/>
+      <c r="BI38" s="2"/>
+      <c r="BJ38" s="2"/>
+      <c r="BK38" s="2"/>
+      <c r="BL38" s="2"/>
+      <c r="BM38" s="2"/>
+      <c r="BN38" s="2"/>
+      <c r="BP38" s="2"/>
     </row>
-    <row r="39" spans="1:31" x14ac:dyDescent="0.45">
+    <row r="39" spans="1:68">
       <c r="A39" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B39">
         <v>-1</v>
@@ -4411,10 +5607,42 @@
       <c r="AE39">
         <v>-1</v>
       </c>
+      <c r="AF39" s="1"/>
+      <c r="AK39" s="2"/>
+      <c r="AL39" s="2"/>
+      <c r="AM39" s="2"/>
+      <c r="AN39" s="2"/>
+      <c r="AO39" s="2"/>
+      <c r="AP39" s="2"/>
+      <c r="AQ39" s="2"/>
+      <c r="AR39" s="2"/>
+      <c r="AS39" s="2"/>
+      <c r="AT39" s="2"/>
+      <c r="AU39" s="2"/>
+      <c r="AV39" s="2"/>
+      <c r="AW39" s="2"/>
+      <c r="AX39" s="2"/>
+      <c r="AY39" s="2"/>
+      <c r="AZ39" s="2"/>
+      <c r="BA39" s="2"/>
+      <c r="BB39" s="2"/>
+      <c r="BC39" s="2"/>
+      <c r="BD39" s="2"/>
+      <c r="BE39" s="2"/>
+      <c r="BF39" s="2"/>
+      <c r="BG39" s="2"/>
+      <c r="BH39" s="2"/>
+      <c r="BI39" s="2"/>
+      <c r="BJ39" s="2"/>
+      <c r="BK39" s="2"/>
+      <c r="BL39" s="2"/>
+      <c r="BM39" s="2"/>
+      <c r="BN39" s="2"/>
+      <c r="BP39" s="2"/>
     </row>
-    <row r="40" spans="1:31" x14ac:dyDescent="0.45">
+    <row r="40" spans="1:68">
       <c r="A40" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B40">
         <v>-1</v>
@@ -4506,10 +5734,42 @@
       <c r="AE40">
         <v>2.1863999999999999</v>
       </c>
+      <c r="AF40" s="1"/>
+      <c r="AK40" s="2"/>
+      <c r="AL40" s="2"/>
+      <c r="AM40" s="2"/>
+      <c r="AN40" s="2"/>
+      <c r="AO40" s="2"/>
+      <c r="AP40" s="2"/>
+      <c r="AQ40" s="2"/>
+      <c r="AR40" s="2"/>
+      <c r="AS40" s="2"/>
+      <c r="AT40" s="2"/>
+      <c r="AU40" s="2"/>
+      <c r="AV40" s="2"/>
+      <c r="AW40" s="2"/>
+      <c r="AX40" s="2"/>
+      <c r="AY40" s="2"/>
+      <c r="AZ40" s="2"/>
+      <c r="BA40" s="2"/>
+      <c r="BB40" s="2"/>
+      <c r="BC40" s="2"/>
+      <c r="BD40" s="2"/>
+      <c r="BE40" s="2"/>
+      <c r="BF40" s="2"/>
+      <c r="BG40" s="2"/>
+      <c r="BH40" s="2"/>
+      <c r="BI40" s="2"/>
+      <c r="BJ40" s="2"/>
+      <c r="BK40" s="2"/>
+      <c r="BL40" s="2"/>
+      <c r="BM40" s="2"/>
+      <c r="BN40" s="2"/>
+      <c r="BP40" s="2"/>
     </row>
-    <row r="41" spans="1:31" x14ac:dyDescent="0.45">
+    <row r="41" spans="1:68">
       <c r="A41" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B41">
         <v>-1</v>
@@ -4601,10 +5861,42 @@
       <c r="AE41">
         <v>-1</v>
       </c>
+      <c r="AF41" s="1"/>
+      <c r="AK41" s="2"/>
+      <c r="AL41" s="2"/>
+      <c r="AM41" s="2"/>
+      <c r="AN41" s="2"/>
+      <c r="AO41" s="2"/>
+      <c r="AP41" s="2"/>
+      <c r="AQ41" s="2"/>
+      <c r="AR41" s="2"/>
+      <c r="AS41" s="2"/>
+      <c r="AT41" s="2"/>
+      <c r="AU41" s="2"/>
+      <c r="AV41" s="2"/>
+      <c r="AW41" s="2"/>
+      <c r="AX41" s="2"/>
+      <c r="AY41" s="2"/>
+      <c r="AZ41" s="2"/>
+      <c r="BA41" s="2"/>
+      <c r="BB41" s="2"/>
+      <c r="BC41" s="2"/>
+      <c r="BD41" s="2"/>
+      <c r="BE41" s="2"/>
+      <c r="BF41" s="2"/>
+      <c r="BG41" s="2"/>
+      <c r="BH41" s="2"/>
+      <c r="BI41" s="2"/>
+      <c r="BJ41" s="2"/>
+      <c r="BK41" s="2"/>
+      <c r="BL41" s="2"/>
+      <c r="BM41" s="2"/>
+      <c r="BN41" s="2"/>
+      <c r="BP41" s="2"/>
     </row>
-    <row r="42" spans="1:31" x14ac:dyDescent="0.45">
+    <row r="42" spans="1:68">
       <c r="A42" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B42">
         <v>-1</v>
@@ -4696,8 +5988,40 @@
       <c r="AE42">
         <v>3.6600999999999999</v>
       </c>
+      <c r="AF42" s="1"/>
+      <c r="AK42" s="2"/>
+      <c r="AL42" s="2"/>
+      <c r="AM42" s="2"/>
+      <c r="AN42" s="2"/>
+      <c r="AO42" s="2"/>
+      <c r="AP42" s="2"/>
+      <c r="AQ42" s="2"/>
+      <c r="AR42" s="2"/>
+      <c r="AS42" s="2"/>
+      <c r="AT42" s="2"/>
+      <c r="AU42" s="2"/>
+      <c r="AV42" s="2"/>
+      <c r="AW42" s="2"/>
+      <c r="AX42" s="2"/>
+      <c r="AY42" s="2"/>
+      <c r="AZ42" s="2"/>
+      <c r="BA42" s="2"/>
+      <c r="BB42" s="2"/>
+      <c r="BC42" s="2"/>
+      <c r="BD42" s="2"/>
+      <c r="BE42" s="2"/>
+      <c r="BF42" s="2"/>
+      <c r="BG42" s="2"/>
+      <c r="BH42" s="2"/>
+      <c r="BI42" s="2"/>
+      <c r="BJ42" s="2"/>
+      <c r="BK42" s="2"/>
+      <c r="BL42" s="2"/>
+      <c r="BM42" s="2"/>
+      <c r="BN42" s="2"/>
+      <c r="BP42" s="2"/>
     </row>
-    <row r="43" spans="1:31" x14ac:dyDescent="0.45">
+    <row r="43" spans="1:68">
       <c r="A43" t="s">
         <v>6</v>
       </c>
@@ -4791,8 +6115,40 @@
       <c r="AE43">
         <v>3.6074999999999999</v>
       </c>
+      <c r="AF43" s="1"/>
+      <c r="AK43" s="2"/>
+      <c r="AL43" s="2"/>
+      <c r="AM43" s="2"/>
+      <c r="AN43" s="2"/>
+      <c r="AO43" s="2"/>
+      <c r="AP43" s="2"/>
+      <c r="AQ43" s="2"/>
+      <c r="AR43" s="2"/>
+      <c r="AS43" s="2"/>
+      <c r="AT43" s="2"/>
+      <c r="AU43" s="2"/>
+      <c r="AV43" s="2"/>
+      <c r="AW43" s="2"/>
+      <c r="AX43" s="2"/>
+      <c r="AY43" s="2"/>
+      <c r="AZ43" s="2"/>
+      <c r="BA43" s="2"/>
+      <c r="BB43" s="2"/>
+      <c r="BC43" s="2"/>
+      <c r="BD43" s="2"/>
+      <c r="BE43" s="2"/>
+      <c r="BF43" s="2"/>
+      <c r="BG43" s="2"/>
+      <c r="BH43" s="2"/>
+      <c r="BI43" s="2"/>
+      <c r="BJ43" s="2"/>
+      <c r="BK43" s="2"/>
+      <c r="BL43" s="2"/>
+      <c r="BM43" s="2"/>
+      <c r="BN43" s="2"/>
+      <c r="BP43" s="2"/>
     </row>
-    <row r="44" spans="1:31" x14ac:dyDescent="0.45">
+    <row r="44" spans="1:68">
       <c r="A44" t="s">
         <v>8</v>
       </c>
@@ -4886,10 +6242,42 @@
       <c r="AE44">
         <v>-1</v>
       </c>
+      <c r="AF44" s="1"/>
+      <c r="AK44" s="2"/>
+      <c r="AL44" s="2"/>
+      <c r="AM44" s="2"/>
+      <c r="AN44" s="2"/>
+      <c r="AO44" s="2"/>
+      <c r="AP44" s="2"/>
+      <c r="AQ44" s="2"/>
+      <c r="AR44" s="2"/>
+      <c r="AS44" s="2"/>
+      <c r="AT44" s="2"/>
+      <c r="AU44" s="2"/>
+      <c r="AV44" s="2"/>
+      <c r="AW44" s="2"/>
+      <c r="AX44" s="2"/>
+      <c r="AY44" s="2"/>
+      <c r="AZ44" s="2"/>
+      <c r="BA44" s="2"/>
+      <c r="BB44" s="2"/>
+      <c r="BC44" s="2"/>
+      <c r="BD44" s="2"/>
+      <c r="BE44" s="2"/>
+      <c r="BF44" s="2"/>
+      <c r="BG44" s="2"/>
+      <c r="BH44" s="2"/>
+      <c r="BI44" s="2"/>
+      <c r="BJ44" s="2"/>
+      <c r="BK44" s="2"/>
+      <c r="BL44" s="2"/>
+      <c r="BM44" s="2"/>
+      <c r="BN44" s="2"/>
+      <c r="BP44" s="2"/>
     </row>
-    <row r="45" spans="1:31" x14ac:dyDescent="0.45">
+    <row r="45" spans="1:68">
       <c r="A45" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B45">
         <v>-1</v>
@@ -4981,8 +6369,40 @@
       <c r="AE45">
         <v>0</v>
       </c>
+      <c r="AF45" s="1"/>
+      <c r="AK45" s="2"/>
+      <c r="AL45" s="2"/>
+      <c r="AM45" s="2"/>
+      <c r="AN45" s="2"/>
+      <c r="AO45" s="2"/>
+      <c r="AP45" s="2"/>
+      <c r="AQ45" s="2"/>
+      <c r="AR45" s="2"/>
+      <c r="AS45" s="2"/>
+      <c r="AT45" s="2"/>
+      <c r="AU45" s="2"/>
+      <c r="AV45" s="2"/>
+      <c r="AW45" s="2"/>
+      <c r="AX45" s="2"/>
+      <c r="AY45" s="2"/>
+      <c r="AZ45" s="2"/>
+      <c r="BA45" s="2"/>
+      <c r="BB45" s="2"/>
+      <c r="BC45" s="2"/>
+      <c r="BD45" s="2"/>
+      <c r="BE45" s="2"/>
+      <c r="BF45" s="2"/>
+      <c r="BG45" s="2"/>
+      <c r="BH45" s="2"/>
+      <c r="BI45" s="2"/>
+      <c r="BJ45" s="2"/>
+      <c r="BK45" s="2"/>
+      <c r="BL45" s="2"/>
+      <c r="BM45" s="2"/>
+      <c r="BN45" s="2"/>
+      <c r="BP45" s="2"/>
     </row>
-    <row r="46" spans="1:31" x14ac:dyDescent="0.45">
+    <row r="46" spans="1:68">
       <c r="A46" t="s">
         <v>23</v>
       </c>
@@ -5076,10 +6496,42 @@
       <c r="AE46">
         <v>-1</v>
       </c>
+      <c r="AF46" s="1"/>
+      <c r="AK46" s="2"/>
+      <c r="AL46" s="2"/>
+      <c r="AM46" s="2"/>
+      <c r="AN46" s="2"/>
+      <c r="AO46" s="2"/>
+      <c r="AP46" s="2"/>
+      <c r="AQ46" s="2"/>
+      <c r="AR46" s="2"/>
+      <c r="AS46" s="2"/>
+      <c r="AT46" s="2"/>
+      <c r="AU46" s="2"/>
+      <c r="AV46" s="2"/>
+      <c r="AW46" s="2"/>
+      <c r="AX46" s="2"/>
+      <c r="AY46" s="2"/>
+      <c r="AZ46" s="2"/>
+      <c r="BA46" s="2"/>
+      <c r="BB46" s="2"/>
+      <c r="BC46" s="2"/>
+      <c r="BD46" s="2"/>
+      <c r="BE46" s="2"/>
+      <c r="BF46" s="2"/>
+      <c r="BG46" s="2"/>
+      <c r="BH46" s="2"/>
+      <c r="BI46" s="2"/>
+      <c r="BJ46" s="2"/>
+      <c r="BK46" s="2"/>
+      <c r="BL46" s="2"/>
+      <c r="BM46" s="2"/>
+      <c r="BN46" s="2"/>
+      <c r="BP46" s="2"/>
     </row>
-    <row r="47" spans="1:31" x14ac:dyDescent="0.45">
+    <row r="47" spans="1:68">
       <c r="A47" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B47">
         <v>-1</v>
@@ -5171,10 +6623,42 @@
       <c r="AE47">
         <v>-1</v>
       </c>
+      <c r="AF47" s="1"/>
+      <c r="AK47" s="2"/>
+      <c r="AL47" s="2"/>
+      <c r="AM47" s="2"/>
+      <c r="AN47" s="2"/>
+      <c r="AO47" s="2"/>
+      <c r="AP47" s="2"/>
+      <c r="AQ47" s="2"/>
+      <c r="AR47" s="2"/>
+      <c r="AS47" s="2"/>
+      <c r="AT47" s="2"/>
+      <c r="AU47" s="2"/>
+      <c r="AV47" s="2"/>
+      <c r="AW47" s="2"/>
+      <c r="AX47" s="2"/>
+      <c r="AY47" s="2"/>
+      <c r="AZ47" s="2"/>
+      <c r="BA47" s="2"/>
+      <c r="BB47" s="2"/>
+      <c r="BC47" s="2"/>
+      <c r="BD47" s="2"/>
+      <c r="BE47" s="2"/>
+      <c r="BF47" s="2"/>
+      <c r="BG47" s="2"/>
+      <c r="BH47" s="2"/>
+      <c r="BI47" s="2"/>
+      <c r="BJ47" s="2"/>
+      <c r="BK47" s="2"/>
+      <c r="BL47" s="2"/>
+      <c r="BM47" s="2"/>
+      <c r="BN47" s="2"/>
+      <c r="BP47" s="2"/>
     </row>
-    <row r="48" spans="1:31" x14ac:dyDescent="0.45">
+    <row r="48" spans="1:68">
       <c r="A48" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B48">
         <v>-1</v>
@@ -5266,10 +6750,42 @@
       <c r="AE48">
         <v>-1</v>
       </c>
+      <c r="AF48" s="1"/>
+      <c r="AK48" s="2"/>
+      <c r="AL48" s="2"/>
+      <c r="AM48" s="2"/>
+      <c r="AN48" s="2"/>
+      <c r="AO48" s="2"/>
+      <c r="AP48" s="2"/>
+      <c r="AQ48" s="2"/>
+      <c r="AR48" s="2"/>
+      <c r="AS48" s="2"/>
+      <c r="AT48" s="2"/>
+      <c r="AU48" s="2"/>
+      <c r="AV48" s="2"/>
+      <c r="AW48" s="2"/>
+      <c r="AX48" s="2"/>
+      <c r="AY48" s="2"/>
+      <c r="AZ48" s="2"/>
+      <c r="BA48" s="2"/>
+      <c r="BB48" s="2"/>
+      <c r="BC48" s="2"/>
+      <c r="BD48" s="2"/>
+      <c r="BE48" s="2"/>
+      <c r="BF48" s="2"/>
+      <c r="BG48" s="2"/>
+      <c r="BH48" s="2"/>
+      <c r="BI48" s="2"/>
+      <c r="BJ48" s="2"/>
+      <c r="BK48" s="2"/>
+      <c r="BL48" s="2"/>
+      <c r="BM48" s="2"/>
+      <c r="BN48" s="2"/>
+      <c r="BP48" s="2"/>
     </row>
-    <row r="49" spans="1:31" x14ac:dyDescent="0.45">
+    <row r="49" spans="1:68">
       <c r="A49" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B49">
         <v>-1</v>
@@ -5361,10 +6877,42 @@
       <c r="AE49">
         <v>-1</v>
       </c>
+      <c r="AF49" s="1"/>
+      <c r="AK49" s="2"/>
+      <c r="AL49" s="2"/>
+      <c r="AM49" s="2"/>
+      <c r="AN49" s="2"/>
+      <c r="AO49" s="2"/>
+      <c r="AP49" s="2"/>
+      <c r="AQ49" s="2"/>
+      <c r="AR49" s="2"/>
+      <c r="AS49" s="2"/>
+      <c r="AT49" s="2"/>
+      <c r="AU49" s="2"/>
+      <c r="AV49" s="2"/>
+      <c r="AW49" s="2"/>
+      <c r="AX49" s="2"/>
+      <c r="AY49" s="2"/>
+      <c r="AZ49" s="2"/>
+      <c r="BA49" s="2"/>
+      <c r="BB49" s="2"/>
+      <c r="BC49" s="2"/>
+      <c r="BD49" s="2"/>
+      <c r="BE49" s="2"/>
+      <c r="BF49" s="2"/>
+      <c r="BG49" s="2"/>
+      <c r="BH49" s="2"/>
+      <c r="BI49" s="2"/>
+      <c r="BJ49" s="2"/>
+      <c r="BK49" s="2"/>
+      <c r="BL49" s="2"/>
+      <c r="BM49" s="2"/>
+      <c r="BN49" s="2"/>
+      <c r="BP49" s="2"/>
     </row>
-    <row r="50" spans="1:31" x14ac:dyDescent="0.45">
+    <row r="50" spans="1:68">
       <c r="A50" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B50">
         <v>-1</v>
@@ -5456,10 +7004,42 @@
       <c r="AE50">
         <v>-1</v>
       </c>
+      <c r="AF50" s="1"/>
+      <c r="AK50" s="2"/>
+      <c r="AL50" s="2"/>
+      <c r="AM50" s="2"/>
+      <c r="AN50" s="2"/>
+      <c r="AO50" s="2"/>
+      <c r="AP50" s="2"/>
+      <c r="AQ50" s="2"/>
+      <c r="AR50" s="2"/>
+      <c r="AS50" s="2"/>
+      <c r="AT50" s="2"/>
+      <c r="AU50" s="2"/>
+      <c r="AV50" s="2"/>
+      <c r="AW50" s="2"/>
+      <c r="AX50" s="2"/>
+      <c r="AY50" s="2"/>
+      <c r="AZ50" s="2"/>
+      <c r="BA50" s="2"/>
+      <c r="BB50" s="2"/>
+      <c r="BC50" s="2"/>
+      <c r="BD50" s="2"/>
+      <c r="BE50" s="2"/>
+      <c r="BF50" s="2"/>
+      <c r="BG50" s="2"/>
+      <c r="BH50" s="2"/>
+      <c r="BI50" s="2"/>
+      <c r="BJ50" s="2"/>
+      <c r="BK50" s="2"/>
+      <c r="BL50" s="2"/>
+      <c r="BM50" s="2"/>
+      <c r="BN50" s="2"/>
+      <c r="BP50" s="2"/>
     </row>
-    <row r="51" spans="1:31" x14ac:dyDescent="0.45">
+    <row r="51" spans="1:68">
       <c r="A51" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B51">
         <v>-1</v>
@@ -5551,10 +7131,42 @@
       <c r="AE51">
         <v>-1</v>
       </c>
+      <c r="AF51" s="1"/>
+      <c r="AK51" s="2"/>
+      <c r="AL51" s="2"/>
+      <c r="AM51" s="2"/>
+      <c r="AN51" s="2"/>
+      <c r="AO51" s="2"/>
+      <c r="AP51" s="2"/>
+      <c r="AQ51" s="2"/>
+      <c r="AR51" s="2"/>
+      <c r="AS51" s="2"/>
+      <c r="AT51" s="2"/>
+      <c r="AU51" s="2"/>
+      <c r="AV51" s="2"/>
+      <c r="AW51" s="2"/>
+      <c r="AX51" s="2"/>
+      <c r="AY51" s="2"/>
+      <c r="AZ51" s="2"/>
+      <c r="BA51" s="2"/>
+      <c r="BB51" s="2"/>
+      <c r="BC51" s="2"/>
+      <c r="BD51" s="2"/>
+      <c r="BE51" s="2"/>
+      <c r="BF51" s="2"/>
+      <c r="BG51" s="2"/>
+      <c r="BH51" s="2"/>
+      <c r="BI51" s="2"/>
+      <c r="BJ51" s="2"/>
+      <c r="BK51" s="2"/>
+      <c r="BL51" s="2"/>
+      <c r="BM51" s="2"/>
+      <c r="BN51" s="2"/>
+      <c r="BP51" s="2"/>
     </row>
-    <row r="52" spans="1:31" x14ac:dyDescent="0.45">
+    <row r="52" spans="1:68">
       <c r="A52" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B52">
         <v>-1</v>
@@ -5646,8 +7258,40 @@
       <c r="AE52">
         <v>-1</v>
       </c>
+      <c r="AF52" s="1"/>
+      <c r="AK52" s="2"/>
+      <c r="AL52" s="2"/>
+      <c r="AM52" s="2"/>
+      <c r="AN52" s="2"/>
+      <c r="AO52" s="2"/>
+      <c r="AP52" s="2"/>
+      <c r="AQ52" s="2"/>
+      <c r="AR52" s="2"/>
+      <c r="AS52" s="2"/>
+      <c r="AT52" s="2"/>
+      <c r="AU52" s="2"/>
+      <c r="AV52" s="2"/>
+      <c r="AW52" s="2"/>
+      <c r="AX52" s="2"/>
+      <c r="AY52" s="2"/>
+      <c r="AZ52" s="2"/>
+      <c r="BA52" s="2"/>
+      <c r="BB52" s="2"/>
+      <c r="BC52" s="2"/>
+      <c r="BD52" s="2"/>
+      <c r="BE52" s="2"/>
+      <c r="BF52" s="2"/>
+      <c r="BG52" s="2"/>
+      <c r="BH52" s="2"/>
+      <c r="BI52" s="2"/>
+      <c r="BJ52" s="2"/>
+      <c r="BK52" s="2"/>
+      <c r="BL52" s="2"/>
+      <c r="BM52" s="2"/>
+      <c r="BN52" s="2"/>
+      <c r="BP52" s="2"/>
     </row>
-    <row r="53" spans="1:31" x14ac:dyDescent="0.45">
+    <row r="53" spans="1:68">
       <c r="A53" t="s">
         <v>7</v>
       </c>
@@ -5741,10 +7385,42 @@
       <c r="AE53">
         <v>4.6512000000000002</v>
       </c>
+      <c r="AF53" s="1"/>
+      <c r="AK53" s="2"/>
+      <c r="AL53" s="2"/>
+      <c r="AM53" s="2"/>
+      <c r="AN53" s="2"/>
+      <c r="AO53" s="2"/>
+      <c r="AP53" s="2"/>
+      <c r="AQ53" s="2"/>
+      <c r="AR53" s="2"/>
+      <c r="AS53" s="2"/>
+      <c r="AT53" s="2"/>
+      <c r="AU53" s="2"/>
+      <c r="AV53" s="2"/>
+      <c r="AW53" s="2"/>
+      <c r="AX53" s="2"/>
+      <c r="AY53" s="2"/>
+      <c r="AZ53" s="2"/>
+      <c r="BA53" s="2"/>
+      <c r="BB53" s="2"/>
+      <c r="BC53" s="2"/>
+      <c r="BD53" s="2"/>
+      <c r="BE53" s="2"/>
+      <c r="BF53" s="2"/>
+      <c r="BG53" s="2"/>
+      <c r="BH53" s="2"/>
+      <c r="BI53" s="2"/>
+      <c r="BJ53" s="2"/>
+      <c r="BK53" s="2"/>
+      <c r="BL53" s="2"/>
+      <c r="BM53" s="2"/>
+      <c r="BN53" s="2"/>
+      <c r="BP53" s="2"/>
     </row>
-    <row r="54" spans="1:31" x14ac:dyDescent="0.45">
+    <row r="54" spans="1:68">
       <c r="A54" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B54">
         <v>-1</v>
@@ -5836,10 +7512,42 @@
       <c r="AE54">
         <v>-1</v>
       </c>
+      <c r="AF54" s="1"/>
+      <c r="AK54" s="2"/>
+      <c r="AL54" s="2"/>
+      <c r="AM54" s="2"/>
+      <c r="AN54" s="2"/>
+      <c r="AO54" s="2"/>
+      <c r="AP54" s="2"/>
+      <c r="AQ54" s="2"/>
+      <c r="AR54" s="2"/>
+      <c r="AS54" s="2"/>
+      <c r="AT54" s="2"/>
+      <c r="AU54" s="2"/>
+      <c r="AV54" s="2"/>
+      <c r="AW54" s="2"/>
+      <c r="AX54" s="2"/>
+      <c r="AY54" s="2"/>
+      <c r="AZ54" s="2"/>
+      <c r="BA54" s="2"/>
+      <c r="BB54" s="2"/>
+      <c r="BC54" s="2"/>
+      <c r="BD54" s="2"/>
+      <c r="BE54" s="2"/>
+      <c r="BF54" s="2"/>
+      <c r="BG54" s="2"/>
+      <c r="BH54" s="2"/>
+      <c r="BI54" s="2"/>
+      <c r="BJ54" s="2"/>
+      <c r="BK54" s="2"/>
+      <c r="BL54" s="2"/>
+      <c r="BM54" s="2"/>
+      <c r="BN54" s="2"/>
+      <c r="BP54" s="2"/>
     </row>
-    <row r="55" spans="1:31" x14ac:dyDescent="0.45">
+    <row r="55" spans="1:68">
       <c r="A55" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B55">
         <v>-1</v>
@@ -5931,10 +7639,42 @@
       <c r="AE55">
         <v>2.6444999999999999</v>
       </c>
+      <c r="AF55" s="1"/>
+      <c r="AK55" s="2"/>
+      <c r="AL55" s="2"/>
+      <c r="AM55" s="2"/>
+      <c r="AN55" s="2"/>
+      <c r="AO55" s="2"/>
+      <c r="AP55" s="2"/>
+      <c r="AQ55" s="2"/>
+      <c r="AR55" s="2"/>
+      <c r="AS55" s="2"/>
+      <c r="AT55" s="2"/>
+      <c r="AU55" s="2"/>
+      <c r="AV55" s="2"/>
+      <c r="AW55" s="2"/>
+      <c r="AX55" s="2"/>
+      <c r="AY55" s="2"/>
+      <c r="AZ55" s="2"/>
+      <c r="BA55" s="2"/>
+      <c r="BB55" s="2"/>
+      <c r="BC55" s="2"/>
+      <c r="BD55" s="2"/>
+      <c r="BE55" s="2"/>
+      <c r="BF55" s="2"/>
+      <c r="BG55" s="2"/>
+      <c r="BH55" s="2"/>
+      <c r="BI55" s="2"/>
+      <c r="BJ55" s="2"/>
+      <c r="BK55" s="2"/>
+      <c r="BL55" s="2"/>
+      <c r="BM55" s="2"/>
+      <c r="BN55" s="2"/>
+      <c r="BP55" s="2"/>
     </row>
-    <row r="56" spans="1:31" x14ac:dyDescent="0.45">
+    <row r="56" spans="1:68">
       <c r="A56" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B56">
         <v>-1</v>
@@ -6026,10 +7766,42 @@
       <c r="AE56">
         <v>-1</v>
       </c>
+      <c r="AF56" s="1"/>
+      <c r="AK56" s="2"/>
+      <c r="AL56" s="2"/>
+      <c r="AM56" s="2"/>
+      <c r="AN56" s="2"/>
+      <c r="AO56" s="2"/>
+      <c r="AP56" s="2"/>
+      <c r="AQ56" s="2"/>
+      <c r="AR56" s="2"/>
+      <c r="AS56" s="2"/>
+      <c r="AT56" s="2"/>
+      <c r="AU56" s="2"/>
+      <c r="AV56" s="2"/>
+      <c r="AW56" s="2"/>
+      <c r="AX56" s="2"/>
+      <c r="AY56" s="2"/>
+      <c r="AZ56" s="2"/>
+      <c r="BA56" s="2"/>
+      <c r="BB56" s="2"/>
+      <c r="BC56" s="2"/>
+      <c r="BD56" s="2"/>
+      <c r="BE56" s="2"/>
+      <c r="BF56" s="2"/>
+      <c r="BG56" s="2"/>
+      <c r="BH56" s="2"/>
+      <c r="BI56" s="2"/>
+      <c r="BJ56" s="2"/>
+      <c r="BK56" s="2"/>
+      <c r="BL56" s="2"/>
+      <c r="BM56" s="2"/>
+      <c r="BN56" s="2"/>
+      <c r="BP56" s="2"/>
     </row>
-    <row r="57" spans="1:31" x14ac:dyDescent="0.45">
+    <row r="57" spans="1:68">
       <c r="A57" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B57">
         <v>-1</v>
@@ -6121,10 +7893,42 @@
       <c r="AE57">
         <v>1.8826000000000001</v>
       </c>
+      <c r="AF57" s="1"/>
+      <c r="AK57" s="2"/>
+      <c r="AL57" s="2"/>
+      <c r="AM57" s="2"/>
+      <c r="AN57" s="2"/>
+      <c r="AO57" s="2"/>
+      <c r="AP57" s="2"/>
+      <c r="AQ57" s="2"/>
+      <c r="AR57" s="2"/>
+      <c r="AS57" s="2"/>
+      <c r="AT57" s="2"/>
+      <c r="AU57" s="2"/>
+      <c r="AV57" s="2"/>
+      <c r="AW57" s="2"/>
+      <c r="AX57" s="2"/>
+      <c r="AY57" s="2"/>
+      <c r="AZ57" s="2"/>
+      <c r="BA57" s="2"/>
+      <c r="BB57" s="2"/>
+      <c r="BC57" s="2"/>
+      <c r="BD57" s="2"/>
+      <c r="BE57" s="2"/>
+      <c r="BF57" s="2"/>
+      <c r="BG57" s="2"/>
+      <c r="BH57" s="2"/>
+      <c r="BI57" s="2"/>
+      <c r="BJ57" s="2"/>
+      <c r="BK57" s="2"/>
+      <c r="BL57" s="2"/>
+      <c r="BM57" s="2"/>
+      <c r="BN57" s="2"/>
+      <c r="BP57" s="2"/>
     </row>
-    <row r="58" spans="1:31" x14ac:dyDescent="0.45">
+    <row r="58" spans="1:68">
       <c r="A58" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B58">
         <v>-1</v>
@@ -6216,10 +8020,42 @@
       <c r="AE58">
         <v>0</v>
       </c>
+      <c r="AF58" s="1"/>
+      <c r="AK58" s="2"/>
+      <c r="AL58" s="2"/>
+      <c r="AM58" s="2"/>
+      <c r="AN58" s="2"/>
+      <c r="AO58" s="2"/>
+      <c r="AP58" s="2"/>
+      <c r="AQ58" s="2"/>
+      <c r="AR58" s="2"/>
+      <c r="AS58" s="2"/>
+      <c r="AT58" s="2"/>
+      <c r="AU58" s="2"/>
+      <c r="AV58" s="2"/>
+      <c r="AW58" s="2"/>
+      <c r="AX58" s="2"/>
+      <c r="AY58" s="2"/>
+      <c r="AZ58" s="2"/>
+      <c r="BA58" s="2"/>
+      <c r="BB58" s="2"/>
+      <c r="BC58" s="2"/>
+      <c r="BD58" s="2"/>
+      <c r="BE58" s="2"/>
+      <c r="BF58" s="2"/>
+      <c r="BG58" s="2"/>
+      <c r="BH58" s="2"/>
+      <c r="BI58" s="2"/>
+      <c r="BJ58" s="2"/>
+      <c r="BK58" s="2"/>
+      <c r="BL58" s="2"/>
+      <c r="BM58" s="2"/>
+      <c r="BN58" s="2"/>
+      <c r="BP58" s="2"/>
     </row>
-    <row r="59" spans="1:31" x14ac:dyDescent="0.45">
+    <row r="59" spans="1:68">
       <c r="A59" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B59">
         <v>-1</v>
@@ -6311,10 +8147,42 @@
       <c r="AE59">
         <v>1.2613000000000001</v>
       </c>
+      <c r="AF59" s="1"/>
+      <c r="AK59" s="2"/>
+      <c r="AL59" s="2"/>
+      <c r="AM59" s="2"/>
+      <c r="AN59" s="2"/>
+      <c r="AO59" s="2"/>
+      <c r="AP59" s="2"/>
+      <c r="AQ59" s="2"/>
+      <c r="AR59" s="2"/>
+      <c r="AS59" s="2"/>
+      <c r="AT59" s="2"/>
+      <c r="AU59" s="2"/>
+      <c r="AV59" s="2"/>
+      <c r="AW59" s="2"/>
+      <c r="AX59" s="2"/>
+      <c r="AY59" s="2"/>
+      <c r="AZ59" s="2"/>
+      <c r="BA59" s="2"/>
+      <c r="BB59" s="2"/>
+      <c r="BC59" s="2"/>
+      <c r="BD59" s="2"/>
+      <c r="BE59" s="2"/>
+      <c r="BF59" s="2"/>
+      <c r="BG59" s="2"/>
+      <c r="BH59" s="2"/>
+      <c r="BI59" s="2"/>
+      <c r="BJ59" s="2"/>
+      <c r="BK59" s="2"/>
+      <c r="BL59" s="2"/>
+      <c r="BM59" s="2"/>
+      <c r="BN59" s="2"/>
+      <c r="BP59" s="2"/>
     </row>
-    <row r="60" spans="1:31" x14ac:dyDescent="0.45">
+    <row r="60" spans="1:68">
       <c r="A60" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B60">
         <v>-1</v>
@@ -6406,10 +8274,42 @@
       <c r="AE60">
         <v>3.7797999999999998</v>
       </c>
+      <c r="AF60" s="1"/>
+      <c r="AK60" s="2"/>
+      <c r="AL60" s="2"/>
+      <c r="AM60" s="2"/>
+      <c r="AN60" s="2"/>
+      <c r="AO60" s="2"/>
+      <c r="AP60" s="2"/>
+      <c r="AQ60" s="2"/>
+      <c r="AR60" s="2"/>
+      <c r="AS60" s="2"/>
+      <c r="AT60" s="2"/>
+      <c r="AU60" s="2"/>
+      <c r="AV60" s="2"/>
+      <c r="AW60" s="2"/>
+      <c r="AX60" s="2"/>
+      <c r="AY60" s="2"/>
+      <c r="AZ60" s="2"/>
+      <c r="BA60" s="2"/>
+      <c r="BB60" s="2"/>
+      <c r="BC60" s="2"/>
+      <c r="BD60" s="2"/>
+      <c r="BE60" s="2"/>
+      <c r="BF60" s="2"/>
+      <c r="BG60" s="2"/>
+      <c r="BH60" s="2"/>
+      <c r="BI60" s="2"/>
+      <c r="BJ60" s="2"/>
+      <c r="BK60" s="2"/>
+      <c r="BL60" s="2"/>
+      <c r="BM60" s="2"/>
+      <c r="BN60" s="2"/>
+      <c r="BP60" s="2"/>
     </row>
-    <row r="61" spans="1:31" x14ac:dyDescent="0.45">
+    <row r="61" spans="1:68">
       <c r="A61" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B61">
         <v>-1</v>
@@ -6501,10 +8401,42 @@
       <c r="AE61">
         <v>-1</v>
       </c>
+      <c r="AF61" s="1"/>
+      <c r="AK61" s="2"/>
+      <c r="AL61" s="2"/>
+      <c r="AM61" s="2"/>
+      <c r="AN61" s="2"/>
+      <c r="AO61" s="2"/>
+      <c r="AP61" s="2"/>
+      <c r="AQ61" s="2"/>
+      <c r="AR61" s="2"/>
+      <c r="AS61" s="2"/>
+      <c r="AT61" s="2"/>
+      <c r="AU61" s="2"/>
+      <c r="AV61" s="2"/>
+      <c r="AW61" s="2"/>
+      <c r="AX61" s="2"/>
+      <c r="AY61" s="2"/>
+      <c r="AZ61" s="2"/>
+      <c r="BA61" s="2"/>
+      <c r="BB61" s="2"/>
+      <c r="BC61" s="2"/>
+      <c r="BD61" s="2"/>
+      <c r="BE61" s="2"/>
+      <c r="BF61" s="2"/>
+      <c r="BG61" s="2"/>
+      <c r="BH61" s="2"/>
+      <c r="BI61" s="2"/>
+      <c r="BJ61" s="2"/>
+      <c r="BK61" s="2"/>
+      <c r="BL61" s="2"/>
+      <c r="BM61" s="2"/>
+      <c r="BN61" s="2"/>
+      <c r="BP61" s="2"/>
     </row>
-    <row r="62" spans="1:31" x14ac:dyDescent="0.45">
+    <row r="62" spans="1:68">
       <c r="A62" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B62">
         <v>-1</v>
@@ -6596,9 +8528,41 @@
       <c r="AE62">
         <v>5.2779999999999996</v>
       </c>
+      <c r="AF62" s="1"/>
+      <c r="AK62" s="2"/>
+      <c r="AL62" s="2"/>
+      <c r="AM62" s="2"/>
+      <c r="AN62" s="2"/>
+      <c r="AO62" s="2"/>
+      <c r="AP62" s="2"/>
+      <c r="AQ62" s="2"/>
+      <c r="AR62" s="2"/>
+      <c r="AS62" s="2"/>
+      <c r="AT62" s="2"/>
+      <c r="AU62" s="2"/>
+      <c r="AV62" s="2"/>
+      <c r="AW62" s="2"/>
+      <c r="AX62" s="2"/>
+      <c r="AY62" s="2"/>
+      <c r="AZ62" s="2"/>
+      <c r="BA62" s="2"/>
+      <c r="BB62" s="2"/>
+      <c r="BC62" s="2"/>
+      <c r="BD62" s="2"/>
+      <c r="BE62" s="2"/>
+      <c r="BF62" s="2"/>
+      <c r="BG62" s="2"/>
+      <c r="BH62" s="2"/>
+      <c r="BI62" s="2"/>
+      <c r="BJ62" s="2"/>
+      <c r="BK62" s="2"/>
+      <c r="BL62" s="2"/>
+      <c r="BM62" s="2"/>
+      <c r="BN62" s="2"/>
+      <c r="BP62" s="2"/>
     </row>
   </sheetData>
-  <sortState ref="A2:AE32">
+  <sortState ref="A2:BH32">
     <sortCondition ref="A2"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -6608,19 +8572,20 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:AD79"/>
+  <dimension ref="A1:AF79"/>
   <sheetViews>
-    <sheetView topLeftCell="Q46" workbookViewId="0">
-      <selection activeCell="AE46" sqref="AE1:BP1048576"/>
+    <sheetView topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="A20" sqref="A20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.65" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="14.65"/>
   <cols>
     <col min="1" max="1" width="18.28515625" customWidth="1"/>
-    <col min="2" max="30" width="9.140625" customWidth="1"/>
+    <col min="2" max="31" width="9.140625" customWidth="1"/>
+    <col min="33" max="36" width="18.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:30" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:32">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -6711,8 +8676,11 @@
       <c r="AD1">
         <v>59</v>
       </c>
+      <c r="AE1">
+        <v>13</v>
+      </c>
     </row>
-    <row r="2" spans="1:30" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:32">
       <c r="A2" t="s">
         <v>26</v>
       </c>
@@ -6803,8 +8771,12 @@
       <c r="AD2">
         <v>2.0651999999999999</v>
       </c>
+      <c r="AE2">
+        <v>4.6242999999999999</v>
+      </c>
+      <c r="AF2" s="1"/>
     </row>
-    <row r="3" spans="1:30" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:32">
       <c r="A3" t="s">
         <v>5</v>
       </c>
@@ -6895,10 +8867,14 @@
       <c r="AD3">
         <v>4.5636999999999999</v>
       </c>
+      <c r="AE3">
+        <v>3.8835000000000002</v>
+      </c>
+      <c r="AF3" s="1"/>
     </row>
-    <row r="4" spans="1:30" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:32">
       <c r="A4" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B4">
         <v>-1</v>
@@ -6987,10 +8963,14 @@
       <c r="AD4">
         <v>-1</v>
       </c>
+      <c r="AE4">
+        <v>-1</v>
+      </c>
+      <c r="AF4" s="1"/>
     </row>
-    <row r="5" spans="1:30" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:32">
       <c r="A5" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B5">
         <v>-1</v>
@@ -7079,10 +9059,14 @@
       <c r="AD5">
         <v>-1</v>
       </c>
+      <c r="AE5">
+        <v>-1</v>
+      </c>
+      <c r="AF5" s="1"/>
     </row>
-    <row r="6" spans="1:30" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:32">
       <c r="A6" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B6">
         <v>-1</v>
@@ -7171,10 +9155,14 @@
       <c r="AD6">
         <v>-1</v>
       </c>
+      <c r="AE6">
+        <v>2.3386999999999998</v>
+      </c>
+      <c r="AF6" s="1"/>
     </row>
-    <row r="7" spans="1:30" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:32">
       <c r="A7" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B7">
         <v>-1</v>
@@ -7263,10 +9251,14 @@
       <c r="AD7">
         <v>3.7528999999999999</v>
       </c>
+      <c r="AE7">
+        <v>-1</v>
+      </c>
+      <c r="AF7" s="1"/>
     </row>
-    <row r="8" spans="1:30" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:32">
       <c r="A8" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B8">
         <v>-1</v>
@@ -7355,8 +9347,12 @@
       <c r="AD8">
         <v>4.7347999999999999</v>
       </c>
+      <c r="AE8">
+        <v>0</v>
+      </c>
+      <c r="AF8" s="1"/>
     </row>
-    <row r="9" spans="1:30" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:32">
       <c r="A9" t="s">
         <v>27</v>
       </c>
@@ -7447,10 +9443,14 @@
       <c r="AD9">
         <v>-1</v>
       </c>
+      <c r="AE9">
+        <v>-1</v>
+      </c>
+      <c r="AF9" s="1"/>
     </row>
-    <row r="10" spans="1:30" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:32">
       <c r="A10" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B10">
         <v>-1</v>
@@ -7539,10 +9539,14 @@
       <c r="AD10">
         <v>-1</v>
       </c>
+      <c r="AE10">
+        <v>-1</v>
+      </c>
+      <c r="AF10" s="1"/>
     </row>
-    <row r="11" spans="1:30" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:32">
       <c r="A11" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B11">
         <v>-1</v>
@@ -7631,10 +9635,14 @@
       <c r="AD11">
         <v>-1</v>
       </c>
+      <c r="AE11">
+        <v>-1</v>
+      </c>
+      <c r="AF11" s="1"/>
     </row>
-    <row r="12" spans="1:30" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:32">
       <c r="A12" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B12">
         <v>-1</v>
@@ -7723,10 +9731,14 @@
       <c r="AD12">
         <v>-1</v>
       </c>
+      <c r="AE12">
+        <v>3.6568999999999998</v>
+      </c>
+      <c r="AF12" s="1"/>
     </row>
-    <row r="13" spans="1:30" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:32">
       <c r="A13" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B13">
         <v>-1</v>
@@ -7815,8 +9827,12 @@
       <c r="AD13">
         <v>-1</v>
       </c>
+      <c r="AE13">
+        <v>-1</v>
+      </c>
+      <c r="AF13" s="1"/>
     </row>
-    <row r="14" spans="1:30" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:32">
       <c r="A14" t="s">
         <v>18</v>
       </c>
@@ -7907,8 +9923,12 @@
       <c r="AD14">
         <v>-1</v>
       </c>
+      <c r="AE14">
+        <v>3.2282000000000002</v>
+      </c>
+      <c r="AF14" s="1"/>
     </row>
-    <row r="15" spans="1:30" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:32">
       <c r="A15" t="s">
         <v>3</v>
       </c>
@@ -7999,8 +10019,12 @@
       <c r="AD15">
         <v>4.0034999999999998</v>
       </c>
+      <c r="AE15">
+        <v>5.4383999999999997</v>
+      </c>
+      <c r="AF15" s="1"/>
     </row>
-    <row r="16" spans="1:30" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:32">
       <c r="A16" t="s">
         <v>14</v>
       </c>
@@ -8091,10 +10115,14 @@
       <c r="AD16">
         <v>2.7921</v>
       </c>
+      <c r="AE16">
+        <v>4.5929000000000002</v>
+      </c>
+      <c r="AF16" s="1"/>
     </row>
-    <row r="17" spans="1:30" x14ac:dyDescent="0.45">
+    <row r="17" spans="1:32">
       <c r="A17" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B17">
         <v>4.5382999999999996</v>
@@ -8183,8 +10211,12 @@
       <c r="AD17">
         <v>5.2583000000000002</v>
       </c>
+      <c r="AE17">
+        <v>-1</v>
+      </c>
+      <c r="AF17" s="1"/>
     </row>
-    <row r="18" spans="1:30" x14ac:dyDescent="0.45">
+    <row r="18" spans="1:32">
       <c r="A18" t="s">
         <v>4</v>
       </c>
@@ -8275,10 +10307,14 @@
       <c r="AD18">
         <v>1.9968999999999999</v>
       </c>
+      <c r="AE18">
+        <v>6.5919999999999996</v>
+      </c>
+      <c r="AF18" s="1"/>
     </row>
-    <row r="19" spans="1:30" x14ac:dyDescent="0.45">
+    <row r="19" spans="1:32">
       <c r="A19" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B19">
         <v>-1</v>
@@ -8367,10 +10403,14 @@
       <c r="AD19">
         <v>-1</v>
       </c>
+      <c r="AE19">
+        <v>-1</v>
+      </c>
+      <c r="AF19" s="1"/>
     </row>
-    <row r="20" spans="1:30" x14ac:dyDescent="0.45">
+    <row r="20" spans="1:32">
       <c r="A20" t="s">
-        <v>28</v>
+        <v>10</v>
       </c>
       <c r="B20">
         <v>-1</v>
@@ -8459,8 +10499,12 @@
       <c r="AD20">
         <v>-1</v>
       </c>
+      <c r="AE20">
+        <v>-1</v>
+      </c>
+      <c r="AF20" s="1"/>
     </row>
-    <row r="21" spans="1:30" x14ac:dyDescent="0.45">
+    <row r="21" spans="1:32">
       <c r="A21" t="s">
         <v>20</v>
       </c>
@@ -8551,10 +10595,14 @@
       <c r="AD21">
         <v>-1</v>
       </c>
+      <c r="AE21">
+        <v>-1</v>
+      </c>
+      <c r="AF21" s="1"/>
     </row>
-    <row r="22" spans="1:30" x14ac:dyDescent="0.45">
+    <row r="22" spans="1:32">
       <c r="A22" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B22">
         <v>-1</v>
@@ -8643,8 +10691,12 @@
       <c r="AD22">
         <v>2.0424000000000002</v>
       </c>
+      <c r="AE22">
+        <v>-1</v>
+      </c>
+      <c r="AF22" s="1"/>
     </row>
-    <row r="23" spans="1:30" x14ac:dyDescent="0.45">
+    <row r="23" spans="1:32">
       <c r="A23" t="s">
         <v>9</v>
       </c>
@@ -8735,10 +10787,14 @@
       <c r="AD23">
         <v>6.0126999999999997</v>
       </c>
+      <c r="AE23">
+        <v>2.7372000000000001</v>
+      </c>
+      <c r="AF23" s="1"/>
     </row>
-    <row r="24" spans="1:30" x14ac:dyDescent="0.45">
+    <row r="24" spans="1:32">
       <c r="A24" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B24">
         <v>-1</v>
@@ -8827,8 +10883,12 @@
       <c r="AD24">
         <v>-1</v>
       </c>
+      <c r="AE24">
+        <v>-1</v>
+      </c>
+      <c r="AF24" s="1"/>
     </row>
-    <row r="25" spans="1:30" x14ac:dyDescent="0.45">
+    <row r="25" spans="1:32">
       <c r="A25" t="s">
         <v>24</v>
       </c>
@@ -8919,8 +10979,12 @@
       <c r="AD25">
         <v>-1</v>
       </c>
+      <c r="AE25">
+        <v>-1</v>
+      </c>
+      <c r="AF25" s="1"/>
     </row>
-    <row r="26" spans="1:30" x14ac:dyDescent="0.45">
+    <row r="26" spans="1:32">
       <c r="A26" t="s">
         <v>1</v>
       </c>
@@ -9011,10 +11075,14 @@
       <c r="AD26">
         <v>3.1153</v>
       </c>
+      <c r="AE26">
+        <v>7.9062999999999999</v>
+      </c>
+      <c r="AF26" s="1"/>
     </row>
-    <row r="27" spans="1:30" x14ac:dyDescent="0.45">
+    <row r="27" spans="1:32">
       <c r="A27" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B27">
         <v>2.7254</v>
@@ -9103,10 +11171,14 @@
       <c r="AD27">
         <v>-1</v>
       </c>
+      <c r="AE27">
+        <v>2.2115</v>
+      </c>
+      <c r="AF27" s="1"/>
     </row>
-    <row r="28" spans="1:30" x14ac:dyDescent="0.45">
+    <row r="28" spans="1:32">
       <c r="A28" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B28">
         <v>-1</v>
@@ -9195,10 +11267,14 @@
       <c r="AD28">
         <v>-1</v>
       </c>
+      <c r="AE28">
+        <v>5.6009000000000002</v>
+      </c>
+      <c r="AF28" s="1"/>
     </row>
-    <row r="29" spans="1:30" x14ac:dyDescent="0.45">
+    <row r="29" spans="1:32">
       <c r="A29" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B29">
         <v>-1</v>
@@ -9287,10 +11363,14 @@
       <c r="AD29">
         <v>-1</v>
       </c>
+      <c r="AE29">
+        <v>-1</v>
+      </c>
+      <c r="AF29" s="1"/>
     </row>
-    <row r="30" spans="1:30" x14ac:dyDescent="0.45">
+    <row r="30" spans="1:32">
       <c r="A30" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B30">
         <v>-1</v>
@@ -9379,8 +11459,12 @@
       <c r="AD30">
         <v>-1</v>
       </c>
+      <c r="AE30">
+        <v>6.6501999999999999</v>
+      </c>
+      <c r="AF30" s="1"/>
     </row>
-    <row r="31" spans="1:30" x14ac:dyDescent="0.45">
+    <row r="31" spans="1:32">
       <c r="A31" t="s">
         <v>25</v>
       </c>
@@ -9471,10 +11555,14 @@
       <c r="AD31">
         <v>0</v>
       </c>
+      <c r="AE31">
+        <v>3.3965000000000001</v>
+      </c>
+      <c r="AF31" s="1"/>
     </row>
-    <row r="32" spans="1:30" x14ac:dyDescent="0.45">
+    <row r="32" spans="1:32">
       <c r="A32" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B32">
         <v>-1</v>
@@ -9563,10 +11651,14 @@
       <c r="AD32">
         <v>-1</v>
       </c>
+      <c r="AE32">
+        <v>-1</v>
+      </c>
+      <c r="AF32" s="1"/>
     </row>
-    <row r="33" spans="1:30" x14ac:dyDescent="0.45">
+    <row r="33" spans="1:32">
       <c r="A33" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B33">
         <v>4.0983999999999998</v>
@@ -9655,8 +11747,12 @@
       <c r="AD33">
         <v>-1</v>
       </c>
+      <c r="AE33">
+        <v>-1</v>
+      </c>
+      <c r="AF33" s="1"/>
     </row>
-    <row r="34" spans="1:30" x14ac:dyDescent="0.45">
+    <row r="34" spans="1:32">
       <c r="A34" t="s">
         <v>11</v>
       </c>
@@ -9747,10 +11843,14 @@
       <c r="AD34">
         <v>-1</v>
       </c>
+      <c r="AE34">
+        <v>4.2419000000000002</v>
+      </c>
+      <c r="AF34" s="1"/>
     </row>
-    <row r="35" spans="1:30" x14ac:dyDescent="0.45">
+    <row r="35" spans="1:32">
       <c r="A35" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B35">
         <v>-1</v>
@@ -9839,10 +11939,14 @@
       <c r="AD35">
         <v>-1</v>
       </c>
+      <c r="AE35">
+        <v>0</v>
+      </c>
+      <c r="AF35" s="1"/>
     </row>
-    <row r="36" spans="1:30" x14ac:dyDescent="0.45">
+    <row r="36" spans="1:32">
       <c r="A36" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B36">
         <v>2.4135</v>
@@ -9931,10 +12035,14 @@
       <c r="AD36">
         <v>-1</v>
       </c>
+      <c r="AE36">
+        <v>-1</v>
+      </c>
+      <c r="AF36" s="1"/>
     </row>
-    <row r="37" spans="1:30" x14ac:dyDescent="0.45">
+    <row r="37" spans="1:32">
       <c r="A37" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B37">
         <v>-1</v>
@@ -10023,10 +12131,14 @@
       <c r="AD37">
         <v>-1</v>
       </c>
+      <c r="AE37">
+        <v>0</v>
+      </c>
+      <c r="AF37" s="1"/>
     </row>
-    <row r="38" spans="1:30" x14ac:dyDescent="0.45">
+    <row r="38" spans="1:32">
       <c r="A38" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B38">
         <v>-1</v>
@@ -10115,10 +12227,14 @@
       <c r="AD38">
         <v>-1</v>
       </c>
+      <c r="AE38">
+        <v>-1</v>
+      </c>
+      <c r="AF38" s="1"/>
     </row>
-    <row r="39" spans="1:30" x14ac:dyDescent="0.45">
+    <row r="39" spans="1:32">
       <c r="A39" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B39">
         <v>-1</v>
@@ -10207,10 +12323,14 @@
       <c r="AD39">
         <v>-1</v>
       </c>
+      <c r="AE39">
+        <v>-1</v>
+      </c>
+      <c r="AF39" s="1"/>
     </row>
-    <row r="40" spans="1:30" x14ac:dyDescent="0.45">
+    <row r="40" spans="1:32">
       <c r="A40" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B40">
         <v>-1</v>
@@ -10299,10 +12419,14 @@
       <c r="AD40">
         <v>-1</v>
       </c>
+      <c r="AE40">
+        <v>2.573</v>
+      </c>
+      <c r="AF40" s="1"/>
     </row>
-    <row r="41" spans="1:30" x14ac:dyDescent="0.45">
+    <row r="41" spans="1:32">
       <c r="A41" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B41">
         <v>-1</v>
@@ -10391,10 +12515,14 @@
       <c r="AD41">
         <v>-1</v>
       </c>
+      <c r="AE41">
+        <v>-1</v>
+      </c>
+      <c r="AF41" s="1"/>
     </row>
-    <row r="42" spans="1:30" x14ac:dyDescent="0.45">
+    <row r="42" spans="1:32">
       <c r="A42" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B42">
         <v>-1</v>
@@ -10483,8 +12611,12 @@
       <c r="AD42">
         <v>4.7275999999999998</v>
       </c>
+      <c r="AE42">
+        <v>5.2355999999999998</v>
+      </c>
+      <c r="AF42" s="1"/>
     </row>
-    <row r="43" spans="1:30" x14ac:dyDescent="0.45">
+    <row r="43" spans="1:32">
       <c r="A43" t="s">
         <v>12</v>
       </c>
@@ -10575,8 +12707,12 @@
       <c r="AD43">
         <v>-1</v>
       </c>
+      <c r="AE43">
+        <v>4.931</v>
+      </c>
+      <c r="AF43" s="1"/>
     </row>
-    <row r="44" spans="1:30" x14ac:dyDescent="0.45">
+    <row r="44" spans="1:32">
       <c r="A44" t="s">
         <v>19</v>
       </c>
@@ -10667,10 +12803,14 @@
       <c r="AD44">
         <v>-1</v>
       </c>
+      <c r="AE44">
+        <v>-1</v>
+      </c>
+      <c r="AF44" s="1"/>
     </row>
-    <row r="45" spans="1:30" x14ac:dyDescent="0.45">
+    <row r="45" spans="1:32">
       <c r="A45" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B45">
         <v>-1</v>
@@ -10759,8 +12899,12 @@
       <c r="AD45">
         <v>4.8109999999999999</v>
       </c>
+      <c r="AE45">
+        <v>4.7664</v>
+      </c>
+      <c r="AF45" s="1"/>
     </row>
-    <row r="46" spans="1:30" x14ac:dyDescent="0.45">
+    <row r="46" spans="1:32">
       <c r="A46" t="s">
         <v>8</v>
       </c>
@@ -10851,10 +12995,14 @@
       <c r="AD46">
         <v>-1</v>
       </c>
+      <c r="AE46">
+        <v>2.1355</v>
+      </c>
+      <c r="AF46" s="1"/>
     </row>
-    <row r="47" spans="1:30" x14ac:dyDescent="0.45">
+    <row r="47" spans="1:32">
       <c r="A47" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B47">
         <v>-1</v>
@@ -10943,10 +13091,14 @@
       <c r="AD47">
         <v>-1</v>
       </c>
+      <c r="AE47">
+        <v>4.6154000000000002</v>
+      </c>
+      <c r="AF47" s="1"/>
     </row>
-    <row r="48" spans="1:30" x14ac:dyDescent="0.45">
+    <row r="48" spans="1:32">
       <c r="A48" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B48">
         <v>-1</v>
@@ -11035,10 +13187,14 @@
       <c r="AD48">
         <v>-1</v>
       </c>
+      <c r="AE48">
+        <v>-1</v>
+      </c>
+      <c r="AF48" s="1"/>
     </row>
-    <row r="49" spans="1:30" x14ac:dyDescent="0.45">
+    <row r="49" spans="1:32">
       <c r="A49" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B49">
         <v>-1</v>
@@ -11127,10 +13283,14 @@
       <c r="AD49">
         <v>3.2967</v>
       </c>
+      <c r="AE49">
+        <v>5.3747999999999996</v>
+      </c>
+      <c r="AF49" s="1"/>
     </row>
-    <row r="50" spans="1:30" x14ac:dyDescent="0.45">
+    <row r="50" spans="1:32">
       <c r="A50" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B50">
         <v>-1</v>
@@ -11219,10 +13379,14 @@
       <c r="AD50">
         <v>-1</v>
       </c>
+      <c r="AE50">
+        <v>-1</v>
+      </c>
+      <c r="AF50" s="1"/>
     </row>
-    <row r="51" spans="1:30" x14ac:dyDescent="0.45">
+    <row r="51" spans="1:32">
       <c r="A51" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B51">
         <v>-1</v>
@@ -11311,8 +13475,12 @@
       <c r="AD51">
         <v>-1</v>
       </c>
+      <c r="AE51">
+        <v>5.7458999999999998</v>
+      </c>
+      <c r="AF51" s="1"/>
     </row>
-    <row r="52" spans="1:30" x14ac:dyDescent="0.45">
+    <row r="52" spans="1:32">
       <c r="A52" t="s">
         <v>22</v>
       </c>
@@ -11403,8 +13571,12 @@
       <c r="AD52">
         <v>-1</v>
       </c>
+      <c r="AE52">
+        <v>3.7831999999999999</v>
+      </c>
+      <c r="AF52" s="1"/>
     </row>
-    <row r="53" spans="1:30" x14ac:dyDescent="0.45">
+    <row r="53" spans="1:32">
       <c r="A53" t="s">
         <v>23</v>
       </c>
@@ -11495,10 +13667,14 @@
       <c r="AD53">
         <v>6.5434000000000001</v>
       </c>
+      <c r="AE53">
+        <v>7.5472000000000001</v>
+      </c>
+      <c r="AF53" s="1"/>
     </row>
-    <row r="54" spans="1:30" x14ac:dyDescent="0.45">
+    <row r="54" spans="1:32">
       <c r="A54" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B54">
         <v>-1</v>
@@ -11587,8 +13763,12 @@
       <c r="AD54">
         <v>-1</v>
       </c>
+      <c r="AE54">
+        <v>-1</v>
+      </c>
+      <c r="AF54" s="1"/>
     </row>
-    <row r="55" spans="1:30" x14ac:dyDescent="0.45">
+    <row r="55" spans="1:32">
       <c r="A55" t="s">
         <v>21</v>
       </c>
@@ -11679,10 +13859,14 @@
       <c r="AD55">
         <v>-1</v>
       </c>
+      <c r="AE55">
+        <v>-1</v>
+      </c>
+      <c r="AF55" s="1"/>
     </row>
-    <row r="56" spans="1:30" x14ac:dyDescent="0.45">
+    <row r="56" spans="1:32">
       <c r="A56" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B56">
         <v>-1</v>
@@ -11771,10 +13955,14 @@
       <c r="AD56">
         <v>-1</v>
       </c>
+      <c r="AE56">
+        <v>-1</v>
+      </c>
+      <c r="AF56" s="1"/>
     </row>
-    <row r="57" spans="1:30" x14ac:dyDescent="0.45">
+    <row r="57" spans="1:32">
       <c r="A57" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B57">
         <v>-1</v>
@@ -11863,10 +14051,14 @@
       <c r="AD57">
         <v>-1</v>
       </c>
+      <c r="AE57">
+        <v>0.3755</v>
+      </c>
+      <c r="AF57" s="1"/>
     </row>
-    <row r="58" spans="1:30" x14ac:dyDescent="0.45">
+    <row r="58" spans="1:32">
       <c r="A58" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B58">
         <v>-1</v>
@@ -11955,10 +14147,14 @@
       <c r="AD58">
         <v>-1</v>
       </c>
+      <c r="AE58">
+        <v>-1</v>
+      </c>
+      <c r="AF58" s="1"/>
     </row>
-    <row r="59" spans="1:30" x14ac:dyDescent="0.45">
+    <row r="59" spans="1:32">
       <c r="A59" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B59">
         <v>-1</v>
@@ -12047,10 +14243,14 @@
       <c r="AD59">
         <v>-1</v>
       </c>
+      <c r="AE59">
+        <v>-1</v>
+      </c>
+      <c r="AF59" s="1"/>
     </row>
-    <row r="60" spans="1:30" x14ac:dyDescent="0.45">
+    <row r="60" spans="1:32">
       <c r="A60" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B60">
         <v>-1</v>
@@ -12139,8 +14339,12 @@
       <c r="AD60">
         <v>-1</v>
       </c>
+      <c r="AE60">
+        <v>4.9069000000000003</v>
+      </c>
+      <c r="AF60" s="1"/>
     </row>
-    <row r="61" spans="1:30" x14ac:dyDescent="0.45">
+    <row r="61" spans="1:32">
       <c r="A61" t="s">
         <v>15</v>
       </c>
@@ -12231,10 +14435,14 @@
       <c r="AD61">
         <v>-1</v>
       </c>
+      <c r="AE61">
+        <v>-1</v>
+      </c>
+      <c r="AF61" s="1"/>
     </row>
-    <row r="62" spans="1:30" x14ac:dyDescent="0.45">
+    <row r="62" spans="1:32">
       <c r="A62" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B62">
         <v>-1</v>
@@ -12323,10 +14531,14 @@
       <c r="AD62">
         <v>2.3797000000000001</v>
       </c>
+      <c r="AE62">
+        <v>-1</v>
+      </c>
+      <c r="AF62" s="1"/>
     </row>
-    <row r="63" spans="1:30" x14ac:dyDescent="0.45">
+    <row r="63" spans="1:32">
       <c r="A63" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B63">
         <v>-1</v>
@@ -12415,10 +14627,14 @@
       <c r="AD63">
         <v>-1</v>
       </c>
+      <c r="AE63">
+        <v>-1</v>
+      </c>
+      <c r="AF63" s="1"/>
     </row>
-    <row r="64" spans="1:30" x14ac:dyDescent="0.45">
+    <row r="64" spans="1:32">
       <c r="A64" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B64">
         <v>-1</v>
@@ -12507,10 +14723,14 @@
       <c r="AD64">
         <v>-1</v>
       </c>
+      <c r="AE64">
+        <v>-1</v>
+      </c>
+      <c r="AF64" s="1"/>
     </row>
-    <row r="65" spans="1:30" x14ac:dyDescent="0.45">
+    <row r="65" spans="1:32">
       <c r="A65" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B65">
         <v>-1</v>
@@ -12599,10 +14819,14 @@
       <c r="AD65">
         <v>-1</v>
       </c>
+      <c r="AE65">
+        <v>-1</v>
+      </c>
+      <c r="AF65" s="1"/>
     </row>
-    <row r="66" spans="1:30" x14ac:dyDescent="0.45">
+    <row r="66" spans="1:32">
       <c r="A66" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B66">
         <v>-1</v>
@@ -12691,10 +14915,14 @@
       <c r="AD66">
         <v>-1</v>
       </c>
+      <c r="AE66">
+        <v>-1</v>
+      </c>
+      <c r="AF66" s="1"/>
     </row>
-    <row r="67" spans="1:30" x14ac:dyDescent="0.45">
+    <row r="67" spans="1:32">
       <c r="A67" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B67">
         <v>-1</v>
@@ -12783,10 +15011,14 @@
       <c r="AD67">
         <v>-1</v>
       </c>
+      <c r="AE67">
+        <v>-1</v>
+      </c>
+      <c r="AF67" s="1"/>
     </row>
-    <row r="68" spans="1:30" x14ac:dyDescent="0.45">
+    <row r="68" spans="1:32">
       <c r="A68" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B68">
         <v>-1</v>
@@ -12875,8 +15107,12 @@
       <c r="AD68">
         <v>-1</v>
       </c>
+      <c r="AE68">
+        <v>-1</v>
+      </c>
+      <c r="AF68" s="1"/>
     </row>
-    <row r="69" spans="1:30" x14ac:dyDescent="0.45">
+    <row r="69" spans="1:32">
       <c r="A69" t="s">
         <v>7</v>
       </c>
@@ -12967,10 +15203,14 @@
       <c r="AD69">
         <v>4.4603000000000002</v>
       </c>
+      <c r="AE69">
+        <v>5.2880000000000003</v>
+      </c>
+      <c r="AF69" s="1"/>
     </row>
-    <row r="70" spans="1:30" x14ac:dyDescent="0.45">
+    <row r="70" spans="1:32">
       <c r="A70" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B70">
         <v>3.0488</v>
@@ -13059,10 +15299,14 @@
       <c r="AD70">
         <v>3.9188000000000001</v>
       </c>
+      <c r="AE70">
+        <v>3.5908000000000002</v>
+      </c>
+      <c r="AF70" s="1"/>
     </row>
-    <row r="71" spans="1:30" x14ac:dyDescent="0.45">
+    <row r="71" spans="1:32">
       <c r="A71" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B71">
         <v>-1</v>
@@ -13151,10 +15395,14 @@
       <c r="AD71">
         <v>-1</v>
       </c>
+      <c r="AE71">
+        <v>-1</v>
+      </c>
+      <c r="AF71" s="1"/>
     </row>
-    <row r="72" spans="1:30" x14ac:dyDescent="0.45">
+    <row r="72" spans="1:32">
       <c r="A72" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B72">
         <v>-1</v>
@@ -13243,10 +15491,14 @@
       <c r="AD72">
         <v>-1</v>
       </c>
+      <c r="AE72">
+        <v>-1</v>
+      </c>
+      <c r="AF72" s="1"/>
     </row>
-    <row r="73" spans="1:30" x14ac:dyDescent="0.45">
+    <row r="73" spans="1:32">
       <c r="A73" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B73">
         <v>-1</v>
@@ -13335,10 +15587,14 @@
       <c r="AD73">
         <v>-1</v>
       </c>
+      <c r="AE73">
+        <v>-1</v>
+      </c>
+      <c r="AF73" s="1"/>
     </row>
-    <row r="74" spans="1:30" x14ac:dyDescent="0.45">
+    <row r="74" spans="1:32">
       <c r="A74" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B74">
         <v>-1</v>
@@ -13427,10 +15683,14 @@
       <c r="AD74">
         <v>-1</v>
       </c>
+      <c r="AE74">
+        <v>-1</v>
+      </c>
+      <c r="AF74" s="1"/>
     </row>
-    <row r="75" spans="1:30" x14ac:dyDescent="0.45">
+    <row r="75" spans="1:32">
       <c r="A75" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B75">
         <v>2.6223999999999998</v>
@@ -13519,8 +15779,12 @@
       <c r="AD75">
         <v>3.5287000000000002</v>
       </c>
+      <c r="AE75">
+        <v>2.8197999999999999</v>
+      </c>
+      <c r="AF75" s="1"/>
     </row>
-    <row r="76" spans="1:30" x14ac:dyDescent="0.45">
+    <row r="76" spans="1:32">
       <c r="A76" t="s">
         <v>13</v>
       </c>
@@ -13611,8 +15875,12 @@
       <c r="AD76">
         <v>-1</v>
       </c>
+      <c r="AE76">
+        <v>3.2</v>
+      </c>
+      <c r="AF76" s="1"/>
     </row>
-    <row r="77" spans="1:30" x14ac:dyDescent="0.45">
+    <row r="77" spans="1:32">
       <c r="A77" t="s">
         <v>17</v>
       </c>
@@ -13703,10 +15971,14 @@
       <c r="AD77">
         <v>-1</v>
       </c>
+      <c r="AE77">
+        <v>0.33439999999999998</v>
+      </c>
+      <c r="AF77" s="1"/>
     </row>
-    <row r="78" spans="1:30" x14ac:dyDescent="0.45">
+    <row r="78" spans="1:32">
       <c r="A78" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B78">
         <v>-1</v>
@@ -13795,10 +16067,14 @@
       <c r="AD78">
         <v>-1</v>
       </c>
+      <c r="AE78">
+        <v>3.2894999999999999</v>
+      </c>
+      <c r="AF78" s="1"/>
     </row>
-    <row r="79" spans="1:30" x14ac:dyDescent="0.45">
+    <row r="79" spans="1:32">
       <c r="A79" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B79">
         <v>-1</v>
@@ -13887,9 +16163,13 @@
       <c r="AD79">
         <v>-1</v>
       </c>
+      <c r="AE79">
+        <v>-1</v>
+      </c>
+      <c r="AF79" s="1"/>
     </row>
   </sheetData>
-  <sortState ref="A2:AD36">
+  <sortState ref="A2:BJ36">
     <sortCondition ref="A2"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -13901,16 +16181,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:U6"/>
   <sheetViews>
-    <sheetView topLeftCell="H1" workbookViewId="0">
-      <selection activeCell="V1" sqref="V1:AV1048576"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="N14" sqref="N14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.65" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="14.65"/>
   <cols>
     <col min="1" max="1" width="18.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:21" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:21">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -13975,7 +16255,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="2" spans="1:21" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:21">
       <c r="A2" t="s">
         <v>5</v>
       </c>
@@ -14040,9 +16320,9 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="3" spans="1:21" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:21">
       <c r="A3" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B3">
         <v>-1</v>
@@ -14105,7 +16385,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="4" spans="1:21" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:21">
       <c r="A4" t="s">
         <v>17</v>
       </c>
@@ -14170,9 +16450,9 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="5" spans="1:21" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:21">
       <c r="A5" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B5">
         <v>-1</v>
@@ -14235,7 +16515,7 @@
         <v>1.1646000000000001</v>
       </c>
     </row>
-    <row r="6" spans="1:21" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:21">
       <c r="A6" t="s">
         <v>8</v>
       </c>
@@ -14301,7 +16581,7 @@
       </c>
     </row>
   </sheetData>
-  <sortState ref="A2:U3">
+  <sortState ref="A2:Y3">
     <sortCondition ref="A2"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -14313,17 +16593,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:AC17"/>
   <sheetViews>
-    <sheetView topLeftCell="P1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="AE5" sqref="AE5"/>
+    <sheetView topLeftCell="T1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="AH17" sqref="AH17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.65" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="14.65"/>
   <cols>
     <col min="1" max="1" width="18.28515625" customWidth="1"/>
     <col min="20" max="20" width="9.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:29" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:29">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -14412,7 +16692,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="2" spans="1:29" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:29">
       <c r="A2" t="s">
         <v>26</v>
       </c>
@@ -14501,7 +16781,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="3" spans="1:29" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:29">
       <c r="A3" t="s">
         <v>3</v>
       </c>
@@ -14590,7 +16870,7 @@
         <v>4.4462999999999999</v>
       </c>
     </row>
-    <row r="4" spans="1:29" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:29">
       <c r="A4" t="s">
         <v>14</v>
       </c>
@@ -14679,7 +16959,7 @@
         <v>7.1429</v>
       </c>
     </row>
-    <row r="5" spans="1:29" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:29">
       <c r="A5" t="s">
         <v>4</v>
       </c>
@@ -14768,7 +17048,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="6" spans="1:29" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:29">
       <c r="A6" t="s">
         <v>9</v>
       </c>
@@ -14857,7 +17137,7 @@
         <v>5.2477999999999998</v>
       </c>
     </row>
-    <row r="7" spans="1:29" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:29">
       <c r="A7" t="s">
         <v>1</v>
       </c>
@@ -14946,9 +17226,9 @@
         <v>6.5517000000000003</v>
       </c>
     </row>
-    <row r="8" spans="1:29" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:29">
       <c r="A8" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B8">
         <v>-1</v>
@@ -15035,9 +17315,9 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="9" spans="1:29" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:29">
       <c r="A9" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B9">
         <v>-1</v>
@@ -15124,9 +17404,9 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="10" spans="1:29" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:29">
       <c r="A10" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B10">
         <v>-1</v>
@@ -15213,9 +17493,9 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="11" spans="1:29" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:29">
       <c r="A11" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B11">
         <v>-1</v>
@@ -15302,9 +17582,9 @@
         <v>1.7722</v>
       </c>
     </row>
-    <row r="12" spans="1:29" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:29">
       <c r="A12" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B12">
         <v>-1</v>
@@ -15391,7 +17671,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="13" spans="1:29" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:29">
       <c r="A13" t="s">
         <v>12</v>
       </c>
@@ -15480,9 +17760,9 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="14" spans="1:29" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:29">
       <c r="A14" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B14">
         <v>-1</v>
@@ -15569,7 +17849,7 @@
         <v>2.4965000000000002</v>
       </c>
     </row>
-    <row r="15" spans="1:29" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:29">
       <c r="A15" t="s">
         <v>8</v>
       </c>
@@ -15658,9 +17938,9 @@
         <v>4.3724999999999996</v>
       </c>
     </row>
-    <row r="16" spans="1:29" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:29">
       <c r="A16" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B16">
         <v>-1</v>
@@ -15747,7 +18027,7 @@
         <v>5.4526000000000003</v>
       </c>
     </row>
-    <row r="17" spans="1:29" x14ac:dyDescent="0.45">
+    <row r="17" spans="1:29">
       <c r="A17" t="s">
         <v>7</v>
       </c>
@@ -15850,15 +18130,15 @@
   <dimension ref="A1:AD8"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="Q1" workbookViewId="0">
-      <selection activeCell="AE1" sqref="AE1:BN1048576"/>
+      <selection activeCell="AK10" sqref="AK10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.65" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="14.65"/>
   <cols>
     <col min="1" max="1" width="18.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:30" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:30">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -15950,7 +18230,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="2" spans="1:30" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:30">
       <c r="A2" t="s">
         <v>5</v>
       </c>
@@ -16042,7 +18322,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="3" spans="1:30" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:30">
       <c r="A3" t="s">
         <v>9</v>
       </c>
@@ -16134,7 +18414,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="4" spans="1:30" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:30">
       <c r="A4" t="s">
         <v>1</v>
       </c>
@@ -16226,9 +18506,9 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="5" spans="1:30" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:30">
       <c r="A5" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B5">
         <v>-1</v>
@@ -16318,7 +18598,7 @@
         <v>4.2878999999999996</v>
       </c>
     </row>
-    <row r="6" spans="1:30" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:30">
       <c r="A6" t="s">
         <v>15</v>
       </c>
@@ -16410,9 +18690,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:30" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:30">
       <c r="A7" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B7">
         <v>-1</v>
@@ -16502,9 +18782,9 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="8" spans="1:30" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:30">
       <c r="A8" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B8">
         <v>-1</v>

</xml_diff>